<commit_message>
Update Readme, added documentation, and added the adjustedbeta function.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4803BA-7865-4FD6-9C3E-F9D94C32616F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9F22D-AEBE-47D9-B9CA-71794CF2D52F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4815" yWindow="3585" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$29</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$30</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>RFR</t>
   </si>
@@ -139,13 +139,40 @@
   </si>
   <si>
     <t>Revised Sharpe Ratio</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>Rp</t>
+  </si>
+  <si>
+    <t>Selectivity</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Rf</t>
+  </si>
+  <si>
+    <t>Fama Beta</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Adjusted Beta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -153,6 +180,7 @@
     <numFmt numFmtId="167" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;?????_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -197,7 +225,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -222,9 +250,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -541,23 +571,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1119,7 +1149,7 @@
         <v>-6.3539265847126769E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>8.218509209156899E-5</v>
       </c>
@@ -1144,11 +1174,11 @@
         <v>2.6039764394154563E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1169,7 +1199,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1190,7 +1220,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1199,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="8" cm="1">
-        <f t="array" ref="D21">_xlfn.COVARIANCE.P(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)/_xlfn.VAR.P($C$3:$C$17-$B$3:$B$17)</f>
+        <f t="array" ref="D21">_xlfn.COVARIANCE.S(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)/_xlfn.VAR.S($C$3:$C$17-$B$3:$B$17)</f>
         <v>0.94109509071871278</v>
       </c>
       <c r="G21" s="9" cm="1">
@@ -1215,299 +1245,400 @@
         <v>0.12710524781890767</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="8">
+        <f>C21*2/3+1/3</f>
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <f>D21*2/3+1/3</f>
+        <v>0.96073006047914178</v>
+      </c>
+      <c r="G22" s="9" cm="1">
+        <f t="array" ref="G22">_xll.AdjustedBeta(D3:D17,C3:C17,B3:B17)</f>
+        <v>0.96073006047914178</v>
+      </c>
+      <c r="H22" s="10">
+        <f>D22-G22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="8" cm="1">
-        <f t="array" ref="C22">SLOPE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0))</f>
+      <c r="C23" s="8" cm="1">
+        <f t="array" ref="C23">SLOPE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0))</f>
         <v>1</v>
       </c>
-      <c r="D22" s="8" cm="1">
-        <f t="array" ref="D22">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0))</f>
+      <c r="D23" s="8" cm="1">
+        <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0))</f>
         <v>1.0869193898495133</v>
       </c>
-      <c r="G22" s="9" cm="1">
-        <f t="array" ref="G22">_xll.BullBeta(D3:D17,C3:C17,B3:B17)</f>
+      <c r="G23" s="9" cm="1">
+        <f t="array" ref="G23">_xll.BullBeta(D3:D17,C3:C17,B3:B17)</f>
         <v>1.0869193898495135</v>
       </c>
-      <c r="H22" s="10">
-        <f t="shared" ref="H22:H31" si="1">D22-G22</f>
-        <v>0</v>
-      </c>
-      <c r="L22" cm="1">
-        <f t="array" ref="L22">_xll.BullBeta(L3:L17,K3:K17)</f>
+      <c r="H23" s="10">
+        <f t="shared" ref="H23:H32" si="1">D23-G23</f>
+        <v>0</v>
+      </c>
+      <c r="L23" cm="1">
+        <f t="array" ref="L23">_xll.BullBeta(L3:L17,K3:K17)</f>
         <v>0.12710524781890767</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="8" cm="1">
-        <f t="array" ref="C23">SLOPE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0))</f>
+      <c r="C24" s="8" cm="1">
+        <f t="array" ref="C24">SLOPE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0))</f>
         <v>1</v>
       </c>
-      <c r="D23" s="8" cm="1">
-        <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0))</f>
+      <c r="D24" s="8" cm="1">
+        <f t="array" ref="D24">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0))</f>
         <v>0.53164017255257146</v>
       </c>
-      <c r="G23" s="9" cm="1">
-        <f t="array" ref="G23">_xll.BearBeta(D3:D17,C3:C17,B3:B17)</f>
+      <c r="G24" s="9" cm="1">
+        <f t="array" ref="G24">_xll.BearBeta(D3:D17,C3:C17,B3:B17)</f>
         <v>0.53164017255257146</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L23" t="e" cm="1">
-        <f t="array" ref="L23">_xll.BearBeta(L3:L17,K3:K17,B3:B17)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="8">
-        <f>C22/C23</f>
-        <v>1</v>
-      </c>
-      <c r="D24" s="8">
-        <f>D22/D23</f>
-        <v>2.0444643688810649</v>
-      </c>
-      <c r="G24" s="9" cm="1">
-        <f t="array" ref="G24">_xll.BetaTimingRatio(D3:D17,C3:C17,B3:B17)</f>
-        <v>2.0444643688810649</v>
       </c>
       <c r="H24" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L24" s="15" t="e" cm="1">
-        <f t="array" ref="L24">_xll.BetaTimingRatio(L3:L17,K3:K17)</f>
+      <c r="L24" t="e" cm="1">
+        <f t="array" ref="L24">_xll.BearBeta(L3:L17,K3:K17,B3:B17)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="8">
+        <f>C23/C24</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="8">
+        <f>D23/D24</f>
+        <v>2.0444643688810649</v>
+      </c>
+      <c r="G25" s="9" cm="1">
+        <f t="array" ref="G25">_xll.BetaTimingRatio(D3:D17,C3:C17,B3:B17)</f>
+        <v>2.0444643688810649</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="15" t="e" cm="1">
+        <f t="array" ref="L25">_xll.BetaTimingRatio(L3:L17,K3:K17)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="8">
+      <c r="B26" s="1"/>
+      <c r="C26" s="8">
         <f>(AVERAGE(C3:C17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(C3:C17)</f>
         <v>-0.11295268790654267</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D26" s="8">
         <f>(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(D3:D17)</f>
         <v>5.1687248496316764E-2</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="G25" s="9" cm="1">
-        <f t="array" ref="G25">_xll.SharpeRatio(D3:D17,B3:B17)</f>
-        <v>5.1687248496316764E-2</v>
-      </c>
-      <c r="H25" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="8" cm="1">
-        <f t="array" ref="C26">(AVERAGE(C3:C17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(C3:C17-$B$3:$B$17)</f>
-        <v>-0.11273902975687349</v>
-      </c>
-      <c r="D26" s="8" cm="1">
-        <f t="array" ref="D26">(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(D3:D17-$B$3:$B$17)</f>
-        <v>5.1676557020390534E-2</v>
-      </c>
       <c r="E26" s="2"/>
       <c r="G26" s="9" cm="1">
-        <f t="array" ref="G26">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
-        <v>5.1676557020390521E-2</v>
+        <f t="array" ref="G26">_xll.SharpeRatio(D3:D17,B3:B17)</f>
+        <v>5.1687248496316764E-2</v>
       </c>
       <c r="H26" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="8" cm="1">
+        <f t="array" ref="C27">(AVERAGE(C3:C17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(C3:C17-$B$3:$B$17)</f>
+        <v>-0.11273902975687349</v>
+      </c>
+      <c r="D27" s="8" cm="1">
+        <f t="array" ref="D27">(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/_xlfn.STDEV.S(D3:D17-$B$3:$B$17)</f>
+        <v>5.1676557020390534E-2</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="G27" s="9" cm="1">
+        <f t="array" ref="G27">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
+        <v>5.1676557020390521E-2</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="8">
+      <c r="B28" s="1"/>
+      <c r="C28" s="8">
         <f>(AVERAGE(C3:C17)-AVERAGE($B$3:$B$17))/C21</f>
         <v>-4.7023516149291567E-4</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D28" s="8">
         <f>(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/D21</f>
         <v>3.0032369912462605E-4</v>
       </c>
-      <c r="G27" s="9" cm="1">
-        <f t="array" ref="G27">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
+      <c r="G28" s="9" cm="1">
+        <f t="array" ref="G28">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
         <v>3.0032369912462605E-4</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H28" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C29" s="8">
         <f>(_xlfn.STDEV.S($C$3:$C$17)/_xlfn.STDEV.S(C3:C17))*(C19-$B$19)+$B$19</f>
         <v>-3.7160406004862107E-4</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D29" s="8">
         <f>(_xlfn.STDEV.S($C$3:$C$17)/_xlfn.STDEV.S(D3:D17))*(D19-$B$19)+$B$19</f>
         <v>3.138111214532042E-4</v>
       </c>
-      <c r="G28" s="9" cm="1">
-        <f t="array" ref="G28">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
+      <c r="G29" s="9" cm="1">
+        <f t="array" ref="G29">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
         <v>3.1381112145320415E-4</v>
-      </c>
-      <c r="H28" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="12" cm="1">
-        <f t="array" ref="C29">INTERCEPT(C3:C17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="12" cm="1">
-        <f t="array" ref="D29">INTERCEPT(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
-        <v>7.2516916083697341E-4</v>
-      </c>
-      <c r="G29" s="13" cm="1">
-        <f t="array" ref="G29">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
-        <v>7.2516916083697341E-4</v>
       </c>
       <c r="H29" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C30" s="12" cm="1">
-        <f t="array" ref="C30">_xlfn.STDEV.S(C3:C17-$C$3:$C$17)</f>
+        <f t="array" ref="C30">INTERCEPT(C3:C17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
         <v>0</v>
       </c>
       <c r="D30" s="12" cm="1">
-        <f t="array" ref="D30">_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
-        <v>3.816440754566235E-3</v>
+        <f t="array" ref="D30">INTERCEPT(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
+        <v>7.2516916083697341E-4</v>
       </c>
       <c r="G30" s="13" cm="1">
-        <f t="array" ref="G30">_xll.TrackingError(D3:D17,C3:C17)</f>
-        <v>3.816440754566235E-3</v>
+        <f t="array" ref="G30">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
+        <v>7.2516916083697341E-4</v>
       </c>
       <c r="H30" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8" cm="1">
-        <f t="array" ref="D31">(AVERAGE(D3:D17)-AVERAGE($C$3:$C$17))/_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
-        <v>0.19726975178765843</v>
-      </c>
-      <c r="G31" s="8" cm="1">
-        <f t="array" ref="G31">_xll.InformationRatio(D3:D17,C3:C17)</f>
-        <v>0.19726975178765843</v>
+        <v>21</v>
+      </c>
+      <c r="C31" s="12" cm="1">
+        <f t="array" ref="C31">_xlfn.STDEV.S(C3:C17-$C$3:$C$17)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="12" cm="1">
+        <f t="array" ref="D31">_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
+        <v>3.816440754566235E-3</v>
+      </c>
+      <c r="G31" s="13" cm="1">
+        <f t="array" ref="G31">_xll.TrackingError(D3:D17,C3:C17)</f>
+        <v>3.816440754566235E-3</v>
       </c>
       <c r="H31" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="1"/>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="G34" s="18" t="str" cm="1">
-        <f t="array" ref="G34:H40">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" cm="1">
+        <f t="array" ref="D32">(AVERAGE(D3:D17)-AVERAGE($C$3:$C$17))/_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
+        <v>0.19726975178765843</v>
+      </c>
+      <c r="G32" s="8" cm="1">
+        <f t="array" ref="G32">_xll.InformationRatio(D3:D17,C3:C17)</f>
+        <v>0.19726975178765843</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="G33" s="10"/>
+      <c r="K33" t="s">
+        <v>30</v>
+      </c>
+      <c r="L33" s="11">
+        <f>AVERAGE(B3:B17)</f>
+        <v>9.8631101444294586E-5</v>
+      </c>
+      <c r="M33" s="11">
+        <f>L33</f>
+        <v>9.8631101444294586E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C34" s="8"/>
+      <c r="G34" s="16"/>
+      <c r="K34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" s="1">
+        <f>AVERAGE(D3:D17)</f>
+        <v>3.8126426031696398E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C35" s="8"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="G35" s="18" t="str" cm="1">
+        <f t="array" ref="G35:H41">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
         <v>Risk Premium</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H35" s="1">
         <v>2.8263315887266938E-4</v>
       </c>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G35" t="str">
+      <c r="J35" s="11"/>
+      <c r="K35" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="1">
+        <f>AVERAGE(B3:B17)+D21*(AVERAGE(C3:C17)-AVERAGE(B3:B17))</f>
+        <v>-3.4390490052000944E-4</v>
+      </c>
+      <c r="M35" s="11">
+        <f>L35</f>
+        <v>-3.4390490052000944E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
         <v>Due to Risk</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H36" s="1">
         <v>-4.4253600196430404E-4</v>
       </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G36" t="str">
+      <c r="K36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="1">
+        <f>L34-L35</f>
+        <v>7.2516916083697341E-4</v>
+      </c>
+      <c r="M36" s="19">
+        <f>M35-M33</f>
+        <v>-4.4253600196430404E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G37" t="str">
         <v>Due to Selectivity</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H37" s="1">
         <v>7.2516916083697341E-4</v>
       </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G37" t="str">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
         <v>Due to Investor's Risk</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H38" s="1">
         <v>-6.1130570994079043E-4</v>
       </c>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G38" t="str">
+      <c r="K38" t="s">
+        <v>31</v>
+      </c>
+      <c r="L38" s="2">
+        <f>_xlfn.COVARIANCE.S(D3:D17,C3:C17)/_xlfn.STDEV.S(C3:C17)</f>
+        <v>3.9233689462754183E-3</v>
+      </c>
+      <c r="M38" s="20">
+        <f>_xlfn.STDEV.S(D3:D17)/_xlfn.STDEV.S(C3:C17)</f>
+        <v>1.3134730578655343</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
         <v>Due to Manager's Risk</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H39" s="1">
         <v>1.6876970797648637E-4</v>
       </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G39" t="str">
+    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
         <v>Diversification</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H40" s="1">
         <v>8.4527012988867047E-5</v>
       </c>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G40" t="str">
+      <c r="K40" t="s">
+        <v>27</v>
+      </c>
+      <c r="L40" s="1">
+        <f>L34-L35*L38</f>
+        <v>3.8261352612413614E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G41" t="str">
         <v>Net Selectivity</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H41" s="1">
         <v>6.4064214784810634E-4</v>
+      </c>
+      <c r="K41" t="s">
+        <v>29</v>
+      </c>
+      <c r="L41" s="1">
+        <f>M35*L38-M33</f>
+        <v>-9.9980367251466734E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>32</v>
+      </c>
+      <c r="L42" s="1">
+        <f>SUM(L40:L41)</f>
+        <v>2.8263315887266938E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some code fixes, clean up, and added intellisense.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9F22D-AEBE-47D9-B9CA-71794CF2D52F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85CE8A2-185E-41B4-820A-22A8CE978E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="3585" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="4815" yWindow="3585" windowWidth="27480" windowHeight="15990" activeTab="1" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>RFR</t>
   </si>
@@ -166,13 +167,67 @@
   </si>
   <si>
     <t>Adjusted Beta</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Magellan</t>
+  </si>
+  <si>
+    <t>44 Wall Street</t>
+  </si>
+  <si>
+    <t>New Horizons</t>
+  </si>
+  <si>
+    <t>S&amp;P 500</t>
+  </si>
+  <si>
+    <t>1Yr Treasury</t>
+  </si>
+  <si>
+    <t>1-Yr Treasury</t>
+  </si>
+  <si>
+    <t>HPR</t>
+  </si>
+  <si>
+    <t>Avg Annual HPR (Arithmetic)</t>
+  </si>
+  <si>
+    <t>Avg Annual HPR (Geometric)</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Correlation with S&amp;P 500</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio (Arithmetic)</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio (Geometric)</t>
+  </si>
+  <si>
+    <t>Treynor Index (Arithmetic)</t>
+  </si>
+  <si>
+    <t>Treynor Index (Geometric)</t>
+  </si>
+  <si>
+    <t>Jensen's Alpha (Arithmetic)</t>
+  </si>
+  <si>
+    <t>Jensen's Alpha (Geometric)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="10">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -181,6 +236,8 @@
     <numFmt numFmtId="168" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;?????_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="0.00000"/>
     <numFmt numFmtId="170" formatCode="0.0000%"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -225,7 +282,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -255,6 +312,17 @@
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -272,6 +340,95 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDCED7E-B802-4702-B75A-25F1B3FA7BA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2476500"/>
+          <a:ext cx="5019675" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Source: Moses, E. A., &amp; Cheney, J. M. (1989). Investments: Analysis, Selection, and Management.West Publishing Company. Table 8.1, page 194.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The calculations at right match</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> those in the source after allowing for slight rounding in the source material.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,13 +1385,13 @@
         <f t="array" ref="C21">_xlfn.COVARIANCE.P(C3:C17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)/_xlfn.VAR.P($C$3:$C$17-$B$3:$B$17)</f>
         <v>1</v>
       </c>
-      <c r="D21" s="8" cm="1">
-        <f t="array" ref="D21">_xlfn.COVARIANCE.S(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)/_xlfn.VAR.S($C$3:$C$17-$B$3:$B$17)</f>
-        <v>0.94109509071871278</v>
+      <c r="D21" s="8">
+        <f>_xlfn.COVARIANCE.S(D3:D17,$C$3:$C$17)/_xlfn.VAR.S($C$3:$C$17)</f>
+        <v>0.94241159407120378</v>
       </c>
       <c r="G21" s="9" cm="1">
-        <f t="array" ref="G21">_xll.Beta(D3:D17,C3:C17,B3:B17)</f>
-        <v>0.94109509071871278</v>
+        <f t="array" ref="G21">_xll.Beta(D3:D17,C3:C17)</f>
+        <v>0.94241159407120412</v>
       </c>
       <c r="H21" s="10">
         <f>D21-G21</f>
@@ -1255,7 +1412,7 @@
       </c>
       <c r="D22" s="8">
         <f>D21*2/3+1/3</f>
-        <v>0.96073006047914178</v>
+        <v>0.96160772938080252</v>
       </c>
       <c r="G22" s="9" cm="1">
         <f t="array" ref="G22">_xll.AdjustedBeta(D3:D17,C3:C17,B3:B17)</f>
@@ -1263,7 +1420,7 @@
       </c>
       <c r="H22" s="10">
         <f>D22-G22</f>
-        <v>0</v>
+        <v>8.7766890166074418E-4</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1398,11 +1555,11 @@
       </c>
       <c r="D28" s="8">
         <f>(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/D21</f>
-        <v>3.0032369912462605E-4</v>
+        <v>2.9990416146271975E-4</v>
       </c>
       <c r="G28" s="9" cm="1">
         <f t="array" ref="G28">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
-        <v>3.0032369912462605E-4</v>
+        <v>2.9990416146271964E-4</v>
       </c>
       <c r="H28" s="10">
         <f t="shared" si="1"/>
@@ -1434,17 +1591,17 @@
       <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="12" cm="1">
-        <f t="array" ref="C30">INTERCEPT(C3:C17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="12" cm="1">
-        <f t="array" ref="D30">INTERCEPT(D3:D17-$B$3:$B$17,$C$3:$C$17-$B$3:$B$17)</f>
-        <v>7.2516916083697341E-4</v>
+      <c r="C30" s="12">
+        <f>C19-$B$19-C21*($C$19-$B$19)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="12">
+        <f>D19-$B$19-D21*($C$19-$B$19)</f>
+        <v>7.2578822700353793E-4</v>
       </c>
       <c r="G30" s="13" cm="1">
         <f t="array" ref="G30">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
-        <v>7.2516916083697341E-4</v>
+        <v>7.2578822700353814E-4</v>
       </c>
       <c r="H30" s="10">
         <f t="shared" si="1"/>
@@ -1540,11 +1697,11 @@
       </c>
       <c r="L35" s="1">
         <f>AVERAGE(B3:B17)+D21*(AVERAGE(C3:C17)-AVERAGE(B3:B17))</f>
-        <v>-3.4390490052000944E-4</v>
+        <v>-3.44523966686574E-4</v>
       </c>
       <c r="M35" s="11">
         <f>L35</f>
-        <v>-3.4390490052000944E-4</v>
+        <v>-3.44523966686574E-4</v>
       </c>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
@@ -1559,11 +1716,11 @@
       </c>
       <c r="L36" s="1">
         <f>L34-L35</f>
-        <v>7.2516916083697341E-4</v>
+        <v>7.2578822700353793E-4</v>
       </c>
       <c r="M36" s="19">
         <f>M35-M33</f>
-        <v>-4.4253600196430404E-4</v>
+        <v>-4.431550681308686E-4</v>
       </c>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.25">
@@ -1614,7 +1771,7 @@
       </c>
       <c r="L40" s="1">
         <f>L34-L35*L38</f>
-        <v>3.8261352612413614E-4</v>
+        <v>3.8261595494910969E-4</v>
       </c>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
@@ -1629,7 +1786,7 @@
       </c>
       <c r="L41" s="1">
         <f>M35*L38-M33</f>
-        <v>-9.9980367251466734E-5</v>
+        <v>-9.9982796076440316E-5</v>
       </c>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
@@ -1644,4 +1801,921 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5E2AEA-8CFA-45DF-BCFE-1A720439ADBA}">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1975</v>
+      </c>
+      <c r="B2" s="22">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="22">
+        <v>10000</v>
+      </c>
+      <c r="D2" s="22">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="22">
+        <v>10000</v>
+      </c>
+      <c r="F2" s="22">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="24">
+        <v>1976</v>
+      </c>
+      <c r="I2" s="14">
+        <f>B3/B2-1</f>
+        <v>0.33600000000000008</v>
+      </c>
+      <c r="J2" s="14">
+        <f t="shared" ref="J2:M11" si="0">C3/C2-1</f>
+        <v>0.46500000000000008</v>
+      </c>
+      <c r="K2" s="14">
+        <f t="shared" si="0"/>
+        <v>0.11099999999999999</v>
+      </c>
+      <c r="L2" s="14">
+        <f t="shared" si="0"/>
+        <v>0.17100000000000004</v>
+      </c>
+      <c r="M2" s="14">
+        <f t="shared" si="0"/>
+        <v>5.7700000000000085E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1976</v>
+      </c>
+      <c r="B3" s="22">
+        <v>13360</v>
+      </c>
+      <c r="C3" s="22">
+        <v>14650</v>
+      </c>
+      <c r="D3" s="22">
+        <v>11110</v>
+      </c>
+      <c r="E3" s="22">
+        <v>11710</v>
+      </c>
+      <c r="F3" s="22">
+        <v>10577</v>
+      </c>
+      <c r="H3" s="24">
+        <v>1977</v>
+      </c>
+      <c r="I3" s="14">
+        <f t="shared" ref="I3:I11" si="1">B4/B3-1</f>
+        <v>0.14498502994011986</v>
+      </c>
+      <c r="J3" s="14">
+        <f t="shared" si="0"/>
+        <v>0.16498293515358364</v>
+      </c>
+      <c r="K3" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12700270027002691</v>
+      </c>
+      <c r="L3" s="14">
+        <f t="shared" si="0"/>
+        <v>0.14500426985482484</v>
+      </c>
+      <c r="M3" s="14">
+        <f t="shared" si="0"/>
+        <v>5.2945069490403673E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1977</v>
+      </c>
+      <c r="B4" s="22">
+        <v>15297</v>
+      </c>
+      <c r="C4" s="22">
+        <v>17067</v>
+      </c>
+      <c r="D4" s="22">
+        <v>12521</v>
+      </c>
+      <c r="E4" s="22">
+        <v>13408</v>
+      </c>
+      <c r="F4" s="22">
+        <v>11137</v>
+      </c>
+      <c r="H4" s="24">
+        <v>1978</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" si="1"/>
+        <v>0.31699025952801207</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="0"/>
+        <v>0.32899748051795874</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" si="0"/>
+        <v>0.20900886510662087</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" si="0"/>
+        <v>8.5023866348448607E-2</v>
+      </c>
+      <c r="M4" s="14">
+        <f t="shared" si="0"/>
+        <v>7.2730537846816823E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1978</v>
+      </c>
+      <c r="B5" s="22">
+        <v>20146</v>
+      </c>
+      <c r="C5" s="22">
+        <v>22682</v>
+      </c>
+      <c r="D5" s="22">
+        <v>15138</v>
+      </c>
+      <c r="E5" s="22">
+        <v>14548</v>
+      </c>
+      <c r="F5" s="22">
+        <v>11947</v>
+      </c>
+      <c r="H5" s="24">
+        <v>1979</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" si="1"/>
+        <v>0.51702571230020844</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.73604620403844456</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.35500066058924551</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.15596645587022273</v>
+      </c>
+      <c r="M5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.10412655896877876</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1979</v>
+      </c>
+      <c r="B6" s="22">
+        <v>30562</v>
+      </c>
+      <c r="C6" s="22">
+        <v>39377</v>
+      </c>
+      <c r="D6" s="22">
+        <v>20512</v>
+      </c>
+      <c r="E6" s="22">
+        <v>16817</v>
+      </c>
+      <c r="F6" s="22">
+        <v>13191</v>
+      </c>
+      <c r="H6" s="24">
+        <v>1980</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="1"/>
+        <v>0.76500229042601919</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.36399420981791408</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.57600429017160693</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.34102396384610811</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12061253885224765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1980</v>
+      </c>
+      <c r="B7" s="22">
+        <v>53942</v>
+      </c>
+      <c r="C7" s="22">
+        <v>53710</v>
+      </c>
+      <c r="D7" s="22">
+        <v>32327</v>
+      </c>
+      <c r="E7" s="22">
+        <v>22552</v>
+      </c>
+      <c r="F7" s="22">
+        <v>14782</v>
+      </c>
+      <c r="H7" s="24">
+        <v>1981</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.1210003336917429</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>-0.22800223422081545</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="0"/>
+        <v>-7.8015281343768339E-2</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="0"/>
+        <v>-4.8022348350478916E-2</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.14077932620754963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1981</v>
+      </c>
+      <c r="B8" s="22">
+        <v>60469</v>
+      </c>
+      <c r="C8" s="22">
+        <v>41464</v>
+      </c>
+      <c r="D8" s="22">
+        <v>29805</v>
+      </c>
+      <c r="E8" s="22">
+        <v>21469</v>
+      </c>
+      <c r="F8" s="22">
+        <v>16863</v>
+      </c>
+      <c r="H8" s="24">
+        <v>1982</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="1"/>
+        <v>0.48100679687112402</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
+        <v>8.4989388385105169E-2</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="0"/>
+        <v>0.22801543365207189</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="0"/>
+        <v>0.22199450370301355</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="0"/>
+        <v>0.14321295143212942</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1982</v>
+      </c>
+      <c r="B9" s="22">
+        <v>89555</v>
+      </c>
+      <c r="C9" s="22">
+        <v>44988</v>
+      </c>
+      <c r="D9" s="22">
+        <v>36601</v>
+      </c>
+      <c r="E9" s="22">
+        <v>26235</v>
+      </c>
+      <c r="F9" s="22">
+        <v>19278</v>
+      </c>
+      <c r="H9" s="24">
+        <v>1983</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="1"/>
+        <v>0.38599743174585455</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="0"/>
+        <v>6.8018138170178766E-2</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.19499467227671374</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.21299790356394133</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="0"/>
+        <v>8.6212262682850982E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1983</v>
+      </c>
+      <c r="B10" s="22">
+        <v>124123</v>
+      </c>
+      <c r="C10" s="22">
+        <v>48048</v>
+      </c>
+      <c r="D10" s="22">
+        <v>43738</v>
+      </c>
+      <c r="E10" s="22">
+        <v>31823</v>
+      </c>
+      <c r="F10" s="22">
+        <v>20940</v>
+      </c>
+      <c r="H10" s="24">
+        <v>1984</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="1"/>
+        <v>1.9996293998694847E-2</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="0"/>
+        <v>-0.59600815850815847</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="0"/>
+        <v>-9.600347523892272E-2</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="0"/>
+        <v>4.1008075919932052E-2</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="0"/>
+        <v>9.8997134670487208E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1984</v>
+      </c>
+      <c r="B11" s="22">
+        <v>126605</v>
+      </c>
+      <c r="C11" s="22">
+        <v>19411</v>
+      </c>
+      <c r="D11" s="22">
+        <v>39539</v>
+      </c>
+      <c r="E11" s="22">
+        <v>33128</v>
+      </c>
+      <c r="F11" s="22">
+        <v>23013</v>
+      </c>
+      <c r="H11" s="24">
+        <v>1985</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.43100193515264018</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="0"/>
+        <v>-0.2009685230024213</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.24300058170414029</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.29899178942284466</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="0"/>
+        <v>9.3295094077260776E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1985</v>
+      </c>
+      <c r="B12" s="22">
+        <v>181172</v>
+      </c>
+      <c r="C12" s="22">
+        <v>15510</v>
+      </c>
+      <c r="D12" s="22">
+        <v>49147</v>
+      </c>
+      <c r="E12" s="22">
+        <v>43033</v>
+      </c>
+      <c r="F12" s="22">
+        <v>25160</v>
+      </c>
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="26" cm="1">
+        <f t="array" ref="I13">PRODUCT(1+I2:I11)-1</f>
+        <v>17.117200000000004</v>
+      </c>
+      <c r="J13" s="26" cm="1">
+        <f t="array" ref="J13">PRODUCT(1+J2:J11)-1</f>
+        <v>0.5510000000000006</v>
+      </c>
+      <c r="K13" s="26" cm="1">
+        <f t="array" ref="K13">PRODUCT(1+K2:K11)-1</f>
+        <v>3.9146999999999998</v>
+      </c>
+      <c r="L13" s="26" cm="1">
+        <f t="array" ref="L13">PRODUCT(1+L2:L11)-1</f>
+        <v>3.3032999999999992</v>
+      </c>
+      <c r="M13" s="26" cm="1">
+        <f t="array" ref="M13">PRODUCT(1+M2:M11)-1</f>
+        <v>1.516</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="26">
+        <f>AVERAGE(I2:I11)</f>
+        <v>0.35190060836544157</v>
+      </c>
+      <c r="J14" s="26">
+        <f t="shared" ref="J14:M14" si="2">AVERAGE(J2:J11)</f>
+        <v>0.11870494403517898</v>
+      </c>
+      <c r="K14" s="26">
+        <f t="shared" si="2"/>
+        <v>0.18700084471877351</v>
+      </c>
+      <c r="L14" s="26">
+        <f t="shared" si="2"/>
+        <v>0.16249884801788569</v>
+      </c>
+      <c r="M14" s="26">
+        <f t="shared" si="2"/>
+        <v>9.7061147422852503E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="26" cm="1">
+        <f t="array" ref="I15">GEOMEAN(1+I2:I11)-1</f>
+        <v>0.33600815124726502</v>
+      </c>
+      <c r="J15" s="26" cm="1">
+        <f t="array" ref="J15">GEOMEAN(1+J2:J11)-1</f>
+        <v>4.4867401051168043E-2</v>
+      </c>
+      <c r="K15" s="26" cm="1">
+        <f t="array" ref="K15">GEOMEAN(1+K2:K11)-1</f>
+        <v>0.17259949092949345</v>
+      </c>
+      <c r="L15" s="26" cm="1">
+        <f t="array" ref="L15">GEOMEAN(1+L2:L11)-1</f>
+        <v>0.15712469523352701</v>
+      </c>
+      <c r="M15" s="26" cm="1">
+        <f t="array" ref="M15">GEOMEAN(1+M2:M11)-1</f>
+        <v>9.6657627730115214E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="14">
+        <f>_xlfn.STDEV.S(I2:I11)</f>
+        <v>0.21852239905084198</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" ref="J16:M16" si="3">_xlfn.STDEV.S(J2:J11)</f>
+        <v>0.38650566005190573</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" si="3"/>
+        <v>0.19567970936600529</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="3"/>
+        <v>0.11647316538757187</v>
+      </c>
+      <c r="M16" s="14">
+        <f t="shared" si="3"/>
+        <v>3.1391776300293349E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="21">
+        <f>CORREL(I2:I11,$L$2:$L$11)</f>
+        <v>0.82068383022789493</v>
+      </c>
+      <c r="J17" s="21">
+        <f t="shared" ref="J17:M17" si="4">CORREL(J2:J11,$L$2:$L$11)</f>
+        <v>0.33868524468644617</v>
+      </c>
+      <c r="K17" s="21">
+        <f t="shared" si="4"/>
+        <v>0.81760384770774464</v>
+      </c>
+      <c r="L17" s="21">
+        <f t="shared" si="4"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="M17" s="21">
+        <f t="shared" si="4"/>
+        <v>-3.872533196034407E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="21">
+        <f>_xlfn.COVARIANCE.S(I2:I11,$L$2:$L$11)/_xlfn.VAR.S($L$2:$L$11)</f>
+        <v>1.539734915307535</v>
+      </c>
+      <c r="J18" s="21">
+        <f t="shared" ref="J18:M18" si="5">_xlfn.COVARIANCE.S(J2:J11,$L$2:$L$11)/_xlfn.VAR.S($L$2:$L$11)</f>
+        <v>1.1238963379400353</v>
+      </c>
+      <c r="K18" s="21">
+        <f t="shared" si="5"/>
+        <v>1.3736080990295689</v>
+      </c>
+      <c r="L18" s="21">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="M18" s="21">
+        <f t="shared" si="5"/>
+        <v>-1.0437227785546531E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="21">
+        <f>(I14-$M$14)/I16</f>
+        <v>1.1661937725811691</v>
+      </c>
+      <c r="J19" s="21">
+        <f t="shared" ref="J19:M19" si="6">(J14-$M$14)/J16</f>
+        <v>5.5998653705148387E-2</v>
+      </c>
+      <c r="K19" s="21">
+        <f t="shared" si="6"/>
+        <v>0.45962709975051658</v>
+      </c>
+      <c r="L19" s="21">
+        <f t="shared" si="6"/>
+        <v>0.56182641192316773</v>
+      </c>
+      <c r="M19" s="21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="21">
+        <f>(I15-$M$15)/I16</f>
+        <v>1.0953134532513618</v>
+      </c>
+      <c r="J20" s="21">
+        <f t="shared" ref="J20:M20" si="7">(J15-$M$15)/J16</f>
+        <v>-0.13399603688078465</v>
+      </c>
+      <c r="K20" s="21">
+        <f t="shared" si="7"/>
+        <v>0.38809268189035512</v>
+      </c>
+      <c r="L20" s="21">
+        <f t="shared" si="7"/>
+        <v>0.5191502034155574</v>
+      </c>
+      <c r="M20" s="21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="21">
+        <f>(I14-$M$14)/I18</f>
+        <v>0.16550865893152092</v>
+      </c>
+      <c r="J21" s="21">
+        <f t="shared" ref="J21:M21" si="8">(J14-$M$14)/J18</f>
+        <v>1.925782288070883E-2</v>
+      </c>
+      <c r="K21" s="21">
+        <f t="shared" si="8"/>
+        <v>6.5476970730925288E-2</v>
+      </c>
+      <c r="L21" s="21">
+        <f t="shared" si="8"/>
+        <v>6.5437700595033177E-2</v>
+      </c>
+      <c r="M21" s="21">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="27">
+        <f>(I15-$M$15)/I18</f>
+        <v>0.15544917578838155</v>
+      </c>
+      <c r="J22" s="27">
+        <f t="shared" ref="J22:M22" si="9">(J15-$M$15)/J18</f>
+        <v>-4.6080963991636748E-2</v>
+      </c>
+      <c r="K22" s="27">
+        <f t="shared" si="9"/>
+        <v>5.5286411934401002E-2</v>
+      </c>
+      <c r="L22" s="27">
+        <f t="shared" si="9"/>
+        <v>6.0467067503411784E-2</v>
+      </c>
+      <c r="M22" s="27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="21" cm="1">
+        <f t="array" ref="I23">AVERAGE(I2:I11-$M$2:$M$11)-I18*AVERAGE($L$2:$L$11-$M$2:$M$11)</f>
+        <v>0.15408274855897586</v>
+      </c>
+      <c r="J23" s="21" cm="1">
+        <f t="array" ref="J23">AVERAGE(J2:J11-$M$2:$M$11)-J18*AVERAGE($L$2:$L$11-$M$2:$M$11)</f>
+        <v>-5.1901395449647801E-2</v>
+      </c>
+      <c r="K23" s="21" cm="1">
+        <f t="array" ref="K23">AVERAGE(K2:K11-$M$2:$M$11)-K18*AVERAGE($L$2:$L$11-$M$2:$M$11)</f>
+        <v>5.3941776711363687E-5</v>
+      </c>
+      <c r="L23" s="21" cm="1">
+        <f t="array" ref="L23">AVERAGE(L2:L11-$M$2:$M$11)-L18*AVERAGE($L$2:$L$11-$M$2:$M$11)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="21" cm="1">
+        <f t="array" ref="M23">AVERAGE(M2:M11-$M$2:$M$11)-M18*AVERAGE($L$2:$L$11-$M$2:$M$11)</f>
+        <v>6.8298818687275538E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="21" cm="1">
+        <f t="array" ref="I24">(GEOMEAN(1+I2:I11-$M$2:$M$11)-1)-I18*(GEOMEAN(1+$L$2:$L$11-$M$2:$M$11)-1)</f>
+        <v>0.14784041632705563</v>
+      </c>
+      <c r="J24" s="21" cm="1">
+        <f t="array" ref="J24">(GEOMEAN(1+J2:J11-$M$2:$M$11)-1)-J18*(GEOMEAN(1+$L$2:$L$11-$M$2:$M$11)-1)</f>
+        <v>-0.13274680018062748</v>
+      </c>
+      <c r="K24" s="21" cm="1">
+        <f t="array" ref="K24">(GEOMEAN(1+K2:K11-$M$2:$M$11)-1)-K18*(GEOMEAN(1+$L$2:$L$11-$M$2:$M$11)-1)</f>
+        <v>-7.0162470757607759E-3</v>
+      </c>
+      <c r="L24" s="21" cm="1">
+        <f t="array" ref="L24">(GEOMEAN(1+L2:L11-$M$2:$M$11)-1)-L18*(GEOMEAN(1+$L$2:$L$11-$M$2:$M$11)-1)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="21" cm="1">
+        <f t="array" ref="M24">(GEOMEAN(1+M2:M11-$M$2:$M$11)-1)-M18*(GEOMEAN(1+$L$2:$L$11-$M$2:$M$11)-1)</f>
+        <v>6.1288769290833965E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="21" cm="1">
+        <f t="array" ref="I27">_xll.Beta(I2:I11,$L$2:$L$11)</f>
+        <v>1.5397349153075346</v>
+      </c>
+      <c r="J27" s="21" cm="1">
+        <f t="array" ref="J27">_xll.Beta(J2:J11,$L$2:$L$11)</f>
+        <v>1.1238963379400351</v>
+      </c>
+      <c r="K27" s="21" cm="1">
+        <f t="array" ref="K27">_xll.Beta(K2:K11,$L$2:$L$11)</f>
+        <v>1.3736080990295685</v>
+      </c>
+      <c r="L27" s="21" cm="1">
+        <f t="array" ref="L27">_xll.Beta(L2:L11,$L$2:$L$11)</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="21" cm="1">
+        <f t="array" ref="M27">_xll.Beta(M2:M11,$L$2:$L$11)</f>
+        <v>-1.0437227785546526E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="21" cm="1">
+        <f t="array" ref="I28">_xll.SharpeRatio(I2:I11,$M$2:$M$11)</f>
+        <v>1.1661937725811693</v>
+      </c>
+      <c r="J28" s="21" cm="1">
+        <f t="array" ref="J28">_xll.SharpeRatio(J2:J11,$M$2:$M$11)</f>
+        <v>5.599865370514838E-2</v>
+      </c>
+      <c r="K28" s="21" cm="1">
+        <f t="array" ref="K28">_xll.SharpeRatio(K2:K11,$M$2:$M$11)</f>
+        <v>0.45962709975051652</v>
+      </c>
+      <c r="L28" s="21" cm="1">
+        <f t="array" ref="L28">_xll.SharpeRatio(L2:L11,$M$2:$M$11)</f>
+        <v>0.56182641192316762</v>
+      </c>
+      <c r="M28" s="21" cm="1">
+        <f t="array" ref="M28">_xll.SharpeRatio(M2:M11,$M$2:$M$11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="21" cm="1">
+        <f t="array" ref="I29">_xll.TreynorIndex(I2:I11,I27,$M$2:$M$11)</f>
+        <v>0.16550865893152097</v>
+      </c>
+      <c r="J29" s="21" cm="1">
+        <f t="array" ref="J29">_xll.TreynorIndex(J2:J11,J27,$M$2:$M$11)</f>
+        <v>1.9257822880708833E-2</v>
+      </c>
+      <c r="K29" s="21" cm="1">
+        <f t="array" ref="K29">_xll.TreynorIndex(K2:K11,K27,$M$2:$M$11)</f>
+        <v>6.5476970730925316E-2</v>
+      </c>
+      <c r="L29" s="21" cm="1">
+        <f t="array" ref="L29">_xll.TreynorIndex(L2:L11,L27,$M$2:$M$11)</f>
+        <v>6.5437700595033191E-2</v>
+      </c>
+      <c r="M29" s="21" cm="1">
+        <f t="array" ref="M29">_xll.TreynorIndex(M2:M11,M27,$M$2:$M$11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="21" cm="1">
+        <f t="array" ref="I30">_xll.JensensAlpha(I2:I11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>0.15408274855897586</v>
+      </c>
+      <c r="J30" s="21" cm="1">
+        <f t="array" ref="J30">_xll.JensensAlpha(J2:J11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>-5.190139544964778E-2</v>
+      </c>
+      <c r="K30" s="21" cm="1">
+        <f t="array" ref="K30">_xll.JensensAlpha(K2:K11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>5.394177671140532E-5</v>
+      </c>
+      <c r="L30" s="21" cm="1">
+        <f t="array" ref="L30">_xll.JensensAlpha(L2:L11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="21" cm="1">
+        <f t="array" ref="M30">_xll.JensensAlpha(M2:M11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>6.8298818687275483E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated documentation and revised Jensen's alpha and Fama's decomposition functions.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85CE8A2-185E-41B4-820A-22A8CE978E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201E7D9D-9193-4516-BFD8-35D26065A8BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="3585" windowWidth="27480" windowHeight="15990" activeTab="1" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="4815" yWindow="3585" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>RFR</t>
   </si>
@@ -140,30 +140,6 @@
   </si>
   <si>
     <t>Revised Sharpe Ratio</t>
-  </si>
-  <si>
-    <t>Rx</t>
-  </si>
-  <si>
-    <t>Rp</t>
-  </si>
-  <si>
-    <t>Selectivity</t>
-  </si>
-  <si>
-    <t>Diff</t>
-  </si>
-  <si>
-    <t>Risk</t>
-  </si>
-  <si>
-    <t>Rf</t>
-  </si>
-  <si>
-    <t>Fama Beta</t>
-  </si>
-  <si>
-    <t>Sum</t>
   </si>
   <si>
     <t>Adjusted Beta</t>
@@ -227,7 +203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="12">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -238,6 +214,8 @@
     <numFmt numFmtId="170" formatCode="0.0000%"/>
     <numFmt numFmtId="171" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="172" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="0.00000000000000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -282,7 +260,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -323,6 +301,10 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -728,21 +710,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1306,7 +1291,7 @@
         <v>-6.3539265847126769E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>8.218509209156899E-5</v>
       </c>
@@ -1331,11 +1316,11 @@
         <v>2.6039764394154563E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1351,12 +1336,13 @@
         <f>AVERAGE(D3:D17)</f>
         <v>3.8126426031696398E-4</v>
       </c>
+      <c r="E19" s="30"/>
       <c r="G19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1377,7 +1363,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1402,9 +1388,9 @@
         <v>0.12710524781890767</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C22" s="8">
         <f>C21*2/3+1/3</f>
@@ -1415,15 +1401,15 @@
         <v>0.96160772938080252</v>
       </c>
       <c r="G22" s="9" cm="1">
-        <f t="array" ref="G22">_xll.AdjustedBeta(D3:D17,C3:C17,B3:B17)</f>
-        <v>0.96073006047914178</v>
+        <f t="array" ref="G22">_xll.AdjustedBeta(D3:D17,C3:C17)</f>
+        <v>0.96160772938080274</v>
       </c>
       <c r="H22" s="10">
         <f>D22-G22</f>
-        <v>8.7766890166074418E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1448,7 +1434,7 @@
         <v>0.12710524781890767</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1459,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1498,7 +1484,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1521,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1544,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1566,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -1608,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1629,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1646,117 +1632,71 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L32" t="s">
-        <v>27</v>
-      </c>
-      <c r="M32" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="G33" s="10"/>
-      <c r="K33" t="s">
-        <v>30</v>
-      </c>
-      <c r="L33" s="11">
-        <f>AVERAGE(B3:B17)</f>
-        <v>9.8631101444294586E-5</v>
-      </c>
-      <c r="M33" s="11">
-        <f>L33</f>
-        <v>9.8631101444294586E-5</v>
-      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C34" s="8"/>
       <c r="G34" s="16"/>
-      <c r="K34" t="s">
-        <v>26</v>
-      </c>
-      <c r="L34" s="1">
-        <f>AVERAGE(D3:D17)</f>
-        <v>3.8126426031696398E-4</v>
-      </c>
+      <c r="L34" s="1"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C35" s="8"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="G35" s="18" t="str" cm="1">
-        <f t="array" ref="G35:H41">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
+        <f t="array" ref="G35:H44">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
         <v>Risk Premium</v>
       </c>
       <c r="H35" s="1">
         <v>2.8263315887266938E-4</v>
       </c>
+      <c r="I35" s="30"/>
       <c r="J35" s="11"/>
-      <c r="K35" t="s">
-        <v>25</v>
-      </c>
-      <c r="L35" s="1">
-        <f>AVERAGE(B3:B17)+D21*(AVERAGE(C3:C17)-AVERAGE(B3:B17))</f>
-        <v>-3.44523966686574E-4</v>
-      </c>
-      <c r="M35" s="11">
-        <f>L35</f>
-        <v>-3.44523966686574E-4</v>
-      </c>
+      <c r="L35" s="1"/>
+      <c r="M35" s="11"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G36" t="str">
         <v>Due to Risk</v>
       </c>
       <c r="H36" s="1">
-        <v>-4.4253600196430404E-4</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="1">
-        <f>L34-L35</f>
-        <v>7.2578822700353793E-4</v>
-      </c>
-      <c r="M36" s="19">
-        <f>M35-M33</f>
-        <v>-4.431550681308686E-4</v>
-      </c>
+        <v>-4.4315506813086877E-4</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="19"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G37" t="str">
-        <v>Due to Selectivity</v>
+        <v>Due to Investor's Risk</v>
       </c>
       <c r="H37" s="1">
-        <v>7.2516916083697341E-4</v>
+        <v>-6.1130570994079043E-4</v>
       </c>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G38" t="str">
-        <v>Due to Investor's Risk</v>
+        <v>Due to Manager's Risk</v>
       </c>
       <c r="H38" s="1">
-        <v>-6.1130570994079043E-4</v>
-      </c>
-      <c r="K38" t="s">
-        <v>31</v>
-      </c>
-      <c r="L38" s="2">
-        <f>_xlfn.COVARIANCE.S(D3:D17,C3:C17)/_xlfn.STDEV.S(C3:C17)</f>
-        <v>3.9233689462754183E-3</v>
-      </c>
-      <c r="M38" s="20">
-        <f>_xlfn.STDEV.S(D3:D17)/_xlfn.STDEV.S(C3:C17)</f>
-        <v>1.3134730578655343</v>
-      </c>
+        <v>1.6815064180992164E-4</v>
+      </c>
+      <c r="L38" s="2"/>
+      <c r="M38" s="20"/>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G39" t="str">
-        <v>Due to Manager's Risk</v>
+        <v>Due to Selectivity</v>
       </c>
       <c r="H39" s="1">
-        <v>1.6876970797648637E-4</v>
+        <v>7.2578822700353814E-4</v>
       </c>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
@@ -1764,15 +1704,9 @@
         <v>Diversification</v>
       </c>
       <c r="H40" s="1">
-        <v>8.4527012988867047E-5</v>
-      </c>
-      <c r="K40" t="s">
-        <v>27</v>
-      </c>
-      <c r="L40" s="1">
-        <f>L34-L35*L38</f>
-        <v>3.8261595494910969E-4</v>
-      </c>
+        <v>8.5146079155431776E-5</v>
+      </c>
+      <c r="L40" s="1"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
       <c r="G41" t="str">
@@ -1781,22 +1715,43 @@
       <c r="H41" s="1">
         <v>6.4064214784810634E-4</v>
       </c>
-      <c r="K41" t="s">
-        <v>29</v>
-      </c>
-      <c r="L41" s="1">
-        <f>M35*L38-M33</f>
-        <v>-9.9982796076440316E-5</v>
-      </c>
+      <c r="L41" s="1"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="K42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L42" s="1">
-        <f>SUM(L40:L41)</f>
-        <v>2.8263315887266938E-4</v>
-      </c>
+      <c r="G42" t="str">
+        <v>Hypothetical Beta</v>
+      </c>
+      <c r="H42" s="29">
+        <v>1.3134730578655345</v>
+      </c>
+      <c r="J42" s="8"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G43" t="str">
+        <v>Hypothetical Exp Return</v>
+      </c>
+      <c r="H43" s="1">
+        <v>-5.1901011403769886E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G44" t="str">
+        <v>Hypothetical Risk Premium</v>
+      </c>
+      <c r="H44" s="1">
+        <v>-6.176412154819934E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H45" s="28"/>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1807,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5E2AEA-8CFA-45DF-BCFE-1A720439ADBA}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -1827,40 +1782,40 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="M1" s="25" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2316,7 +2271,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I13" s="26" cm="1">
         <f t="array" ref="I13">PRODUCT(1+I2:I11)-1</f>
@@ -2341,7 +2296,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="I14" s="26">
         <f>AVERAGE(I2:I11)</f>
@@ -2366,7 +2321,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I15" s="26" cm="1">
         <f t="array" ref="I15">GEOMEAN(1+I2:I11)-1</f>
@@ -2391,7 +2346,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I16" s="14">
         <f>_xlfn.STDEV.S(I2:I11)</f>
@@ -2416,7 +2371,7 @@
     </row>
     <row r="17" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I17" s="21">
         <f>CORREL(I2:I11,$L$2:$L$11)</f>
@@ -2466,7 +2421,7 @@
     </row>
     <row r="19" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I19" s="21">
         <f>(I14-$M$14)/I16</f>
@@ -2491,7 +2446,7 @@
     </row>
     <row r="20" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I20" s="21">
         <f>(I15-$M$15)/I16</f>
@@ -2516,7 +2471,7 @@
     </row>
     <row r="21" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I21" s="21">
         <f>(I14-$M$14)/I18</f>
@@ -2541,7 +2496,7 @@
     </row>
     <row r="22" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I22" s="27">
         <f>(I15-$M$15)/I18</f>
@@ -2566,7 +2521,7 @@
     </row>
     <row r="23" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I23" s="21" cm="1">
         <f t="array" ref="I23">AVERAGE(I2:I11-$M$2:$M$11)-I18*AVERAGE($L$2:$L$11-$M$2:$M$11)</f>
@@ -2591,7 +2546,7 @@
     </row>
     <row r="24" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I24" s="21" cm="1">
         <f t="array" ref="I24">(GEOMEAN(1+I2:I11-$M$2:$M$11)-1)-I18*(GEOMEAN(1+$L$2:$L$11-$M$2:$M$11)-1)</f>

</xml_diff>

<commit_message>
Changed beta functions to not allow risk-free rates. Updtaed documentation.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201E7D9D-9193-4516-BFD8-35D26065A8BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABE88EF-D75D-478E-8EC9-9DE04BEC403E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="3585" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="5160" yWindow="3930" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,12 +1418,12 @@
         <v>1</v>
       </c>
       <c r="D23" s="8" cm="1">
-        <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&gt;0))</f>
-        <v>1.0869193898495133</v>
+        <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0))</f>
+        <v>1.0869212641710992</v>
       </c>
       <c r="G23" s="9" cm="1">
-        <f t="array" ref="G23">_xll.BullBeta(D3:D17,C3:C17,B3:B17)</f>
-        <v>1.0869193898495135</v>
+        <f t="array" ref="G23">_xll.BullBeta(D3:D17,C3:C17)</f>
+        <v>1.0869212641710995</v>
       </c>
       <c r="H23" s="10">
         <f t="shared" ref="H23:H32" si="1">D23-G23</f>
@@ -1443,12 +1443,12 @@
         <v>1</v>
       </c>
       <c r="D24" s="8" cm="1">
-        <f t="array" ref="D24">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0)-_xlfn._xlws.FILTER($B$3:$B$17,$C$3:$C$17&lt;0))</f>
-        <v>0.53164017255257146</v>
+        <f t="array" ref="D24">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0))</f>
+        <v>0.54207326774062659</v>
       </c>
       <c r="G24" s="9" cm="1">
-        <f t="array" ref="G24">_xll.BearBeta(D3:D17,C3:C17,B3:B17)</f>
-        <v>0.53164017255257146</v>
+        <f t="array" ref="G24">_xll.BearBeta(D3:D17,C3:C17)</f>
+        <v>0.54207326774062647</v>
       </c>
       <c r="H24" s="10">
         <f t="shared" si="1"/>
@@ -1469,11 +1469,11 @@
       </c>
       <c r="D25" s="8">
         <f>D23/D24</f>
-        <v>2.0444643688810649</v>
+        <v>2.0051187336748981</v>
       </c>
       <c r="G25" s="9" cm="1">
-        <f t="array" ref="G25">_xll.BetaTimingRatio(D3:D17,C3:C17,B3:B17)</f>
-        <v>2.0444643688810649</v>
+        <f t="array" ref="G25">_xll.BetaTimingRatio(D3:D17,C3:C17)</f>
+        <v>2.005118733674899</v>
       </c>
       <c r="H25" s="10">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Upload new build of add-ins.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABE88EF-D75D-478E-8EC9-9DE04BEC403E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="3930" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="5505" yWindow="4275" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,17 +1375,17 @@
         <f>_xlfn.COVARIANCE.S(D3:D17,$C$3:$C$17)/_xlfn.VAR.S($C$3:$C$17)</f>
         <v>0.94241159407120378</v>
       </c>
-      <c r="G21" s="9" cm="1">
-        <f t="array" ref="G21">_xll.Beta(D3:D17,C3:C17)</f>
-        <v>0.94241159407120412</v>
-      </c>
-      <c r="H21" s="10">
-        <f>D21-G21</f>
-        <v>0</v>
-      </c>
-      <c r="L21" cm="1">
-        <f t="array" ref="L21">_xll.Beta(L3:L17,K3:K17)</f>
-        <v>0.12710524781890767</v>
+      <c r="G21" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G21" ca="1">_xll.Beta(D3:D17,C3:C17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H21" s="10" t="e">
+        <f ca="1">D21-G21</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L21" t="e" cm="1">
+        <f t="array" aca="1" ref="L21" ca="1">_xll.Beta(L3:L17,K3:K17)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1400,13 +1400,13 @@
         <f>D21*2/3+1/3</f>
         <v>0.96160772938080252</v>
       </c>
-      <c r="G22" s="9" cm="1">
-        <f t="array" ref="G22">_xll.AdjustedBeta(D3:D17,C3:C17)</f>
-        <v>0.96160772938080274</v>
-      </c>
-      <c r="H22" s="10">
-        <f>D22-G22</f>
-        <v>0</v>
+      <c r="G22" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G22" ca="1">_xll.AdjustedBeta(D3:D17,C3:C17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H22" s="10" t="e">
+        <f ca="1">D22-G22</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1421,17 +1421,17 @@
         <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0))</f>
         <v>1.0869212641710992</v>
       </c>
-      <c r="G23" s="9" cm="1">
-        <f t="array" ref="G23">_xll.BullBeta(D3:D17,C3:C17)</f>
-        <v>1.0869212641710995</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" ref="H23:H32" si="1">D23-G23</f>
-        <v>0</v>
-      </c>
-      <c r="L23" cm="1">
-        <f t="array" ref="L23">_xll.BullBeta(L3:L17,K3:K17)</f>
-        <v>0.12710524781890767</v>
+      <c r="G23" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G23" ca="1">_xll.BullBeta(D3:D17,C3:C17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H23" s="10" t="e">
+        <f t="shared" ref="H23:H32" ca="1" si="1">D23-G23</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L23" t="e" cm="1">
+        <f t="array" aca="1" ref="L23" ca="1">_xll.BullBeta(L3:L17,K3:K17)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1446,16 +1446,16 @@
         <f t="array" ref="D24">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0))</f>
         <v>0.54207326774062659</v>
       </c>
-      <c r="G24" s="9" cm="1">
-        <f t="array" ref="G24">_xll.BearBeta(D3:D17,C3:C17)</f>
-        <v>0.54207326774062647</v>
-      </c>
-      <c r="H24" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G24" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G24" ca="1">_xll.BearBeta(D3:D17,C3:C17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H24" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="L24" t="e" cm="1">
-        <f t="array" ref="L24">_xll.BearBeta(L3:L17,K3:K17,B3:B17)</f>
+        <f t="array" aca="1" ref="L24" ca="1">_xll.BearBeta(L3:L17,K3:K17,B3:B17)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1471,16 +1471,16 @@
         <f>D23/D24</f>
         <v>2.0051187336748981</v>
       </c>
-      <c r="G25" s="9" cm="1">
-        <f t="array" ref="G25">_xll.BetaTimingRatio(D3:D17,C3:C17)</f>
-        <v>2.005118733674899</v>
-      </c>
-      <c r="H25" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G25" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G25" ca="1">_xll.BetaTimingRatio(D3:D17,C3:C17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H25" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="L25" s="15" t="e" cm="1">
-        <f t="array" ref="L25">_xll.BetaTimingRatio(L3:L17,K3:K17)</f>
+        <f t="array" aca="1" ref="L25" ca="1">_xll.BetaTimingRatio(L3:L17,K3:K17)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1498,13 +1498,13 @@
         <v>5.1687248496316764E-2</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="G26" s="9" cm="1">
-        <f t="array" ref="G26">_xll.SharpeRatio(D3:D17,B3:B17)</f>
-        <v>5.1687248496316764E-2</v>
-      </c>
-      <c r="H26" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G26" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G26" ca="1">_xll.SharpeRatio(D3:D17,B3:B17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H26" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1521,13 +1521,13 @@
         <v>5.1676557020390534E-2</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="G27" s="9" cm="1">
-        <f t="array" ref="G27">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
-        <v>5.1676557020390521E-2</v>
-      </c>
-      <c r="H27" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G27" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G27" ca="1">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H27" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1543,13 +1543,13 @@
         <f>(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/D21</f>
         <v>2.9990416146271975E-4</v>
       </c>
-      <c r="G28" s="9" cm="1">
-        <f t="array" ref="G28">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
-        <v>2.9990416146271964E-4</v>
-      </c>
-      <c r="H28" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G28" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G28" ca="1">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H28" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1564,13 +1564,13 @@
         <f>(_xlfn.STDEV.S($C$3:$C$17)/_xlfn.STDEV.S(D3:D17))*(D19-$B$19)+$B$19</f>
         <v>3.138111214532042E-4</v>
       </c>
-      <c r="G29" s="9" cm="1">
-        <f t="array" ref="G29">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
-        <v>3.1381112145320415E-4</v>
-      </c>
-      <c r="H29" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G29" s="9" t="e" cm="1">
+        <f t="array" aca="1" ref="G29" ca="1">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H29" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1585,13 +1585,13 @@
         <f>D19-$B$19-D21*($C$19-$B$19)</f>
         <v>7.2578822700353793E-4</v>
       </c>
-      <c r="G30" s="13" cm="1">
-        <f t="array" ref="G30">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
-        <v>7.2578822700353814E-4</v>
-      </c>
-      <c r="H30" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G30" s="13" t="e" cm="1">
+        <f t="array" aca="1" ref="G30" ca="1">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H30" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1606,13 +1606,13 @@
         <f t="array" ref="D31">_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
         <v>3.816440754566235E-3</v>
       </c>
-      <c r="G31" s="13" cm="1">
-        <f t="array" ref="G31">_xll.TrackingError(D3:D17,C3:C17)</f>
-        <v>3.816440754566235E-3</v>
-      </c>
-      <c r="H31" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G31" s="13" t="e" cm="1">
+        <f t="array" aca="1" ref="G31" ca="1">_xll.TrackingError(D3:D17,C3:C17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H31" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1624,13 +1624,13 @@
         <f t="array" ref="D32">(AVERAGE(D3:D17)-AVERAGE($C$3:$C$17))/_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
         <v>0.19726975178765843</v>
       </c>
-      <c r="G32" s="8" cm="1">
-        <f t="array" ref="G32">_xll.InformationRatio(D3:D17,C3:C17)</f>
-        <v>0.19726975178765843</v>
-      </c>
-      <c r="H32" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G32" s="8" t="e" cm="1">
+        <f t="array" aca="1" ref="G32" ca="1">_xll.InformationRatio(D3:D17,C3:C17)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H32" s="10" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.25">
@@ -1649,100 +1649,53 @@
       <c r="C35" s="8"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
-      <c r="G35" s="18" t="str" cm="1">
-        <f t="array" ref="G35:H44">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
-        <v>Risk Premium</v>
-      </c>
-      <c r="H35" s="1">
-        <v>2.8263315887266938E-4</v>
-      </c>
+      <c r="G35" s="18" t="e" cm="1">
+        <f t="array" aca="1" ref="G35" ca="1">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H35" s="1"/>
       <c r="I35" s="30"/>
       <c r="J35" s="11"/>
       <c r="L35" s="1"/>
       <c r="M35" s="11"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G36" t="str">
-        <v>Due to Risk</v>
-      </c>
-      <c r="H36" s="1">
-        <v>-4.4315506813086877E-4</v>
-      </c>
+      <c r="H36" s="1"/>
       <c r="K36" s="11"/>
       <c r="L36" s="1"/>
       <c r="M36" s="19"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G37" t="str">
-        <v>Due to Investor's Risk</v>
-      </c>
-      <c r="H37" s="1">
-        <v>-6.1130570994079043E-4</v>
-      </c>
+      <c r="H37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G38" t="str">
-        <v>Due to Manager's Risk</v>
-      </c>
-      <c r="H38" s="1">
-        <v>1.6815064180992164E-4</v>
-      </c>
+      <c r="H38" s="1"/>
       <c r="L38" s="2"/>
       <c r="M38" s="20"/>
     </row>
     <row r="39" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G39" t="str">
-        <v>Due to Selectivity</v>
-      </c>
-      <c r="H39" s="1">
-        <v>7.2578822700353814E-4</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G40" t="str">
-        <v>Diversification</v>
-      </c>
-      <c r="H40" s="1">
-        <v>8.5146079155431776E-5</v>
-      </c>
+      <c r="H40" s="1"/>
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G41" t="str">
-        <v>Net Selectivity</v>
-      </c>
-      <c r="H41" s="1">
-        <v>6.4064214784810634E-4</v>
-      </c>
+      <c r="H41" s="1"/>
       <c r="L41" s="1"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G42" t="str">
-        <v>Hypothetical Beta</v>
-      </c>
-      <c r="H42" s="29">
-        <v>1.3134730578655345</v>
-      </c>
+      <c r="H42" s="29"/>
       <c r="J42" s="8"/>
       <c r="K42" s="31"/>
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G43" t="str">
-        <v>Hypothetical Exp Return</v>
-      </c>
-      <c r="H43" s="1">
-        <v>-5.1901011403769886E-4</v>
-      </c>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="G44" t="str">
-        <v>Hypothetical Risk Premium</v>
-      </c>
-      <c r="H44" s="1">
-        <v>-6.176412154819934E-4</v>
-      </c>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
       <c r="H45" s="28"/>
@@ -2573,100 +2526,100 @@
       <c r="H27" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="21" cm="1">
-        <f t="array" ref="I27">_xll.Beta(I2:I11,$L$2:$L$11)</f>
-        <v>1.5397349153075346</v>
-      </c>
-      <c r="J27" s="21" cm="1">
-        <f t="array" ref="J27">_xll.Beta(J2:J11,$L$2:$L$11)</f>
-        <v>1.1238963379400351</v>
-      </c>
-      <c r="K27" s="21" cm="1">
-        <f t="array" ref="K27">_xll.Beta(K2:K11,$L$2:$L$11)</f>
-        <v>1.3736080990295685</v>
-      </c>
-      <c r="L27" s="21" cm="1">
-        <f t="array" ref="L27">_xll.Beta(L2:L11,$L$2:$L$11)</f>
-        <v>1</v>
-      </c>
-      <c r="M27" s="21" cm="1">
-        <f t="array" ref="M27">_xll.Beta(M2:M11,$L$2:$L$11)</f>
-        <v>-1.0437227785546526E-2</v>
+      <c r="I27" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="I27" ca="1">_xll.Beta(I2:I11,$L$2:$L$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J27" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="J27" ca="1">_xll.Beta(J2:J11,$L$2:$L$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="K27" ca="1">_xll.Beta(K2:K11,$L$2:$L$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L27" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="L27" ca="1">_xll.Beta(L2:L11,$L$2:$L$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M27" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="M27" ca="1">_xll.Beta(M2:M11,$L$2:$L$11)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="21" cm="1">
-        <f t="array" ref="I28">_xll.SharpeRatio(I2:I11,$M$2:$M$11)</f>
-        <v>1.1661937725811693</v>
-      </c>
-      <c r="J28" s="21" cm="1">
-        <f t="array" ref="J28">_xll.SharpeRatio(J2:J11,$M$2:$M$11)</f>
-        <v>5.599865370514838E-2</v>
-      </c>
-      <c r="K28" s="21" cm="1">
-        <f t="array" ref="K28">_xll.SharpeRatio(K2:K11,$M$2:$M$11)</f>
-        <v>0.45962709975051652</v>
-      </c>
-      <c r="L28" s="21" cm="1">
-        <f t="array" ref="L28">_xll.SharpeRatio(L2:L11,$M$2:$M$11)</f>
-        <v>0.56182641192316762</v>
-      </c>
-      <c r="M28" s="21" cm="1">
-        <f t="array" ref="M28">_xll.SharpeRatio(M2:M11,$M$2:$M$11)</f>
-        <v>0</v>
+      <c r="I28" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="I28" ca="1">_xll.SharpeRatio(I2:I11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J28" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="J28" ca="1">_xll.SharpeRatio(J2:J11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="K28" ca="1">_xll.SharpeRatio(K2:K11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L28" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="L28" ca="1">_xll.SharpeRatio(L2:L11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M28" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="M28" ca="1">_xll.SharpeRatio(M2:M11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="21" cm="1">
-        <f t="array" ref="I29">_xll.TreynorIndex(I2:I11,I27,$M$2:$M$11)</f>
-        <v>0.16550865893152097</v>
-      </c>
-      <c r="J29" s="21" cm="1">
-        <f t="array" ref="J29">_xll.TreynorIndex(J2:J11,J27,$M$2:$M$11)</f>
-        <v>1.9257822880708833E-2</v>
-      </c>
-      <c r="K29" s="21" cm="1">
-        <f t="array" ref="K29">_xll.TreynorIndex(K2:K11,K27,$M$2:$M$11)</f>
-        <v>6.5476970730925316E-2</v>
-      </c>
-      <c r="L29" s="21" cm="1">
-        <f t="array" ref="L29">_xll.TreynorIndex(L2:L11,L27,$M$2:$M$11)</f>
-        <v>6.5437700595033191E-2</v>
-      </c>
-      <c r="M29" s="21" cm="1">
-        <f t="array" ref="M29">_xll.TreynorIndex(M2:M11,M27,$M$2:$M$11)</f>
-        <v>0</v>
+      <c r="I29" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="I29" ca="1">_xll.TreynorIndex(I2:I11,I27,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J29" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="J29" ca="1">_xll.TreynorIndex(J2:J11,J27,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="K29" ca="1">_xll.TreynorIndex(K2:K11,K27,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L29" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="L29" ca="1">_xll.TreynorIndex(L2:L11,L27,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M29" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="M29" ca="1">_xll.TreynorIndex(M2:M11,M27,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="21" cm="1">
-        <f t="array" ref="I30">_xll.JensensAlpha(I2:I11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>0.15408274855897586</v>
-      </c>
-      <c r="J30" s="21" cm="1">
-        <f t="array" ref="J30">_xll.JensensAlpha(J2:J11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>-5.190139544964778E-2</v>
-      </c>
-      <c r="K30" s="21" cm="1">
-        <f t="array" ref="K30">_xll.JensensAlpha(K2:K11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>5.394177671140532E-5</v>
-      </c>
-      <c r="L30" s="21" cm="1">
-        <f t="array" ref="L30">_xll.JensensAlpha(L2:L11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="21" cm="1">
-        <f t="array" ref="M30">_xll.JensensAlpha(M2:M11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>6.8298818687275483E-4</v>
+      <c r="I30" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="I30" ca="1">_xll.JensensAlpha(I2:I11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J30" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="J30" ca="1">_xll.JensensAlpha(J2:J11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="K30" ca="1">_xll.JensensAlpha(K2:K11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L30" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="L30" ca="1">_xll.JensensAlpha(L2:L11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M30" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="M30" ca="1">_xll.JensensAlpha(M2:M11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some new functions and updated documentation.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad9b1f9bd15b4598/C^N Source/PortfolioPerformance/PortfolioPerformance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="363" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{166DE418-A3C7-4846-B04B-202450FF248F}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="4275" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="5070" yWindow="5010" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 2.4" sheetId="4" r:id="rId3"/>
+    <sheet name="Table 2.5" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>RFR</t>
   </si>
@@ -197,13 +199,43 @@
   </si>
   <si>
     <t>Jensen's Alpha (Geometric)</t>
+  </si>
+  <si>
+    <t>Sample Skewness</t>
+  </si>
+  <si>
+    <t>Sample Kurtosis</t>
+  </si>
+  <si>
+    <t>Sample Excess Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>JB Test</t>
+  </si>
+  <si>
+    <t>Up Capture Raio</t>
+  </si>
+  <si>
+    <t>Down Capture Ratio</t>
+  </si>
+  <si>
+    <t>Up Percentage Ratio</t>
+  </si>
+  <si>
+    <t>Down Percentage Ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="12">
+  <numFmts count="13">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -216,6 +248,7 @@
     <numFmt numFmtId="172" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="173" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="174" formatCode="0.00000000000000%"/>
+    <numFmt numFmtId="175" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -260,7 +293,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -305,6 +338,8 @@
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -710,19 +745,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -802,6 +838,7 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
+      <c r="F3" s="8"/>
       <c r="G3" s="11">
         <f>C3-$B3</f>
         <v>-9.4000423002005284E-5</v>
@@ -851,6 +888,7 @@
       <c r="D4" s="1">
         <v>3.1331199999999892E-3</v>
       </c>
+      <c r="F4" s="8"/>
       <c r="G4" s="11">
         <f t="shared" ref="G4:H17" si="0">C4-$B4</f>
         <v>2.4011746255592215E-4</v>
@@ -894,6 +932,7 @@
       <c r="D5" s="1">
         <v>1.113068622437674E-2</v>
       </c>
+      <c r="F5" s="8"/>
       <c r="G5" s="11">
         <f t="shared" si="0"/>
         <v>7.1474745741937351E-3</v>
@@ -937,6 +976,7 @@
       <c r="D6" s="1">
         <v>-1.5737770653512229E-3</v>
       </c>
+      <c r="F6" s="8"/>
       <c r="G6" s="11">
         <f t="shared" si="0"/>
         <v>2.796920988140883E-3</v>
@@ -980,6 +1020,7 @@
       <c r="D7" s="1">
         <v>-1.2263622560784171E-3</v>
       </c>
+      <c r="F7" s="8"/>
       <c r="G7" s="11">
         <f t="shared" si="0"/>
         <v>-8.0655570066545668E-4</v>
@@ -1023,6 +1064,7 @@
       <c r="D8" s="1">
         <v>-6.0585660461631718E-5</v>
       </c>
+      <c r="F8" s="8"/>
       <c r="G8" s="11">
         <f t="shared" si="0"/>
         <v>-3.3821882023871153E-3</v>
@@ -1066,6 +1108,7 @@
       <c r="D9" s="1">
         <v>2.1230588697924713E-3</v>
       </c>
+      <c r="F9" s="8"/>
       <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>2.4995628940587267E-3</v>
@@ -1109,6 +1152,7 @@
       <c r="D10" s="1">
         <v>-1.2212168590912675E-3</v>
       </c>
+      <c r="F10" s="8"/>
       <c r="G10" s="11">
         <f t="shared" si="0"/>
         <v>2.6049629242241856E-4</v>
@@ -1143,6 +1187,7 @@
       <c r="D11" s="1">
         <v>5.190551166665891E-3</v>
       </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="11">
         <f t="shared" si="0"/>
         <v>-6.2243942139161845E-5</v>
@@ -1168,6 +1213,7 @@
       <c r="D12" s="1">
         <v>-1.1019876585149913E-2</v>
       </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="11">
         <f t="shared" si="0"/>
         <v>-4.9777787427041087E-3</v>
@@ -1201,6 +1247,7 @@
       <c r="D13" s="1">
         <v>2.7731910686723538E-4</v>
       </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="11">
         <f t="shared" si="0"/>
         <v>-3.4349984216608398E-4</v>
@@ -1226,6 +1273,7 @@
       <c r="D14" s="1">
         <v>-4.8789385894569826E-3</v>
       </c>
+      <c r="F14" s="8"/>
       <c r="G14" s="11">
         <f t="shared" si="0"/>
         <v>-8.4985796352023968E-3</v>
@@ -1251,6 +1299,7 @@
       <c r="D15" s="1">
         <v>7.5949356979387872E-3</v>
       </c>
+      <c r="F15" s="8"/>
       <c r="G15" s="11">
         <f t="shared" si="0"/>
         <v>6.0763667579284419E-3</v>
@@ -1276,6 +1325,7 @@
       <c r="D16" s="1">
         <v>-6.3539265847126769E-3</v>
       </c>
+      <c r="F16" s="8"/>
       <c r="G16" s="11">
         <f t="shared" si="0"/>
         <v>-2.5111083492623809E-3</v>
@@ -1301,6 +1351,7 @@
       <c r="D17" s="1">
         <v>2.6039764394154563E-3</v>
       </c>
+      <c r="F17" s="8"/>
       <c r="G17" s="11">
         <f t="shared" si="0"/>
         <v>-5.3985115541651529E-3</v>
@@ -1375,17 +1426,17 @@
         <f>_xlfn.COVARIANCE.S(D3:D17,$C$3:$C$17)/_xlfn.VAR.S($C$3:$C$17)</f>
         <v>0.94241159407120378</v>
       </c>
-      <c r="G21" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G21" ca="1">_xll.Beta(D3:D17,C3:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H21" s="10" t="e">
-        <f ca="1">D21-G21</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L21" t="e" cm="1">
-        <f t="array" aca="1" ref="L21" ca="1">_xll.Beta(L3:L17,K3:K17)</f>
-        <v>#VALUE!</v>
+      <c r="G21" s="9" cm="1">
+        <f t="array" ref="G21">_xll.Beta(D3:D17,C3:C17)</f>
+        <v>0.94241159407120412</v>
+      </c>
+      <c r="H21" s="10">
+        <f>D21-G21</f>
+        <v>0</v>
+      </c>
+      <c r="L21" cm="1">
+        <f t="array" ref="L21">_xll.Beta(L3:L17,K3:K17)</f>
+        <v>0.12710524781890767</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1400,13 +1451,13 @@
         <f>D21*2/3+1/3</f>
         <v>0.96160772938080252</v>
       </c>
-      <c r="G22" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G22" ca="1">_xll.AdjustedBeta(D3:D17,C3:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H22" s="10" t="e">
-        <f ca="1">D22-G22</f>
-        <v>#VALUE!</v>
+      <c r="G22" s="9" cm="1">
+        <f t="array" ref="G22">_xll.AdjustedBeta(D3:D17,C3:C17)</f>
+        <v>0.96160772938080274</v>
+      </c>
+      <c r="H22" s="10">
+        <f>D22-G22</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1421,17 +1472,17 @@
         <f t="array" ref="D23">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0))</f>
         <v>1.0869212641710992</v>
       </c>
-      <c r="G23" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G23" ca="1">_xll.BullBeta(D3:D17,C3:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H23" s="10" t="e">
-        <f t="shared" ref="H23:H32" ca="1" si="1">D23-G23</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L23" t="e" cm="1">
-        <f t="array" aca="1" ref="L23" ca="1">_xll.BullBeta(L3:L17,K3:K17)</f>
-        <v>#VALUE!</v>
+      <c r="G23" s="9" cm="1">
+        <f t="array" ref="G23">_xll.BullBeta(D3:D17,C3:C17)</f>
+        <v>1.0869212641710995</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" ref="H23:H36" si="1">D23-G23</f>
+        <v>0</v>
+      </c>
+      <c r="L23" cm="1">
+        <f t="array" ref="L23">_xll.BullBeta(L3:L17,K3:K17)</f>
+        <v>0.12710524781890767</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1446,16 +1497,16 @@
         <f t="array" ref="D24">SLOPE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0),_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0))</f>
         <v>0.54207326774062659</v>
       </c>
-      <c r="G24" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G24" ca="1">_xll.BearBeta(D3:D17,C3:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H24" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G24" s="9" cm="1">
+        <f t="array" ref="G24">_xll.BearBeta(D3:D17,C3:C17)</f>
+        <v>0.54207326774062647</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="L24" t="e" cm="1">
-        <f t="array" aca="1" ref="L24" ca="1">_xll.BearBeta(L3:L17,K3:K17,B3:B17)</f>
+        <f t="array" ref="L24">_xll.BearBeta(L3:L17,K3:K17,B3:B17)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1471,16 +1522,16 @@
         <f>D23/D24</f>
         <v>2.0051187336748981</v>
       </c>
-      <c r="G25" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G25" ca="1">_xll.BetaTimingRatio(D3:D17,C3:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H25" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G25" s="9" cm="1">
+        <f t="array" ref="G25">_xll.BetaTimingRatio(D3:D17,C3:C17)</f>
+        <v>2.005118733674899</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="L25" s="15" t="e" cm="1">
-        <f t="array" aca="1" ref="L25" ca="1">_xll.BetaTimingRatio(L3:L17,K3:K17)</f>
+        <f t="array" ref="L25">_xll.BetaTimingRatio(L3:L17,K3:K17)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1498,13 +1549,13 @@
         <v>5.1687248496316764E-2</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="G26" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G26" ca="1">_xll.SharpeRatio(D3:D17,B3:B17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H26" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G26" s="9" cm="1">
+        <f t="array" ref="G26">_xll.SharpeRatio(D3:D17,B3:B17)</f>
+        <v>5.1687248496316764E-2</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1521,13 +1572,13 @@
         <v>5.1676557020390534E-2</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="G27" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G27" ca="1">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H27" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G27" s="9" cm="1">
+        <f t="array" ref="G27">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
+        <v>5.1676557020390521E-2</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1543,13 +1594,13 @@
         <f>(AVERAGE(D3:D17)-AVERAGE($B$3:$B$17))/D21</f>
         <v>2.9990416146271975E-4</v>
       </c>
-      <c r="G28" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G28" ca="1">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H28" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G28" s="9" cm="1">
+        <f t="array" ref="G28">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
+        <v>2.9990416146271964E-4</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1564,13 +1615,13 @@
         <f>(_xlfn.STDEV.S($C$3:$C$17)/_xlfn.STDEV.S(D3:D17))*(D19-$B$19)+$B$19</f>
         <v>3.138111214532042E-4</v>
       </c>
-      <c r="G29" s="9" t="e" cm="1">
-        <f t="array" aca="1" ref="G29" ca="1">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H29" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G29" s="9" cm="1">
+        <f t="array" ref="G29">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
+        <v>3.1381112145320415E-4</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1585,13 +1636,13 @@
         <f>D19-$B$19-D21*($C$19-$B$19)</f>
         <v>7.2578822700353793E-4</v>
       </c>
-      <c r="G30" s="13" t="e" cm="1">
-        <f t="array" aca="1" ref="G30" ca="1">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H30" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G30" s="13" cm="1">
+        <f t="array" ref="G30">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
+        <v>7.2578822700353814E-4</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1606,13 +1657,13 @@
         <f t="array" ref="D31">_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
         <v>3.816440754566235E-3</v>
       </c>
-      <c r="G31" s="13" t="e" cm="1">
-        <f t="array" aca="1" ref="G31" ca="1">_xll.TrackingError(D3:D17,C3:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H31" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G31" s="13" cm="1">
+        <f t="array" ref="G31">_xll.TrackingError(D3:D17,C3:C17)</f>
+        <v>3.816440754566235E-3</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1624,87 +1675,224 @@
         <f t="array" ref="D32">(AVERAGE(D3:D17)-AVERAGE($C$3:$C$17))/_xlfn.STDEV.S(D3:D17-$C$3:$C$17)</f>
         <v>0.19726975178765843</v>
       </c>
-      <c r="G32" s="8" t="e" cm="1">
-        <f t="array" aca="1" ref="G32" ca="1">_xll.InformationRatio(D3:D17,C3:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H32" s="10" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="G33" s="10"/>
+      <c r="G32" s="8" cm="1">
+        <f t="array" ref="G32">_xll.InformationRatio(D3:D17,C3:C17)</f>
+        <v>0.19726975178765843</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="8" cm="1">
+        <f t="array" ref="C33">AVERAGE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&gt;0))/AVERAGE(_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0))</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" cm="1">
+        <f t="array" ref="D33">AVERAGE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&gt;0))/AVERAGE(_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0))</f>
+        <v>1.3503270666937031</v>
+      </c>
+      <c r="G33" s="10" cm="1">
+        <f t="array" ref="G33">_xll.UpCaptureRatio(D3:D17,$C$3:$C$17)</f>
+        <v>1.3503270666937031</v>
+      </c>
+      <c r="H33" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L33" s="11"/>
       <c r="M33" s="11"/>
     </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="8"/>
-      <c r="G34" s="16"/>
-      <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C35" s="8"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="G35" s="18" t="e" cm="1">
-        <f t="array" aca="1" ref="G35" ca="1">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="11"/>
-      <c r="L35" s="1"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="8" cm="1">
+        <f t="array" ref="C34">AVERAGE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&lt;0))/AVERAGE(_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0))</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="8" cm="1">
+        <f t="array" ref="D34">AVERAGE(_xlfn._xlws.FILTER(D3:D17,$C$3:$C$17&lt;0))/AVERAGE(_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0))</f>
+        <v>0.82277767682575553</v>
+      </c>
+      <c r="G34" s="10" cm="1">
+        <f t="array" ref="G34">_xll.DownCaptureRatio(D3:D17,C3:C17)</f>
+        <v>0.82277767682575553</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="6" cm="1">
+        <f t="array" ref="C35">SUM(--(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&gt;0)&gt;0))/COUNT(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&gt;0))</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="6" cm="1">
+        <f t="array" ref="D35">SUM(--(_xlfn._xlws.FILTER(D3:D17-$C$3:$C$17,$C$3:$C$17&gt;0)&gt;0))/COUNT(_xlfn._xlws.FILTER(D3:D17-$C$3:$C$17,$C$3:$C$17&gt;0))</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G35" s="6" cm="1">
+        <f t="array" ref="G35">_xll.UpPercentageRatio(D3:D17,C3:C17)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="11"/>
       <c r="M35" s="11"/>
     </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H36" s="1"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="19"/>
-    </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H38" s="1"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="20"/>
-    </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H40" s="1"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="6" cm="1">
+        <f t="array" ref="C36">SUM(--(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&lt;0)&gt;0))/COUNT(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&lt;0))</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="6" cm="1">
+        <f t="array" ref="D36">SUM(--(_xlfn._xlws.FILTER(D3:D17-$C$3:$C$17,$C$3:$C$17&lt;0)&gt;0))/COUNT(_xlfn._xlws.FILTER(D3:D17-$C$3:$C$17,$C$3:$C$17&lt;0))</f>
+        <v>0.625</v>
+      </c>
+      <c r="G36" s="6" cm="1">
+        <f t="array" ref="G36">_xll.DownPercentageRatio(D3:D17,C3:C17)</f>
+        <v>0.625</v>
+      </c>
+      <c r="H36" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="G37" s="10"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F38" s="32"/>
+      <c r="G38" s="16"/>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E39" s="11"/>
+      <c r="G39" s="18" t="str" cm="1">
+        <f t="array" ref="G39:H48">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
+        <v>Risk Premium</v>
+      </c>
+      <c r="H39" s="1">
+        <v>2.8263315887266938E-4</v>
+      </c>
+      <c r="I39" s="30"/>
+      <c r="J39" s="11"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="11"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
+        <v>Due to Risk</v>
+      </c>
+      <c r="H40" s="1">
+        <v>-4.4315506813086877E-4</v>
+      </c>
+      <c r="K40" s="11"/>
       <c r="L40" s="1"/>
-    </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H41" s="1"/>
-      <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H42" s="29"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="1"/>
-    </row>
-    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H45" s="28"/>
-    </row>
-    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H47" s="1"/>
+      <c r="M40" s="19"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G41" t="str">
+        <v>Due to Investor's Risk</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-6.1130570994079043E-4</v>
+      </c>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G42" t="str">
+        <v>Due to Manager's Risk</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1.6815064180992164E-4</v>
+      </c>
+      <c r="L42" s="2"/>
+      <c r="M42" s="20"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G43" t="str">
+        <v>Due to Selectivity</v>
+      </c>
+      <c r="H43" s="1">
+        <v>7.2578822700353814E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G44" t="str">
+        <v>Diversification</v>
+      </c>
+      <c r="H44" s="1">
+        <v>8.5146079155431776E-5</v>
+      </c>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G45" t="str">
+        <v>Net Selectivity</v>
+      </c>
+      <c r="H45" s="1">
+        <v>6.4064214784810634E-4</v>
+      </c>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G46" t="str">
+        <v>Hypothetical Beta</v>
+      </c>
+      <c r="H46" s="29">
+        <v>1.3134730578655345</v>
+      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G47" t="str">
+        <v>Hypothetical Exp Return</v>
+      </c>
+      <c r="H47" s="1">
+        <v>-5.1901011403769886E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G48" t="str">
+        <v>Hypothetical Risk Premium</v>
+      </c>
+      <c r="H48" s="1">
+        <v>-6.176412154819934E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49" s="28"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2526,104 +2714,564 @@
       <c r="H27" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="I27" ca="1">_xll.Beta(I2:I11,$L$2:$L$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J27" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="J27" ca="1">_xll.Beta(J2:J11,$L$2:$L$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K27" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="K27" ca="1">_xll.Beta(K2:K11,$L$2:$L$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L27" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="L27" ca="1">_xll.Beta(L2:L11,$L$2:$L$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M27" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="M27" ca="1">_xll.Beta(M2:M11,$L$2:$L$11)</f>
-        <v>#VALUE!</v>
+      <c r="I27" s="21" cm="1">
+        <f t="array" ref="I27">_xll.Beta(I2:I11,$L$2:$L$11)</f>
+        <v>1.5397349153075346</v>
+      </c>
+      <c r="J27" s="21" cm="1">
+        <f t="array" ref="J27">_xll.Beta(J2:J11,$L$2:$L$11)</f>
+        <v>1.1238963379400351</v>
+      </c>
+      <c r="K27" s="21" cm="1">
+        <f t="array" ref="K27">_xll.Beta(K2:K11,$L$2:$L$11)</f>
+        <v>1.3736080990295685</v>
+      </c>
+      <c r="L27" s="21" cm="1">
+        <f t="array" ref="L27">_xll.Beta(L2:L11,$L$2:$L$11)</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="21" cm="1">
+        <f t="array" ref="M27">_xll.Beta(M2:M11,$L$2:$L$11)</f>
+        <v>-1.0437227785546526E-2</v>
       </c>
     </row>
     <row r="28" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="I28" ca="1">_xll.SharpeRatio(I2:I11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J28" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="J28" ca="1">_xll.SharpeRatio(J2:J11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K28" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="K28" ca="1">_xll.SharpeRatio(K2:K11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L28" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="L28" ca="1">_xll.SharpeRatio(L2:L11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M28" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="M28" ca="1">_xll.SharpeRatio(M2:M11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
+      <c r="I28" s="21" cm="1">
+        <f t="array" ref="I28">_xll.SharpeRatio(I2:I11,$M$2:$M$11)</f>
+        <v>1.1661937725811693</v>
+      </c>
+      <c r="J28" s="21" cm="1">
+        <f t="array" ref="J28">_xll.SharpeRatio(J2:J11,$M$2:$M$11)</f>
+        <v>5.599865370514838E-2</v>
+      </c>
+      <c r="K28" s="21" cm="1">
+        <f t="array" ref="K28">_xll.SharpeRatio(K2:K11,$M$2:$M$11)</f>
+        <v>0.45962709975051652</v>
+      </c>
+      <c r="L28" s="21" cm="1">
+        <f t="array" ref="L28">_xll.SharpeRatio(L2:L11,$M$2:$M$11)</f>
+        <v>0.56182641192316762</v>
+      </c>
+      <c r="M28" s="21" cm="1">
+        <f t="array" ref="M28">_xll.SharpeRatio(M2:M11,$M$2:$M$11)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="I29" ca="1">_xll.TreynorIndex(I2:I11,I27,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J29" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="J29" ca="1">_xll.TreynorIndex(J2:J11,J27,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K29" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="K29" ca="1">_xll.TreynorIndex(K2:K11,K27,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L29" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="L29" ca="1">_xll.TreynorIndex(L2:L11,L27,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M29" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="M29" ca="1">_xll.TreynorIndex(M2:M11,M27,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
+      <c r="I29" s="21" cm="1">
+        <f t="array" ref="I29">_xll.TreynorIndex(I2:I11,I27,$M$2:$M$11)</f>
+        <v>0.16550865893152097</v>
+      </c>
+      <c r="J29" s="21" cm="1">
+        <f t="array" ref="J29">_xll.TreynorIndex(J2:J11,J27,$M$2:$M$11)</f>
+        <v>1.9257822880708833E-2</v>
+      </c>
+      <c r="K29" s="21" cm="1">
+        <f t="array" ref="K29">_xll.TreynorIndex(K2:K11,K27,$M$2:$M$11)</f>
+        <v>6.5476970730925316E-2</v>
+      </c>
+      <c r="L29" s="21" cm="1">
+        <f t="array" ref="L29">_xll.TreynorIndex(L2:L11,L27,$M$2:$M$11)</f>
+        <v>6.5437700595033191E-2</v>
+      </c>
+      <c r="M29" s="21" cm="1">
+        <f t="array" ref="M29">_xll.TreynorIndex(M2:M11,M27,$M$2:$M$11)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="I30" ca="1">_xll.JensensAlpha(I2:I11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J30" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="J30" ca="1">_xll.JensensAlpha(J2:J11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K30" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="K30" ca="1">_xll.JensensAlpha(K2:K11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L30" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="L30" ca="1">_xll.JensensAlpha(L2:L11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M30" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="M30" ca="1">_xll.JensensAlpha(M2:M11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>#VALUE!</v>
+      <c r="I30" s="21" cm="1">
+        <f t="array" ref="I30">_xll.JensensAlpha(I2:I11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>0.15408274855897586</v>
+      </c>
+      <c r="J30" s="21" cm="1">
+        <f t="array" ref="J30">_xll.JensensAlpha(J2:J11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>-5.190139544964778E-2</v>
+      </c>
+      <c r="K30" s="21" cm="1">
+        <f t="array" ref="K30">_xll.JensensAlpha(K2:K11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>5.394177671140532E-5</v>
+      </c>
+      <c r="L30" s="21" cm="1">
+        <f t="array" ref="L30">_xll.JensensAlpha(L2:L11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="21" cm="1">
+        <f t="array" ref="M30">_xll.JensensAlpha(M2:M11,$L$2:$L$11,$M$2:$M$11)</f>
+        <v>6.8298818687275483E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD11076-B722-4F8C-ADE7-A0B47C1E1E3C}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="33" cm="1">
+        <f t="array" ref="D1">_xll.Skewness_P(A1:A36)</f>
+        <v>-0.23799512754333596</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="33" cm="1">
+        <f t="array" ref="D2">_xll.Kurtosis_P_Excess(A1:A36)</f>
+        <v>-2.2361140899221699E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <f>COUNT(A1:A36)/6*(D1^2+D2^2/4)</f>
+        <v>0.34060011533968482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>-9.0000000000000011E-3</v>
+      </c>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4">_xll.JarqueBeraTest(A1:A36)</f>
+        <v>0.34060011533968482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" cm="1">
+        <f t="array" ref="D6">_xll.Skewness_S(A1:A36)</f>
+        <v>-0.24847026397682553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" cm="1">
+        <f t="array" ref="D7">_xll.Kurtosis_S(A1:A36)</f>
+        <v>3.4367578632223772</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>-1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>-3.7000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>5.7999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>-2E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>-6.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>-2E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2760DFB-DE92-4142-BDF1-40CAFDE42BC1}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" cm="1">
+        <f t="array" ref="D1">_xll.Skewness_S(A1:A36)</f>
+        <v>-0.37845974031750912</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" cm="1">
+        <f t="array" ref="D2">_xll.Kurtosis_S(A1:A36)</f>
+        <v>3.5141568846177993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" cm="1">
+        <f t="array" ref="D3">_xll.Kurtosis_S_Excess(A1:A36)</f>
+        <v>0.23875581509908272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>-1.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>-6.2E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>5.5999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>-2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>6.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>-2E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>1.3000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more functions and further updated documentation.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad9b1f9bd15b4598/C^N Source/PortfolioPerformance/PortfolioPerformance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="363" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{166DE418-A3C7-4846-B04B-202450FF248F}"/>
+  <xr:revisionPtr revIDLastSave="535" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B8250677-E36D-450B-9FAE-C073E5EA2A78}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5010" windowWidth="27480" windowHeight="15990" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="5070" yWindow="5010" windowWidth="27480" windowHeight="15990" activeTab="4" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Table 2.4" sheetId="4" r:id="rId3"/>
     <sheet name="Table 2.5" sheetId="3" r:id="rId4"/>
+    <sheet name="Table 2.7 &amp; 2.8" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>RFR</t>
   </si>
@@ -229,13 +230,40 @@
   </si>
   <si>
     <t>Down Percentage Ratio</t>
+  </si>
+  <si>
+    <t>Percentage Gain Ratio</t>
+  </si>
+  <si>
+    <t>Percentage Loss Ratio</t>
+  </si>
+  <si>
+    <t>Portfolio Return</t>
+  </si>
+  <si>
+    <t>Benchmark Return</t>
+  </si>
+  <si>
+    <t>Hurst Exponent</t>
+  </si>
+  <si>
+    <t>Max Cum Dev</t>
+  </si>
+  <si>
+    <t>Portfolio CD</t>
+  </si>
+  <si>
+    <t>Benchmark CD</t>
+  </si>
+  <si>
+    <t>Min Cum Dev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="13">
+  <numFmts count="14">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -249,6 +277,7 @@
     <numFmt numFmtId="173" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="174" formatCode="0.00000000000000%"/>
     <numFmt numFmtId="175" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -293,7 +322,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -340,6 +369,7 @@
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -745,17 +775,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
@@ -1477,7 +1507,7 @@
         <v>1.0869212641710995</v>
       </c>
       <c r="H23" s="10">
-        <f t="shared" ref="H23:H36" si="1">D23-G23</f>
+        <f t="shared" ref="H23:H38" si="1">D23-G23</f>
         <v>0</v>
       </c>
       <c r="L23" cm="1">
@@ -1777,122 +1807,176 @@
       <c r="M36" s="11"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="G37" s="10"/>
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="6" cm="1">
+        <f t="array" ref="C37">SUM(--(C3:C17&gt;0))/SUM(--($C$3:$C$17&gt;0))</f>
+        <v>1</v>
+      </c>
+      <c r="D37" s="6" cm="1">
+        <f t="array" ref="D37">SUM(--(D3:D17&gt;0))/SUM(--($C$3:$C$17&gt;0))</f>
+        <v>1</v>
+      </c>
+      <c r="G37" s="6" cm="1">
+        <f t="array" ref="G37">_xll.PercentageGainRatio(D3:D17,C3:C17)</f>
+        <v>1</v>
+      </c>
+      <c r="H37" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F38" s="32"/>
-      <c r="G38" s="16"/>
-      <c r="L38" s="1"/>
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="6" cm="1">
+        <f t="array" ref="C38">SUM(--(C3:C17&lt;0))/SUM(--($C$3:$C$17&lt;0))</f>
+        <v>1</v>
+      </c>
+      <c r="D38" s="6" cm="1">
+        <f t="array" ref="D38">SUM(--(D3:D17&lt;0))/SUM(--($C$3:$C$17&lt;0))</f>
+        <v>0.875</v>
+      </c>
+      <c r="G38" s="6" cm="1">
+        <f t="array" ref="G38">_xll.PercentageLossRatio(D3:D17,C3:C17)</f>
+        <v>0.875</v>
+      </c>
+      <c r="H38" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E39" s="11"/>
-      <c r="G39" s="18" t="str" cm="1">
-        <f t="array" ref="G39:H48">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="10"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="G40" s="10"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F41" s="32"/>
+      <c r="G41" s="16"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E42" s="11"/>
+      <c r="G42" s="18" t="str" cm="1">
+        <f t="array" ref="G42:H51">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
         <v>Risk Premium</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H42" s="1">
         <v>2.8263315887266938E-4</v>
       </c>
-      <c r="I39" s="30"/>
-      <c r="J39" s="11"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="11"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G40" t="str">
-        <v>Due to Risk</v>
-      </c>
-      <c r="H40" s="1">
-        <v>-4.4315506813086877E-4</v>
-      </c>
-      <c r="K40" s="11"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="19"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G41" t="str">
-        <v>Due to Investor's Risk</v>
-      </c>
-      <c r="H41" s="1">
-        <v>-6.1130570994079043E-4</v>
-      </c>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G42" t="str">
-        <v>Due to Manager's Risk</v>
-      </c>
-      <c r="H42" s="1">
-        <v>1.6815064180992164E-4</v>
-      </c>
-      <c r="L42" s="2"/>
-      <c r="M42" s="20"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="11"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="11"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G43" t="str">
-        <v>Due to Selectivity</v>
+        <v>Due to Risk</v>
       </c>
       <c r="H43" s="1">
-        <v>7.2578822700353814E-4</v>
-      </c>
+        <v>-4.4315506813086877E-4</v>
+      </c>
+      <c r="K43" s="11"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="19"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G44" t="str">
-        <v>Diversification</v>
+        <v>Due to Investor's Risk</v>
       </c>
       <c r="H44" s="1">
-        <v>8.5146079155431776E-5</v>
-      </c>
-      <c r="L44" s="1"/>
+        <v>-6.1130570994079043E-4</v>
+      </c>
+      <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G45" t="str">
-        <v>Net Selectivity</v>
+        <v>Due to Manager's Risk</v>
       </c>
       <c r="H45" s="1">
-        <v>6.4064214784810634E-4</v>
-      </c>
-      <c r="L45" s="1"/>
+        <v>1.6815064180992164E-4</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="M45" s="20"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G46" t="str">
-        <v>Hypothetical Beta</v>
-      </c>
-      <c r="H46" s="29">
-        <v>1.3134730578655345</v>
-      </c>
-      <c r="J46" s="8"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="1"/>
+        <v>Due to Selectivity</v>
+      </c>
+      <c r="H46" s="1">
+        <v>7.2578822700353814E-4</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G47" t="str">
-        <v>Hypothetical Exp Return</v>
+        <v>Diversification</v>
       </c>
       <c r="H47" s="1">
-        <v>-5.1901011403769886E-4</v>
-      </c>
+        <v>8.5146079155431776E-5</v>
+      </c>
+      <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G48" t="str">
+        <v>Net Selectivity</v>
+      </c>
+      <c r="H48" s="1">
+        <v>6.4064214784810634E-4</v>
+      </c>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G49" t="str">
+        <v>Hypothetical Beta</v>
+      </c>
+      <c r="H49" s="29">
+        <v>1.3134730578655345</v>
+      </c>
+      <c r="J49" s="8"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G50" t="str">
+        <v>Hypothetical Exp Return</v>
+      </c>
+      <c r="H50" s="1">
+        <v>-5.1901011403769886E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G51" t="str">
         <v>Hypothetical Risk Premium</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H51" s="1">
         <v>-6.176412154819934E-4</v>
       </c>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H49" s="28"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H51" s="1"/>
+    <row r="52" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H52" s="28"/>
+    </row>
+    <row r="53" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3274,4 +3358,725 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4799EC79-C9E3-4E9F-9D8B-C1C9DE78CC72}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B2" s="34">
+        <v>2E-3</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="14">
+        <f>A2-H$2</f>
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="E2" s="14">
+        <f>B2-I$2</f>
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="26">
+        <f>AVERAGE(A2:A37)</f>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="I2" s="26">
+        <f>AVERAGE(B2:B37)</f>
+        <v>1.2000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="B3" s="34">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="14">
+        <f>D2+A3-H$2</f>
+        <v>7.000000000000001E-3</v>
+      </c>
+      <c r="E3" s="14">
+        <f>E2+B3-I$2</f>
+        <v>2.9999999999999975E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="14">
+        <f>_xlfn.STDEV.P(A2:A37)</f>
+        <v>3.3173784830796742E-2</v>
+      </c>
+      <c r="I3" s="14">
+        <f>_xlfn.STDEV.P(B2:B37)</f>
+        <v>3.3620430296671298E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B4" s="34">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="14">
+        <f t="shared" ref="D4:D37" si="0">D3+A4-H$2</f>
+        <v>7.000000000000001E-3</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" ref="E4:E37" si="1">E3+B4-I$2</f>
+        <v>8.9999999999999959E-3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="26">
+        <f>MAX(D2:D37)</f>
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="I4" s="26">
+        <f>MAX(E2:E37)</f>
+        <v>0.13999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
+        <v>-9.0000000000000011E-3</v>
+      </c>
+      <c r="B5" s="34">
+        <v>-1.1000000000000001E-2</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.3000000000000001E-2</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" si="1"/>
+        <v>-1.4000000000000007E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="26">
+        <f>MIN(D2:D37)</f>
+        <v>-9.200000000000004E-2</v>
+      </c>
+      <c r="I5" s="26">
+        <f>MIN(E2:E37)</f>
+        <v>-0.1240000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B6" s="34">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000004E-2</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
+        <v>-1.2000000000000011E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="21">
+        <f>LOG10((H4-H5)/H3)/LOG10(COUNT(A2:A37))</f>
+        <v>0.55221669170563814</v>
+      </c>
+      <c r="I6" s="21">
+        <f>LOG10((I4-I5)/I3)/LOG10(COUNT(B2:B37))</f>
+        <v>0.57508142465835954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B7" s="34">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="14">
+        <f t="shared" si="0"/>
+        <v>2.9999999999999957E-3</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="1"/>
+        <v>-1.000000000000013E-3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="21" cm="1">
+        <f t="array" ref="H7">_xll.HurstExponent(A2:A37)</f>
+        <v>0.55221669170563814</v>
+      </c>
+      <c r="I7" s="21" cm="1">
+        <f t="array" ref="I7">_xll.HurstExponent(B2:B37)</f>
+        <v>0.57508142465835954</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B8" s="34">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="14">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999941E-3</v>
+      </c>
+      <c r="E8" s="14">
+        <f t="shared" si="1"/>
+        <v>9.9999999999998354E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B9" s="34">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="14">
+        <f t="shared" si="0"/>
+        <v>6.1999999999999993E-2</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" si="1"/>
+        <v>5.3999999999999986E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>-1.3999999999999999E-2</v>
+      </c>
+      <c r="B10" s="34">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="14">
+        <f t="shared" si="0"/>
+        <v>3.6999999999999991E-2</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="1"/>
+        <v>2.6999999999999982E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B11" s="34">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="14">
+        <f t="shared" si="0"/>
+        <v>6.4999999999999988E-2</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" si="1"/>
+        <v>5.6999999999999974E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="B12" s="34">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="14">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999988E-2</v>
+      </c>
+      <c r="E12" s="14">
+        <f t="shared" si="1"/>
+        <v>4.1999999999999968E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="B13" s="34">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="14">
+        <f t="shared" si="0"/>
+        <v>0.11900000000000001</v>
+      </c>
+      <c r="E13" s="14">
+        <f t="shared" si="1"/>
+        <v>0.11299999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>0.04</v>
+      </c>
+      <c r="B14" s="34">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="14">
+        <f t="shared" si="0"/>
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="E14" s="14">
+        <f t="shared" si="1"/>
+        <v>0.13999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="B15" s="34">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="1"/>
+        <v>8.9999999999999955E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="34">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="B16" s="34">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="14">
+        <f t="shared" si="0"/>
+        <v>2.799999999999999E-2</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" si="1"/>
+        <v>1.5999999999999952E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="34">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B17" s="34">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="14">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999986E-2</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="1"/>
+        <v>1.8999999999999947E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="34">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="B18" s="34">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.9000000000000019E-2</v>
+      </c>
+      <c r="E18" s="14">
+        <f t="shared" si="1"/>
+        <v>-4.1000000000000057E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="34">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B19" s="34">
+        <v>-0.02</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="14">
+        <f t="shared" si="0"/>
+        <v>-6.1000000000000019E-2</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="1"/>
+        <v>-7.3000000000000051E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="34">
+        <v>6.2E-2</v>
+      </c>
+      <c r="B20" s="34">
+        <v>0.06</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="14">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000021E-2</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="1"/>
+        <v>-2.5000000000000057E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="34">
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="B21" s="34">
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="14">
+        <f t="shared" si="0"/>
+        <v>3.699999999999997E-2</v>
+      </c>
+      <c r="E21" s="14">
+        <f t="shared" si="1"/>
+        <v>1.8999999999999934E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="34">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="B22" s="34">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="14">
+        <f t="shared" si="0"/>
+        <v>-3.8000000000000034E-2</v>
+      </c>
+      <c r="E22" s="14">
+        <f t="shared" si="1"/>
+        <v>-6.0000000000000074E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B23" s="34">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="14">
+        <f t="shared" si="0"/>
+        <v>-3.2000000000000035E-2</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" si="1"/>
+        <v>-5.3000000000000082E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="34">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="B24" s="34">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="14">
+        <f t="shared" si="0"/>
+        <v>-4.7000000000000035E-2</v>
+      </c>
+      <c r="E24" s="14">
+        <f t="shared" si="1"/>
+        <v>-6.8000000000000088E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="34">
+        <v>-2E-3</v>
+      </c>
+      <c r="B25" s="34">
+        <v>-1E-3</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="14">
+        <f t="shared" si="0"/>
+        <v>-6.0000000000000039E-2</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="shared" si="1"/>
+        <v>-8.1000000000000086E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="34">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B26" s="34">
+        <v>-2.6000000000000002E-2</v>
+      </c>
+      <c r="C26" s="34"/>
+      <c r="D26" s="14">
+        <f t="shared" si="0"/>
+        <v>-9.200000000000004E-2</v>
+      </c>
+      <c r="E26" s="14">
+        <f t="shared" si="1"/>
+        <v>-0.11900000000000009</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="34">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B27" s="34">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="C27" s="34"/>
+      <c r="D27" s="14">
+        <f t="shared" si="0"/>
+        <v>-9.200000000000004E-2</v>
+      </c>
+      <c r="E27" s="14">
+        <f t="shared" si="1"/>
+        <v>-0.1240000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="34">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B28" s="34">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="14">
+        <f t="shared" si="0"/>
+        <v>-5.6000000000000043E-2</v>
+      </c>
+      <c r="E28" s="14">
+        <f t="shared" si="1"/>
+        <v>-9.3000000000000096E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="34">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B29" s="34">
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="14">
+        <f t="shared" si="0"/>
+        <v>-4.3000000000000045E-2</v>
+      </c>
+      <c r="E29" s="14">
+        <f t="shared" si="1"/>
+        <v>-7.6000000000000095E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="34">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="B30" s="34">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C30" s="34"/>
+      <c r="D30" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.1000000000000046E-2</v>
+      </c>
+      <c r="E30" s="14">
+        <f t="shared" si="1"/>
+        <v>-5.00000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="34">
+        <v>-6.9999999999999993E-3</v>
+      </c>
+      <c r="B31" s="34">
+        <v>-2E-3</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="14">
+        <f t="shared" si="0"/>
+        <v>-3.9000000000000049E-2</v>
+      </c>
+      <c r="E31" s="14">
+        <f t="shared" si="1"/>
+        <v>-6.4000000000000098E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="34">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B32" s="34">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="14">
+        <f t="shared" si="0"/>
+        <v>-3.0000000000000495E-3</v>
+      </c>
+      <c r="E32" s="14">
+        <f t="shared" si="1"/>
+        <v>-2.5000000000000105E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="34">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B33" s="34">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="14">
+        <f t="shared" si="0"/>
+        <v>-8.0000000000000505E-3</v>
+      </c>
+      <c r="E33" s="14">
+        <f t="shared" si="1"/>
+        <v>-2.3000000000000111E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="34">
+        <v>0.01</v>
+      </c>
+      <c r="B34" s="34">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="C34" s="34"/>
+      <c r="D34" s="14">
+        <f t="shared" si="0"/>
+        <v>-9.0000000000000514E-3</v>
+      </c>
+      <c r="E34" s="14">
+        <f t="shared" si="1"/>
+        <v>-2.200000000000011E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="34">
+        <v>-2E-3</v>
+      </c>
+      <c r="B35" s="34">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="14">
+        <f t="shared" si="0"/>
+        <v>-2.2000000000000054E-2</v>
+      </c>
+      <c r="E35" s="14">
+        <f t="shared" si="1"/>
+        <v>-3.1000000000000111E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="34">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B36" s="34">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999994711E-4</v>
+      </c>
+      <c r="E36" s="14">
+        <f t="shared" si="1"/>
+        <v>-9.0000000000001103E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="34">
+        <v>0.01</v>
+      </c>
+      <c r="B37" s="34">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="14">
+        <f t="shared" si="0"/>
+        <v>-5.377642775528102E-17</v>
+      </c>
+      <c r="E37" s="14">
+        <f t="shared" si="1"/>
+        <v>-1.1102230246251565E-16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the Bias Ratio and updated documentation.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad9b1f9bd15b4598/C^N Source/PortfolioPerformance/PortfolioPerformance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="535" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B8250677-E36D-450B-9FAE-C073E5EA2A78}"/>
+  <xr:revisionPtr revIDLastSave="635" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7702B17-6949-41AB-8351-68FD864A48A5}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5010" windowWidth="27480" windowHeight="15990" activeTab="4" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="4725" yWindow="3255" windowWidth="27480" windowHeight="15990" activeTab="3" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table 2.4" sheetId="4" r:id="rId3"/>
-    <sheet name="Table 2.5" sheetId="3" r:id="rId4"/>
-    <sheet name="Table 2.7 &amp; 2.8" sheetId="5" r:id="rId5"/>
+    <sheet name="Table 2.4 and 2.5" sheetId="4" r:id="rId3"/>
+    <sheet name="Tables 2.7, 2.8, and 2.9" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>RFR</t>
   </si>
@@ -208,15 +207,6 @@
     <t>Sample Kurtosis</t>
   </si>
   <si>
-    <t>Sample Excess Kurtosis</t>
-  </si>
-  <si>
-    <t>Skewness</t>
-  </si>
-  <si>
-    <t>Kurtosis</t>
-  </si>
-  <si>
     <t>JB Test</t>
   </si>
   <si>
@@ -257,6 +247,30 @@
   </si>
   <si>
     <t>Min Cum Dev</t>
+  </si>
+  <si>
+    <t>Bias Ratio</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Number of Std Devs</t>
+  </si>
+  <si>
+    <t>Count Above</t>
+  </si>
+  <si>
+    <t>Count Below</t>
+  </si>
+  <si>
+    <t>Population Skewness</t>
+  </si>
+  <si>
+    <t>Population Kurtosis</t>
   </si>
 </sst>
 </file>
@@ -276,8 +290,8 @@
     <numFmt numFmtId="172" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="173" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="174" formatCode="0.00000000000000%"/>
-    <numFmt numFmtId="175" formatCode="0.0000"/>
     <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -322,7 +336,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -368,8 +382,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1716,7 +1731,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C33" s="8" cm="1">
         <f t="array" ref="C33">AVERAGE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&gt;0))/AVERAGE(_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&gt;0))</f>
@@ -1739,7 +1754,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" s="8" cm="1">
         <f t="array" ref="C34">AVERAGE(_xlfn._xlws.FILTER(C3:C17,$C$3:$C$17&lt;0))/AVERAGE(_xlfn._xlws.FILTER($C$3:$C$17,$C$3:$C$17&lt;0))</f>
@@ -1762,7 +1777,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C35" s="6" cm="1">
         <f t="array" ref="C35">SUM(--(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&gt;0)&gt;0))/COUNT(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&gt;0))</f>
@@ -1785,7 +1800,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C36" s="6" cm="1">
         <f t="array" ref="C36">SUM(--(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&lt;0)&gt;0))/COUNT(_xlfn._xlws.FILTER(C3:C17-$C$3:$C$17,$C$3:$C$17&lt;0))</f>
@@ -1808,7 +1823,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C37" s="6" cm="1">
         <f t="array" ref="C37">SUM(--(C3:C17&gt;0))/SUM(--($C$3:$C$17&gt;0))</f>
@@ -1831,7 +1846,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C38" s="6" cm="1">
         <f t="array" ref="C38">SUM(--(C3:C17&lt;0))/SUM(--($C$3:$C$17&lt;0))</f>
@@ -2902,234 +2917,399 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD11076-B722-4F8C-ADE7-A0B47C1E1E3C}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="33" cm="1">
-        <f t="array" ref="D1">_xll.Skewness_P(A1:A36)</f>
+      <c r="B2" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="21">
+        <f>_xlfn.SKEW.P(A2:A37)</f>
+        <v>-0.23799512754333593</v>
+      </c>
+      <c r="F2" s="21">
+        <f>_xlfn.SKEW.P(B2:B37)</f>
+        <v>-0.36250444107583124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="21" cm="1">
+        <f t="array" ref="E3">_xll.Skewness_P(A2:A37)</f>
         <v>-0.23799512754333596</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
-        <v>2.6000000000000002E-2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="33" cm="1">
-        <f t="array" ref="D2">_xll.Kurtosis_P_Excess(A1:A36)</f>
+      <c r="F3" s="21" cm="1">
+        <f t="array" ref="F3">_xll.Skewness_P(B2:B37)</f>
+        <v>-0.3625044410758313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1.8000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>-9.0000000000000011E-3</v>
+      </c>
+      <c r="B5" s="14">
+        <v>-1.1000000000000001E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="21" cm="1">
+        <f t="array" ref="E5">_xll.Kurtosis_P_Excess(A2:A37)</f>
         <v>-2.2361140899221699E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="F5" s="21" cm="1">
+        <f t="array" ref="F5">_xll.Kurtosis_P_Excess(B2:B37)</f>
+        <v>4.4698088448780204E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="21">
+        <f>COUNT(A2:A37)/6*(E3^2+E5^2/4)</f>
+        <v>0.34060011533968482</v>
+      </c>
+      <c r="F7" s="21">
+        <f>COUNT(B2:B37)/6*(F3^2+F5^2/4)</f>
+        <v>0.79145369746466754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="21" cm="1">
+        <f t="array" ref="E8">_xll.JarqueBeraTest(A2:A37)</f>
+        <v>0.34060011533968482</v>
+      </c>
+      <c r="F8" s="21" cm="1">
+        <f t="array" ref="F8">_xll.JarqueBeraTest(B2:B37)</f>
+        <v>0.79145369746466754</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B9" s="14">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>-1.3999999999999999E-2</v>
+      </c>
+      <c r="B10" s="14">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="21" cm="1">
+        <f t="array" ref="E10">_xll.Skewness_S(A2:A37)</f>
+        <v>-0.24847026397682553</v>
+      </c>
+      <c r="F10" s="21" cm="1">
+        <f t="array" ref="F10">_xll.Skewness_S(B2:B37)</f>
+        <v>-0.37845974031750912</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B11" s="14">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="21" cm="1">
+        <f t="array" ref="E11">_xll.Kurtosis_S(A2:A37)</f>
+        <v>3.4367578632223772</v>
+      </c>
+      <c r="F11" s="21" cm="1">
+        <f t="array" ref="F11">_xll.Kurtosis_S(B2:B37)</f>
+        <v>3.5141568846177993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="B12" s="14">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="B13" s="14">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="B14" s="14">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="B15" s="14">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="B16" s="14">
+        <v>-6.2E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B17" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="B18" s="14">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B19" s="14">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>6.2E-2</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="B21" s="14">
+        <v>5.5999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="B22" s="14">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B23" s="14">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="B24" s="14">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>-2E-3</v>
+      </c>
+      <c r="B25" s="14">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B26" s="14">
+        <v>-2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
         <v>1.1000000000000001E-2</v>
       </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3">
-        <f>COUNT(A1:A36)/6*(D1^2+D2^2/4)</f>
-        <v>0.34060011533968482</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <v>-9.0000000000000011E-3</v>
-      </c>
-      <c r="D4" cm="1">
-        <f t="array" ref="D4">_xll.JarqueBeraTest(A1:A36)</f>
-        <v>0.34060011533968482</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="B27" s="14">
+        <v>6.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B28" s="14">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B29" s="14">
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="B30" s="14">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>-6.9999999999999993E-3</v>
+      </c>
+      <c r="B31" s="14">
+        <v>-2E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B32" s="14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B33" s="14">
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>2.4E-2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" cm="1">
-        <f t="array" ref="D6">_xll.Skewness_S(A1:A36)</f>
-        <v>-0.24847026397682553</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" cm="1">
-        <f t="array" ref="D7">_xll.Kurtosis_S(A1:A36)</f>
-        <v>3.4367578632223772</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>-1.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>3.9E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <v>8.1000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>-3.7000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>-6.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>1.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <v>-4.9000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>-2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>6.2E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>5.7999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>-6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>-4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="B34" s="14">
+        <v>1.3000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
         <v>-2E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <v>-2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
-        <v>1.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <v>4.7E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
-        <v>-6.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
-        <v>4.7E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+      <c r="B35" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B36" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <v>-2E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
-        <v>0.01</v>
+      <c r="B37" s="14">
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3138,234 +3318,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2760DFB-DE92-4142-BDF1-40CAFDE42BC1}">
-  <dimension ref="A1:D36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14">
-        <v>2E-3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" cm="1">
-        <f t="array" ref="D1">_xll.Skewness_S(A1:A36)</f>
-        <v>-0.37845974031750912</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" cm="1">
-        <f t="array" ref="D2">_xll.Kurtosis_S(A1:A36)</f>
-        <v>3.5141568846177993</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>1.8000000000000002E-2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" cm="1">
-        <f t="array" ref="D3">_xll.Kurtosis_S_Excess(A1:A36)</f>
-        <v>0.23875581509908272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <v>-1.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
-        <v>1.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>1.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>6.5000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>-1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>-3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <v>8.3000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>3.9E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>-3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>-6.2E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <v>-4.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>5.5999999999999994E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>-6.7000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>-3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>-1E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <v>-2.6000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
-        <v>6.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <v>4.2999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <v>2.8999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
-        <v>-2E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
-        <v>5.0999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
-        <v>1.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
-        <v>1.3000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4799EC79-C9E3-4E9F-9D8B-C1C9DE78CC72}">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3373,39 +3330,38 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
       <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="34">
+      <c r="A2" s="33">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="33">
         <v>2E-3</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="14">
         <f>A2-H$2</f>
         <v>-8.0000000000000002E-3</v>
@@ -3427,13 +3383,13 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="34">
+      <c r="A3" s="33">
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="33">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="14">
         <f>D2+A3-H$2</f>
         <v>7.000000000000001E-3</v>
@@ -3455,13 +3411,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
+      <c r="A4" s="33">
         <v>1.1000000000000001E-2</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="33">
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D37" si="0">D3+A4-H$2</f>
         <v>7.000000000000001E-3</v>
@@ -3471,7 +3427,7 @@
         <v>8.9999999999999959E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H4" s="26">
         <f>MAX(D2:D37)</f>
@@ -3483,13 +3439,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="34">
+      <c r="A5" s="33">
         <v>-9.0000000000000011E-3</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="33">
         <v>-1.1000000000000001E-2</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="14">
         <f t="shared" si="0"/>
         <v>-1.3000000000000001E-2</v>
@@ -3499,7 +3455,7 @@
         <v>-1.4000000000000007E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H5" s="26">
         <f>MIN(D2:D37)</f>
@@ -3511,13 +3467,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="33">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="33">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
         <v>-1.0000000000000004E-2</v>
@@ -3527,7 +3483,7 @@
         <v>-1.2000000000000011E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H6" s="21">
         <f>LOG10((H4-H5)/H3)/LOG10(COUNT(A2:A37))</f>
@@ -3539,13 +3495,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="34">
+      <c r="A7" s="33">
         <v>2.4E-2</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="33">
         <v>2.3E-2</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
         <v>2.9999999999999957E-3</v>
@@ -3555,7 +3511,7 @@
         <v>-1.000000000000013E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H7" s="21" cm="1">
         <f t="array" ref="H7">_xll.HurstExponent(A2:A37)</f>
@@ -3567,13 +3523,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+      <c r="A8" s="33">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="33">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
         <v>6.9999999999999941E-3</v>
@@ -3584,13 +3540,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
+      <c r="A9" s="33">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="33">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="14">
         <f t="shared" si="0"/>
         <v>6.1999999999999993E-2</v>
@@ -3599,15 +3555,21 @@
         <f t="shared" si="1"/>
         <v>5.3999999999999986E-2</v>
       </c>
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
+      <c r="A10" s="33">
         <v>-1.3999999999999999E-2</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="33">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="14">
         <f t="shared" si="0"/>
         <v>3.6999999999999991E-2</v>
@@ -3616,15 +3578,25 @@
         <f t="shared" si="1"/>
         <v>2.6999999999999982E-2</v>
       </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="35">
+        <v>1</v>
+      </c>
+      <c r="I10" s="35">
+        <f>H10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
+      <c r="A11" s="33">
         <v>3.9E-2</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="33">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="14">
         <f t="shared" si="0"/>
         <v>6.4999999999999988E-2</v>
@@ -3633,15 +3605,26 @@
         <f t="shared" si="1"/>
         <v>5.6999999999999974E-2</v>
       </c>
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="34" cm="1">
+        <f t="array" ref="H11">SUM((A2:A37&gt;=0)*(A2:A37&lt;=H3))</f>
+        <v>14</v>
+      </c>
+      <c r="I11" s="34" cm="1">
+        <f t="array" ref="I11">SUM((B2:B37&gt;=0)*(B2:B37&lt;=I3))</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="34">
+      <c r="A12" s="33">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="33">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="14">
         <f t="shared" si="0"/>
         <v>4.8999999999999988E-2</v>
@@ -3650,15 +3633,26 @@
         <f t="shared" si="1"/>
         <v>4.1999999999999968E-2</v>
       </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="34" cm="1">
+        <f t="array" ref="H12">SUM((A2:A37&lt;0)*(A2:A37&gt;=-H3))</f>
+        <v>9</v>
+      </c>
+      <c r="I12" s="34" cm="1">
+        <f t="array" ref="I12">SUM((B2:B37&lt;0)*(B2:B37&gt;=-I3))</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="34">
+      <c r="A13" s="33">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="33">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="14">
         <f t="shared" si="0"/>
         <v>0.11900000000000001</v>
@@ -3667,15 +3661,26 @@
         <f t="shared" si="1"/>
         <v>0.11299999999999998</v>
       </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="28" cm="1">
+        <f t="array" ref="H13">SUM((A2:A37&gt;=0)*(A2:A37&lt;=H3*H10))/(1+SUM((A2:A37&lt;0)*(A2:A37&gt;=-H3*H10)))</f>
+        <v>1.4</v>
+      </c>
+      <c r="I13" s="28" cm="1">
+        <f t="array" ref="I13">SUM((B2:B37&gt;=0)*(B2:B37&lt;=I3*I10))/(1+SUM((B2:B37&lt;0)*(B2:B37&gt;=-I3*I10)))</f>
+        <v>1.5555555555555556</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+      <c r="A14" s="33">
         <v>0.04</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="33">
         <v>3.9E-2</v>
       </c>
-      <c r="C14" s="34"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="14">
         <f t="shared" si="0"/>
         <v>0.14799999999999999</v>
@@ -3684,15 +3689,26 @@
         <f t="shared" si="1"/>
         <v>0.13999999999999996</v>
       </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="28" cm="1">
+        <f t="array" ref="H14">_xll.BiasRatio(A2:A37,H10)</f>
+        <v>1.4</v>
+      </c>
+      <c r="I14" s="28" cm="1">
+        <f t="array" ref="I14">_xll.BiasRatio(B2:B37,I10)</f>
+        <v>1.5555555555555556</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
+      <c r="A15" s="33">
         <v>-3.7000000000000005E-2</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="33">
         <v>-3.7999999999999999E-2</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="14">
         <f t="shared" si="0"/>
         <v>9.9999999999999992E-2</v>
@@ -3703,13 +3719,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="34">
+      <c r="A16" s="33">
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="33">
         <v>-6.2E-2</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="14">
         <f t="shared" si="0"/>
         <v>2.799999999999999E-2</v>
@@ -3720,13 +3736,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="34">
+      <c r="A17" s="33">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="33">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="14">
         <f t="shared" si="0"/>
         <v>3.0999999999999986E-2</v>
@@ -3737,13 +3753,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
+      <c r="A18" s="33">
         <v>-4.9000000000000002E-2</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="33">
         <v>-4.8000000000000001E-2</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="14">
         <f t="shared" si="0"/>
         <v>-2.9000000000000019E-2</v>
@@ -3754,13 +3770,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="34">
+      <c r="A19" s="33">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="33">
         <v>-0.02</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="14">
         <f t="shared" si="0"/>
         <v>-6.1000000000000019E-2</v>
@@ -3771,13 +3787,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="34">
+      <c r="A20" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="33">
         <v>0.06</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="14">
         <f t="shared" si="0"/>
         <v>-1.0000000000000021E-2</v>
@@ -3788,13 +3804,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="34">
+      <c r="A21" s="33">
         <v>5.7999999999999996E-2</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="33">
         <v>5.5999999999999994E-2</v>
       </c>
-      <c r="C21" s="34"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="14">
         <f t="shared" si="0"/>
         <v>3.699999999999997E-2</v>
@@ -3805,13 +3821,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="34">
+      <c r="A22" s="33">
         <v>-6.4000000000000001E-2</v>
       </c>
-      <c r="B22" s="34">
+      <c r="B22" s="33">
         <v>-6.7000000000000004E-2</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="14">
         <f t="shared" si="0"/>
         <v>-3.8000000000000034E-2</v>
@@ -3822,13 +3838,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="34">
+      <c r="A23" s="33">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="33">
         <v>1.9E-2</v>
       </c>
-      <c r="C23" s="34"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="14">
         <f t="shared" si="0"/>
         <v>-3.2000000000000035E-2</v>
@@ -3839,13 +3855,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="34">
+      <c r="A24" s="33">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B24" s="33">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="C24" s="34"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="14">
         <f t="shared" si="0"/>
         <v>-4.7000000000000035E-2</v>
@@ -3856,13 +3872,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="34">
+      <c r="A25" s="33">
         <v>-2E-3</v>
       </c>
-      <c r="B25" s="34">
+      <c r="B25" s="33">
         <v>-1E-3</v>
       </c>
-      <c r="C25" s="34"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="14">
         <f t="shared" si="0"/>
         <v>-6.0000000000000039E-2</v>
@@ -3873,13 +3889,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="34">
+      <c r="A26" s="33">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="B26" s="34">
+      <c r="B26" s="33">
         <v>-2.6000000000000002E-2</v>
       </c>
-      <c r="C26" s="34"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="14">
         <f t="shared" si="0"/>
         <v>-9.200000000000004E-2</v>
@@ -3890,13 +3906,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="34">
+      <c r="A27" s="33">
         <v>1.1000000000000001E-2</v>
       </c>
-      <c r="B27" s="34">
+      <c r="B27" s="33">
         <v>6.9999999999999993E-3</v>
       </c>
-      <c r="C27" s="34"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="14">
         <f t="shared" si="0"/>
         <v>-9.200000000000004E-2</v>
@@ -3907,13 +3923,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="34">
+      <c r="A28" s="33">
         <v>4.7E-2</v>
       </c>
-      <c r="B28" s="34">
+      <c r="B28" s="33">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="14">
         <f t="shared" si="0"/>
         <v>-5.6000000000000043E-2</v>
@@ -3924,13 +3940,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="34">
+      <c r="A29" s="33">
         <v>2.4E-2</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="33">
         <v>2.8999999999999998E-2</v>
       </c>
-      <c r="C29" s="34"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="14">
         <f t="shared" si="0"/>
         <v>-4.3000000000000045E-2</v>
@@ -3941,13 +3957,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="34">
+      <c r="A30" s="33">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B30" s="33">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="14">
         <f t="shared" si="0"/>
         <v>-2.1000000000000046E-2</v>
@@ -3958,13 +3974,13 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="34">
+      <c r="A31" s="33">
         <v>-6.9999999999999993E-3</v>
       </c>
-      <c r="B31" s="34">
+      <c r="B31" s="33">
         <v>-2E-3</v>
       </c>
-      <c r="C31" s="34"/>
+      <c r="C31" s="33"/>
       <c r="D31" s="14">
         <f t="shared" si="0"/>
         <v>-3.9000000000000049E-2</v>
@@ -3975,13 +3991,13 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="34">
+      <c r="A32" s="33">
         <v>4.7E-2</v>
       </c>
-      <c r="B32" s="34">
+      <c r="B32" s="33">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C32" s="34"/>
+      <c r="C32" s="33"/>
       <c r="D32" s="14">
         <f t="shared" si="0"/>
         <v>-3.0000000000000495E-3</v>
@@ -3992,13 +4008,13 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="34">
+      <c r="A33" s="33">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="B33" s="34">
+      <c r="B33" s="33">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="C33" s="34"/>
+      <c r="C33" s="33"/>
       <c r="D33" s="14">
         <f t="shared" si="0"/>
         <v>-8.0000000000000505E-3</v>
@@ -4009,13 +4025,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="34">
+      <c r="A34" s="33">
         <v>0.01</v>
       </c>
-      <c r="B34" s="34">
+      <c r="B34" s="33">
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="C34" s="34"/>
+      <c r="C34" s="33"/>
       <c r="D34" s="14">
         <f t="shared" si="0"/>
         <v>-9.0000000000000514E-3</v>
@@ -4026,13 +4042,13 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="34">
+      <c r="A35" s="33">
         <v>-2E-3</v>
       </c>
-      <c r="B35" s="34">
+      <c r="B35" s="33">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C35" s="34"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="14">
         <f t="shared" si="0"/>
         <v>-2.2000000000000054E-2</v>
@@ -4043,13 +4059,13 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="34">
+      <c r="A36" s="33">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="B36" s="34">
+      <c r="B36" s="33">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="C36" s="34"/>
+      <c r="C36" s="33"/>
       <c r="D36" s="14">
         <f t="shared" si="0"/>
         <v>9.9999999999994711E-4</v>
@@ -4060,13 +4076,13 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="34">
+      <c r="A37" s="33">
         <v>0.01</v>
       </c>
-      <c r="B37" s="34">
+      <c r="B37" s="33">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="C37" s="34"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="14">
         <f t="shared" si="0"/>
         <v>-5.377642775528102E-17</v>

</xml_diff>

<commit_message>
Separated risk measures from performance measures, updated documention, and added some functions.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad9b1f9bd15b4598/C^N Source/PortfolioPerformance/PortfolioPerformance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="635" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7702B17-6949-41AB-8351-68FD864A48A5}"/>
+  <xr:revisionPtr revIDLastSave="1601" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE25DFB7-B722-4E05-8370-002781201400}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="3255" windowWidth="27480" windowHeight="15990" activeTab="3" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="8220" yWindow="4845" windowWidth="27480" windowHeight="15990" activeTab="6" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Table 2.4 and 2.5" sheetId="4" r:id="rId3"/>
     <sheet name="Tables 2.7, 2.8, and 2.9" sheetId="5" r:id="rId4"/>
+    <sheet name="Table 3.2" sheetId="6" r:id="rId5"/>
+    <sheet name="Tables 3.4 and 3.5" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -44,6 +47,88 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Timothy R. Mayes, Ph.D.</author>
+  </authors>
+  <commentList>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{CF8FD0E2-AB4C-42AE-B00C-02F694D08FF2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Timothy R. Mayes, Ph.D.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Here I set the data frequency to 1, so the measures are per period.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{D7173E70-8DD5-487D-9D9A-A83733576780}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Timothy R. Mayes, Ph.D.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is Bacon's methodology (i.e., use annualized returns instead of per period returns).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{5CCAA0DA-5FA8-4FC8-B47B-DA427260DD08}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Timothy R. Mayes, Ph.D.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Note that Bacon has the skewness with the wrong sign on page 52, though this doesn't affect his result.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -67,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
   <si>
     <t>RFR</t>
   </si>
@@ -271,6 +356,84 @@
   </si>
   <si>
     <t>Population Kurtosis</t>
+  </si>
+  <si>
+    <t>Risk-Free</t>
+  </si>
+  <si>
+    <t>Adjusted Sharpe Ratio</t>
+  </si>
+  <si>
+    <t>Using Annualized Returns</t>
+  </si>
+  <si>
+    <t>Per Period</t>
+  </si>
+  <si>
+    <t>Tracking Error Arith</t>
+  </si>
+  <si>
+    <t>Tracking Error Geom</t>
+  </si>
+  <si>
+    <t>Annualized</t>
+  </si>
+  <si>
+    <t>Information Ratio Arith</t>
+  </si>
+  <si>
+    <t>Information Ratio Geom</t>
+  </si>
+  <si>
+    <t>Std Deviation</t>
+  </si>
+  <si>
+    <t>All Match?</t>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>All Equal?</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Appraisal Ratio</t>
+  </si>
+  <si>
+    <t>Var Asset</t>
+  </si>
+  <si>
+    <t>Var Mkt</t>
+  </si>
+  <si>
+    <t>Mkt Risk</t>
+  </si>
+  <si>
+    <t>Unique Risk</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Semi-variance</t>
+  </si>
+  <si>
+    <t>Semi-deviation</t>
   </si>
 </sst>
 </file>
@@ -289,11 +452,11 @@
     <numFmt numFmtId="171" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="172" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="173" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="0.00000000000000%"/>
-    <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="0.0%"/>
+    <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.00000000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +471,26 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -336,7 +519,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -380,11 +563,15 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -792,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F76F22F-5A0F-4104-B600-63C465102B60}">
   <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,11 +1870,11 @@
       </c>
       <c r="G30" s="13" cm="1">
         <f t="array" ref="G30">_xll.JensensAlpha(D3:D17,C3:C17,B3:B17)</f>
-        <v>7.2578822700353814E-4</v>
+        <v>7.1946041713468107E-4</v>
       </c>
       <c r="H30" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.3278098688568547E-6</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1883,21 +2070,33 @@
       <c r="M40" s="11"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F41" s="32"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="16"/>
+      <c r="H41" t="s">
+        <v>81</v>
+      </c>
+      <c r="K41" t="s">
+        <v>74</v>
+      </c>
       <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E42" s="11"/>
       <c r="G42" s="18" t="str" cm="1">
-        <f t="array" ref="G42:H51">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3)</f>
+        <f t="array" ref="G42:H51">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3,1)</f>
         <v>Risk Premium</v>
       </c>
       <c r="H42" s="1">
-        <v>2.8263315887266938E-4</v>
+        <v>2.6868219460207676E-4</v>
       </c>
       <c r="I42" s="30"/>
-      <c r="J42" s="11"/>
+      <c r="J42" s="36" t="str" cm="1">
+        <f t="array" ref="J42:K51">_xll.FamaDecomposition(D3:D17,C3:C17,B3:B17,1.3,12)</f>
+        <v>Risk Premium</v>
+      </c>
+      <c r="K42" s="1">
+        <v>3.2324595721133775E-3</v>
+      </c>
       <c r="L42" s="1"/>
       <c r="M42" s="11"/>
     </row>
@@ -1906,9 +2105,14 @@
         <v>Due to Risk</v>
       </c>
       <c r="H43" s="1">
-        <v>-4.4315506813086877E-4</v>
-      </c>
-      <c r="K43" s="11"/>
+        <v>-4.5077822253260436E-4</v>
+      </c>
+      <c r="J43" s="36" t="str">
+        <v>Due to Risk</v>
+      </c>
+      <c r="K43" s="1">
+        <v>-5.4009881205370957E-3</v>
+      </c>
       <c r="L43" s="1"/>
       <c r="M43" s="19"/>
     </row>
@@ -1917,16 +2121,27 @@
         <v>Due to Investor's Risk</v>
       </c>
       <c r="H44" s="1">
-        <v>-6.1130570994079043E-4</v>
-      </c>
-      <c r="J44" s="1"/>
+        <v>-6.2182139203192932E-4</v>
+      </c>
+      <c r="J44" s="37" t="str">
+        <v>Due to Investor's Risk</v>
+      </c>
+      <c r="K44" s="1">
+        <v>-7.450337624101566E-3</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G45" t="str">
         <v>Due to Manager's Risk</v>
       </c>
       <c r="H45" s="1">
-        <v>1.6815064180992164E-4</v>
+        <v>1.7104316949932498E-4</v>
+      </c>
+      <c r="J45" s="37" t="str">
+        <v>Due to Manager's Risk</v>
+      </c>
+      <c r="K45" s="1">
+        <v>2.0493495035644707E-3</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="20"/>
@@ -1936,7 +2151,13 @@
         <v>Due to Selectivity</v>
       </c>
       <c r="H46" s="1">
-        <v>7.2578822700353814E-4</v>
+        <v>7.1946041713468107E-4</v>
+      </c>
+      <c r="J46" s="37" t="str">
+        <v>Due to Selectivity</v>
+      </c>
+      <c r="K46" s="1">
+        <v>8.6334476926504741E-3</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -1944,7 +2165,13 @@
         <v>Diversification</v>
       </c>
       <c r="H47" s="1">
-        <v>8.5146079155431776E-5</v>
+        <v>8.6610762185780418E-5</v>
+      </c>
+      <c r="J47" s="37" t="str">
+        <v>Diversification</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1.0377247042856628E-3</v>
       </c>
       <c r="L47" s="1"/>
     </row>
@@ -1953,7 +2180,13 @@
         <v>Net Selectivity</v>
       </c>
       <c r="H48" s="1">
-        <v>6.4064214784810634E-4</v>
+        <v>6.3284965494890067E-4</v>
+      </c>
+      <c r="J48" s="37" t="str">
+        <v>Net Selectivity</v>
+      </c>
+      <c r="K48" s="1">
+        <v>7.5957229883648111E-3</v>
       </c>
       <c r="L48" s="1"/>
     </row>
@@ -1962,10 +2195,14 @@
         <v>Hypothetical Beta</v>
       </c>
       <c r="H49" s="29">
-        <v>1.3134730578655345</v>
-      </c>
-      <c r="J49" s="8"/>
-      <c r="K49" s="31"/>
+        <v>1.3134730578655347</v>
+      </c>
+      <c r="J49" s="23" t="str">
+        <v>Hypothetical Beta</v>
+      </c>
+      <c r="K49" s="29">
+        <v>1.3134730578655347</v>
+      </c>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="7:12" x14ac:dyDescent="0.25">
@@ -1973,7 +2210,13 @@
         <v>Hypothetical Exp Return</v>
       </c>
       <c r="H50" s="1">
-        <v>-5.1901011403769886E-4</v>
+        <v>-5.2963667077848419E-4</v>
+      </c>
+      <c r="J50" s="37" t="str">
+        <v>Hypothetical Exp Return</v>
+      </c>
+      <c r="K50" s="1">
+        <v>-6.3433593458563399E-3</v>
       </c>
     </row>
     <row r="51" spans="7:12" x14ac:dyDescent="0.25">
@@ -1981,7 +2224,13 @@
         <v>Hypothetical Risk Premium</v>
       </c>
       <c r="H51" s="1">
-        <v>-6.176412154819934E-4</v>
+        <v>-6.2826588095260126E-4</v>
+      </c>
+      <c r="J51" s="37" t="str">
+        <v>Hypothetical Risk Premium</v>
+      </c>
+      <c r="K51" s="1">
+        <v>-7.527552108661021E-3</v>
       </c>
     </row>
     <row r="52" spans="7:12" x14ac:dyDescent="0.25">
@@ -3321,8 +3570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4799EC79-C9E3-4E9F-9D8B-C1C9DE78CC72}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3355,13 +3604,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
+      <c r="A2" s="32">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="32">
         <v>2E-3</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="14">
         <f>A2-H$2</f>
         <v>-8.0000000000000002E-3</v>
@@ -3383,13 +3632,13 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
+      <c r="A3" s="32">
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="14">
         <f>D2+A3-H$2</f>
         <v>7.000000000000001E-3</v>
@@ -3411,13 +3660,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+      <c r="A4" s="32">
         <v>1.1000000000000001E-2</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="32">
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D37" si="0">D3+A4-H$2</f>
         <v>7.000000000000001E-3</v>
@@ -3439,13 +3688,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
+      <c r="A5" s="32">
         <v>-9.0000000000000011E-3</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="32">
         <v>-1.1000000000000001E-2</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="14">
         <f t="shared" si="0"/>
         <v>-1.3000000000000001E-2</v>
@@ -3467,13 +3716,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+      <c r="A6" s="32">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="32">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
         <v>-1.0000000000000004E-2</v>
@@ -3495,13 +3744,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
+      <c r="A7" s="32">
         <v>2.4E-2</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>2.3E-2</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
         <v>2.9999999999999957E-3</v>
@@ -3523,13 +3772,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="33">
+      <c r="A8" s="32">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="14">
         <f t="shared" si="0"/>
         <v>6.9999999999999941E-3</v>
@@ -3540,13 +3789,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
+      <c r="A9" s="32">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="14">
         <f t="shared" si="0"/>
         <v>6.1999999999999993E-2</v>
@@ -3563,13 +3812,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="33">
+      <c r="A10" s="32">
         <v>-1.3999999999999999E-2</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="32">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="14">
         <f t="shared" si="0"/>
         <v>3.6999999999999991E-2</v>
@@ -3581,22 +3830,22 @@
       <c r="G10" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="34">
         <v>1</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I10" s="34">
         <f>H10</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
+      <c r="A11" s="32">
         <v>3.9E-2</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="14">
         <f t="shared" si="0"/>
         <v>6.4999999999999988E-2</v>
@@ -3608,23 +3857,23 @@
       <c r="G11" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="34" cm="1">
+      <c r="H11" s="33" cm="1">
         <f t="array" ref="H11">SUM((A2:A37&gt;=0)*(A2:A37&lt;=H3))</f>
         <v>14</v>
       </c>
-      <c r="I11" s="34" cm="1">
+      <c r="I11" s="33" cm="1">
         <f t="array" ref="I11">SUM((B2:B37&gt;=0)*(B2:B37&lt;=I3))</f>
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
+      <c r="A12" s="32">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="14">
         <f t="shared" si="0"/>
         <v>4.8999999999999988E-2</v>
@@ -3636,23 +3885,23 @@
       <c r="G12" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="34" cm="1">
+      <c r="H12" s="33" cm="1">
         <f t="array" ref="H12">SUM((A2:A37&lt;0)*(A2:A37&gt;=-H3))</f>
         <v>9</v>
       </c>
-      <c r="I12" s="34" cm="1">
+      <c r="I12" s="33" cm="1">
         <f t="array" ref="I12">SUM((B2:B37&lt;0)*(B2:B37&gt;=-I3))</f>
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
+      <c r="A13" s="32">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="14">
         <f t="shared" si="0"/>
         <v>0.11900000000000001</v>
@@ -3674,13 +3923,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="33">
+      <c r="A14" s="32">
         <v>0.04</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>3.9E-2</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="14">
         <f t="shared" si="0"/>
         <v>0.14799999999999999</v>
@@ -3702,13 +3951,13 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
+      <c r="A15" s="32">
         <v>-3.7000000000000005E-2</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="32">
         <v>-3.7999999999999999E-2</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="14">
         <f t="shared" si="0"/>
         <v>9.9999999999999992E-2</v>
@@ -3719,13 +3968,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="33">
+      <c r="A16" s="32">
         <v>-6.0999999999999999E-2</v>
       </c>
-      <c r="B16" s="33">
+      <c r="B16" s="32">
         <v>-6.2E-2</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="14">
         <f t="shared" si="0"/>
         <v>2.799999999999999E-2</v>
@@ -3736,13 +3985,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="33">
+      <c r="A17" s="32">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="32">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C17" s="33"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="14">
         <f t="shared" si="0"/>
         <v>3.0999999999999986E-2</v>
@@ -3753,13 +4002,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
+      <c r="A18" s="32">
         <v>-4.9000000000000002E-2</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>-4.8000000000000001E-2</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="14">
         <f t="shared" si="0"/>
         <v>-2.9000000000000019E-2</v>
@@ -3770,13 +4019,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
+      <c r="A19" s="32">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="32">
         <v>-0.02</v>
       </c>
-      <c r="C19" s="33"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="14">
         <f t="shared" si="0"/>
         <v>-6.1000000000000019E-2</v>
@@ -3787,13 +4036,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
+      <c r="A20" s="32">
         <v>6.2E-2</v>
       </c>
-      <c r="B20" s="33">
+      <c r="B20" s="32">
         <v>0.06</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="14">
         <f t="shared" si="0"/>
         <v>-1.0000000000000021E-2</v>
@@ -3804,13 +4053,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="33">
+      <c r="A21" s="32">
         <v>5.7999999999999996E-2</v>
       </c>
-      <c r="B21" s="33">
+      <c r="B21" s="32">
         <v>5.5999999999999994E-2</v>
       </c>
-      <c r="C21" s="33"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="14">
         <f t="shared" si="0"/>
         <v>3.699999999999997E-2</v>
@@ -3821,13 +4070,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="33">
+      <c r="A22" s="32">
         <v>-6.4000000000000001E-2</v>
       </c>
-      <c r="B22" s="33">
+      <c r="B22" s="32">
         <v>-6.7000000000000004E-2</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="32"/>
       <c r="D22" s="14">
         <f t="shared" si="0"/>
         <v>-3.8000000000000034E-2</v>
@@ -3838,13 +4087,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="33">
+      <c r="A23" s="32">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="B23" s="33">
+      <c r="B23" s="32">
         <v>1.9E-2</v>
       </c>
-      <c r="C23" s="33"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="14">
         <f t="shared" si="0"/>
         <v>-3.2000000000000035E-2</v>
@@ -3855,13 +4104,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="33">
+      <c r="A24" s="32">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="B24" s="33">
+      <c r="B24" s="32">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="14">
         <f t="shared" si="0"/>
         <v>-4.7000000000000035E-2</v>
@@ -3872,13 +4121,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="33">
+      <c r="A25" s="32">
         <v>-2E-3</v>
       </c>
-      <c r="B25" s="33">
+      <c r="B25" s="32">
         <v>-1E-3</v>
       </c>
-      <c r="C25" s="33"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="14">
         <f t="shared" si="0"/>
         <v>-6.0000000000000039E-2</v>
@@ -3889,13 +4138,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="33">
+      <c r="A26" s="32">
         <v>-2.1000000000000001E-2</v>
       </c>
-      <c r="B26" s="33">
+      <c r="B26" s="32">
         <v>-2.6000000000000002E-2</v>
       </c>
-      <c r="C26" s="33"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="14">
         <f t="shared" si="0"/>
         <v>-9.200000000000004E-2</v>
@@ -3906,13 +4155,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="33">
+      <c r="A27" s="32">
         <v>1.1000000000000001E-2</v>
       </c>
-      <c r="B27" s="33">
+      <c r="B27" s="32">
         <v>6.9999999999999993E-3</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="14">
         <f t="shared" si="0"/>
         <v>-9.200000000000004E-2</v>
@@ -3923,13 +4172,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="33">
+      <c r="A28" s="32">
         <v>4.7E-2</v>
       </c>
-      <c r="B28" s="33">
+      <c r="B28" s="32">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="C28" s="33"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="14">
         <f t="shared" si="0"/>
         <v>-5.6000000000000043E-2</v>
@@ -3940,13 +4189,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="33">
+      <c r="A29" s="32">
         <v>2.4E-2</v>
       </c>
-      <c r="B29" s="33">
+      <c r="B29" s="32">
         <v>2.8999999999999998E-2</v>
       </c>
-      <c r="C29" s="33"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="14">
         <f t="shared" si="0"/>
         <v>-4.3000000000000045E-2</v>
@@ -3957,13 +4206,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="33">
+      <c r="A30" s="32">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="B30" s="33">
+      <c r="B30" s="32">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="C30" s="33"/>
+      <c r="C30" s="32"/>
       <c r="D30" s="14">
         <f t="shared" si="0"/>
         <v>-2.1000000000000046E-2</v>
@@ -3974,13 +4223,13 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="33">
+      <c r="A31" s="32">
         <v>-6.9999999999999993E-3</v>
       </c>
-      <c r="B31" s="33">
+      <c r="B31" s="32">
         <v>-2E-3</v>
       </c>
-      <c r="C31" s="33"/>
+      <c r="C31" s="32"/>
       <c r="D31" s="14">
         <f t="shared" si="0"/>
         <v>-3.9000000000000049E-2</v>
@@ -3991,13 +4240,13 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="33">
+      <c r="A32" s="32">
         <v>4.7E-2</v>
       </c>
-      <c r="B32" s="33">
+      <c r="B32" s="32">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C32" s="33"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="14">
         <f t="shared" si="0"/>
         <v>-3.0000000000000495E-3</v>
@@ -4008,13 +4257,13 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="33">
+      <c r="A33" s="32">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="B33" s="33">
+      <c r="B33" s="32">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="C33" s="33"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="14">
         <f t="shared" si="0"/>
         <v>-8.0000000000000505E-3</v>
@@ -4025,13 +4274,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="33">
+      <c r="A34" s="32">
         <v>0.01</v>
       </c>
-      <c r="B34" s="33">
+      <c r="B34" s="32">
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="C34" s="33"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="14">
         <f t="shared" si="0"/>
         <v>-9.0000000000000514E-3</v>
@@ -4042,13 +4291,13 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="33">
+      <c r="A35" s="32">
         <v>-2E-3</v>
       </c>
-      <c r="B35" s="33">
+      <c r="B35" s="32">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C35" s="33"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="14">
         <f t="shared" si="0"/>
         <v>-2.2000000000000054E-2</v>
@@ -4059,13 +4308,13 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="33">
+      <c r="A36" s="32">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="B36" s="33">
+      <c r="B36" s="32">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="C36" s="33"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="14">
         <f t="shared" si="0"/>
         <v>9.9999999999994711E-4</v>
@@ -4076,13 +4325,13 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="33">
+      <c r="A37" s="32">
         <v>0.01</v>
       </c>
-      <c r="B37" s="33">
+      <c r="B37" s="32">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="C37" s="33"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="14">
         <f t="shared" si="0"/>
         <v>-5.377642775528102E-17</v>
@@ -4090,6 +4339,1456 @@
       <c r="E37" s="14">
         <f t="shared" si="1"/>
         <v>-1.1102230246251565E-16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD720BF-B3A2-4768-8CA5-EE00905CFCE9}">
+  <dimension ref="A1:M37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="L1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B2" s="32">
+        <v>2E-3</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="B3" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" cm="1">
+        <f t="array" ref="F3">GEOMEAN(1+A2:A37)-1</f>
+        <v>1.0452163610398468E-2</v>
+      </c>
+      <c r="G3" s="1" cm="1">
+        <f t="array" ref="G3">PRODUCT(1+A2:A37)^(12/36)-1</f>
+        <v>0.13289353350977429</v>
+      </c>
+      <c r="I3" s="1" cm="1">
+        <f t="array" ref="I3">GEOMEAN(1+B2:B37)-1</f>
+        <v>1.1436247371426456E-2</v>
+      </c>
+      <c r="J3" s="1" cm="1">
+        <f t="array" ref="J3">PRODUCT(1+B2:B37)^(12/36)-1</f>
+        <v>0.14620464307207515</v>
+      </c>
+      <c r="L3" s="1" cm="1">
+        <f t="array" ref="L3">GEOMEAN(1+C2:C37)-1</f>
+        <v>1.9995843306364058E-3</v>
+      </c>
+      <c r="M3" s="1" cm="1">
+        <f t="array" ref="M3">PRODUCT(1+C2:C37)^(12/36)-1</f>
+        <v>2.4260669083983943E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="1">
+        <f>_xlfn.STDEV.P(A2:A37)</f>
+        <v>3.3173784830796742E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4*SQRT(12)</f>
+        <v>0.11491736161259533</v>
+      </c>
+      <c r="I4" s="1">
+        <f>_xlfn.STDEV.P(B2:B37)</f>
+        <v>3.3620430296671298E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <f>I4*SQRT(12)</f>
+        <v>0.11646458689232533</v>
+      </c>
+      <c r="L4" s="1">
+        <f>_xlfn.STDEV.P(C2:C37)</f>
+        <v>9.1287092917527674E-4</v>
+      </c>
+      <c r="M4" s="1">
+        <f>L4*SQRT(12)</f>
+        <v>3.1622776601683785E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>-9.0000000000000011E-3</v>
+      </c>
+      <c r="B5" s="32">
+        <v>-1.1000000000000001E-2</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B6" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="21">
+        <f>(F3-L3)/F4</f>
+        <v>0.25479695255981605</v>
+      </c>
+      <c r="G6" s="21">
+        <f>(G3-M3)/G4</f>
+        <v>0.94531290051723404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B7" s="32">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="21" cm="1">
+        <f t="array" ref="F7">(F3-L3)/_xlfn.STDEV.P(A2:A37-C2:C37)</f>
+        <v>0.25497722129753936</v>
+      </c>
+      <c r="G7" s="21" cm="1">
+        <f t="array" ref="G7">(G3-M3)/(_xlfn.STDEV.P(A2:A37-C2:C37)*SQRT(12))</f>
+        <v>0.9459817090002941</v>
+      </c>
+      <c r="J7">
+        <f>_xlfn.VAR.P(B2:B37)</f>
+        <v>1.1303333333333335E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B8" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="21" cm="1">
+        <f t="array" ref="F8">F6+_xll.Skewness_P(A2:A37)/6*F6^2-(_xll.Kurtosis_P(A2:A37)-3)/24*F6^3</f>
+        <v>0.25223719852260701</v>
+      </c>
+      <c r="G8" s="27" cm="1">
+        <f t="array" ref="G8">G6+_xll.Skewness_P(A2:A37)/6*G6^2-(_xll.Kurtosis_P(A2:A37)-3)/24*G6^3</f>
+        <v>0.91065390211902919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B9" s="32">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C9" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="1">
+        <f>F6*_xlfn.STDEV.P($B$2:$B$37)+$L$3</f>
+        <v>1.0565967513977965E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <f>G6*_xlfn.STDEV.P($B$2:$B$37)*SQRT(12)+M3</f>
+        <v>0.13435614552670944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>-1.3999999999999999E-2</v>
+      </c>
+      <c r="B10" s="32">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="C10" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="21">
+        <f>_xlfn.COVARIANCE.P(A2:A37,B2:B37)/_xlfn.VAR.P(B2:B37)</f>
+        <v>0.98144598446869191</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B11" s="32">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C11" s="14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="21">
+        <f>(F3-L3)/F10</f>
+        <v>8.6123733893902332E-3</v>
+      </c>
+      <c r="G11" s="21">
+        <f>(G3-M3)/F10</f>
+        <v>0.11068654428760948</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="B12" s="32">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C12" s="14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <f>F3-L3-F10*(I3-L3)</f>
+        <v>-8.089957684054485E-4</v>
+      </c>
+      <c r="G12" s="1">
+        <f>G3-M3-F10*(J3-M3)</f>
+        <v>-1.104855917497638E-2</v>
+      </c>
+      <c r="I12" s="28"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="B13" s="32">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C13" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="8">
+        <f>F12/SQRT(_xlfn.VAR.P(A2:A37)-F10^2*_xlfn.VAR.P(B2:B37))</f>
+        <v>-0.23629010561291675</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="B14" s="32">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="8" cm="1">
+        <f t="array" ref="F14">SUM(IF(AVERAGE(A2:A37)-A2:A37&lt;0,0,(AVERAGE(A2:A37)-A2:A37)^2))/COUNT(A2:A37)</f>
+        <v>5.83888888888889E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="B15" s="32">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="8">
+        <f>SQRT(F14)</f>
+        <v>2.4163792932585915E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="B16" s="32">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="C16" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B17" s="32">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C17" s="14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="21" cm="1">
+        <f t="array" ref="F17">_xll.SharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25479695255981605</v>
+      </c>
+      <c r="G17" s="21" cm="1">
+        <f t="array" ref="G17">_xll.SharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.94531290051723404</v>
+      </c>
+      <c r="I17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" t="b" cm="1">
+        <f t="array" ref="J17">AND(F6:G15=F17:G26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="B18" s="32">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="21" cm="1">
+        <f t="array" ref="F18">_xll.RevisedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25497722129753936</v>
+      </c>
+      <c r="G18" s="21" cm="1">
+        <f t="array" ref="G18">_xll.RevisedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.9459817090002941</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B19" s="32">
+        <v>-0.02</v>
+      </c>
+      <c r="C19" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="21" cm="1">
+        <f t="array" ref="F19">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25223719852260701</v>
+      </c>
+      <c r="G19" s="21" cm="1">
+        <f t="array" ref="G19">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.91065390211902919</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>6.2E-2</v>
+      </c>
+      <c r="B20" s="32">
+        <v>0.06</v>
+      </c>
+      <c r="C20" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="1" cm="1">
+        <f t="array" ref="F20">_xll.MSquared(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>1.0565967513977965E-2</v>
+      </c>
+      <c r="G20" s="1" cm="1">
+        <f t="array" ref="G20">_xll.MSquared(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>0.13435614552670944</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="B21" s="32">
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="21" cm="1">
+        <f t="array" ref="F21">_xll.Beta(A2:A37,B2:B37)</f>
+        <v>0.98144598446869202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="B22" s="32">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="21" cm="1">
+        <f t="array" ref="F22">_xll.TreynorIndex(A2:A37,F21,C2:C37,1)</f>
+        <v>8.6123733893902332E-3</v>
+      </c>
+      <c r="G22" s="21" cm="1">
+        <f t="array" ref="G22">_xll.TreynorIndex(A2:A37,F21,C2:C37,12)</f>
+        <v>0.11068654428760946</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B23" s="32">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1" cm="1">
+        <f t="array" ref="F23">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>-8.089957684054485E-4</v>
+      </c>
+      <c r="G23" s="1" cm="1">
+        <f t="array" ref="G23">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>-1.1048559174976394E-2</v>
+      </c>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="B24" s="32">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="8" cm="1">
+        <f t="array" ref="F24">_xll.AppraisalRatio($A$2:$A$37,$B$2:$B$37,$C$2:$C$37,1)</f>
+        <v>-0.23629010561291894</v>
+      </c>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>-2E-3</v>
+      </c>
+      <c r="B25" s="32">
+        <v>-1E-3</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="8" cm="1">
+        <f t="array" ref="F25">_xll.SemiVariance(A2:A37)</f>
+        <v>5.83888888888889E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B26" s="32">
+        <v>-2.6000000000000002E-2</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="8" cm="1">
+        <f t="array" ref="F26">_xll.SemiDeviation(A2:A37)</f>
+        <v>2.4163792932585915E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <f>_xlfn.VAR.P(B2:B37)*12*F10^2</f>
+        <v>1.3065336093908721E-2</v>
+      </c>
+      <c r="K26" s="14">
+        <f>F10*_xlfn.STDEV.P(B2:B37)</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B27" s="32">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="F27" s="35"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B28" s="32">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B29" s="32">
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="B30" s="32">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C30" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>-6.9999999999999993E-3</v>
+      </c>
+      <c r="B31" s="32">
+        <v>-2E-3</v>
+      </c>
+      <c r="C31" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="1">
+        <f>_xlfn.VAR.P(A2:A37)</f>
+        <v>1.1005000000000001E-3</v>
+      </c>
+      <c r="G31" s="1">
+        <f>SQRT(F31*12)</f>
+        <v>0.11491736161259535</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B32" s="32">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C32" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="1">
+        <f>_xlfn.VAR.P(B2:B37)</f>
+        <v>1.1303333333333335E-3</v>
+      </c>
+      <c r="G32" s="1">
+        <f>F32*12</f>
+        <v>1.3564000000000001E-2</v>
+      </c>
+      <c r="J32" s="1">
+        <f>F10^2*_xlfn.VAR.P(B2:B37)</f>
+        <v>1.0887780078257267E-3</v>
+      </c>
+      <c r="K32">
+        <f>SQRT(J32)</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B33" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C33" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="1">
+        <f>F10^2*F32</f>
+        <v>1.0887780078257267E-3</v>
+      </c>
+      <c r="G33" s="14">
+        <f>SQRT(F33)</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
+      <c r="H33" s="1" cm="1">
+        <f t="array" ref="H33">SQRT(_xll.MarketRisk(A2:A37,B2:B37,1))</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="B34" s="32">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="C34" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="1">
+        <f>F31-F10^2*F32</f>
+        <v>1.1721992174273423E-5</v>
+      </c>
+      <c r="G34" s="1">
+        <f>SQRT(F34)</f>
+        <v>3.4237395015207311E-3</v>
+      </c>
+      <c r="H34" s="1" cm="1">
+        <f t="array" ref="H34">_xll.UniqueRisk(A2:A37,B2:B37,1)</f>
+        <v>1.1721992174273206E-5</v>
+      </c>
+      <c r="I34">
+        <f>SQRT(H34)</f>
+        <v>3.4237395015206994E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>-2E-3</v>
+      </c>
+      <c r="B35" s="32">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C35" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="H35" s="11">
+        <f>SUM(H33:H34)</f>
+        <v>3.3008358302951873E-2</v>
+      </c>
+      <c r="I35">
+        <f>SQRT(H35)</f>
+        <v>0.18168202526103641</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B36" s="32">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C36" s="14">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="B37" s="32">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C37" s="14">
+        <v>2E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D735904-470D-4D59-8599-F50297C87148}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B2" s="32">
+        <v>2E-3</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="E2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="B3" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B4" s="32">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14" cm="1">
+        <f t="array" ref="E4">GEOMEAN(1+A2:A37)-1</f>
+        <v>1.0452163610398468E-2</v>
+      </c>
+      <c r="F4" s="14" cm="1">
+        <f t="array" ref="F4">PRODUCT(1+A2:A37)^(12/36)-1</f>
+        <v>0.13289353350977429</v>
+      </c>
+      <c r="H4" s="14" cm="1">
+        <f t="array" ref="H4">GEOMEAN(1+B2:B37)-1</f>
+        <v>1.1436247371426456E-2</v>
+      </c>
+      <c r="I4" s="14" cm="1">
+        <f t="array" ref="I4">PRODUCT(1+B2:B37)^(12/36)-1</f>
+        <v>0.14620464307207515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>-9.0000000000000011E-3</v>
+      </c>
+      <c r="B5" s="32">
+        <v>-1.1000000000000001E-2</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="14">
+        <f>_xlfn.STDEV.P(A2:A37)</f>
+        <v>3.3173784830796742E-2</v>
+      </c>
+      <c r="F5" s="14">
+        <f>E5*SQRT(12)</f>
+        <v>0.11491736161259533</v>
+      </c>
+      <c r="H5" s="14">
+        <f>_xlfn.STDEV.P(B2:B37)</f>
+        <v>3.3620430296671298E-2</v>
+      </c>
+      <c r="I5" s="14">
+        <f>H5*SQRT(12)</f>
+        <v>0.11646458689232533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B6" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C6" s="32"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B7" s="32">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="1" cm="1">
+        <f t="array" ref="E7">_xlfn.STDEV.P(A2:A37-B2:B37)</f>
+        <v>3.4801021696368502E-3</v>
+      </c>
+      <c r="F7" s="1" cm="1">
+        <f t="array" ref="F7">_xlfn.STDEV.P(A2:A37-B2:B37)*SQRT(12)</f>
+        <v>1.2055427546683416E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B8" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="1" cm="1">
+        <f t="array" ref="E8">_xlfn.STDEV.P((1+A2:A37)/(1+B2:B37)-1)</f>
+        <v>3.4318750190674599E-3</v>
+      </c>
+      <c r="F8" s="1" cm="1">
+        <f t="array" ref="F8">_xlfn.STDEV.P((1+A2:A37)/(1+B2:B37)-1)*SQRT(12)</f>
+        <v>1.18883637965025E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B9" s="32">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="29">
+        <f>(E4-H4)/E7</f>
+        <v>-0.2827743879515689</v>
+      </c>
+      <c r="F9" s="29">
+        <f>(F4-I4)/F7</f>
+        <v>-1.1041590611991938</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
+        <v>-1.3999999999999999E-2</v>
+      </c>
+      <c r="B10" s="32">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="29">
+        <f>((1+E4)/(1+H4)-1)/E8</f>
+        <v>-0.28350589142369115</v>
+      </c>
+      <c r="F10" s="29">
+        <f>((1+F4)/(1+I4)-1)/F8</f>
+        <v>-0.97685478507947687</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B11" s="32">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C11" s="32"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="32">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="B12" s="32">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C12" s="32"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="B13" s="32">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="1" cm="1">
+        <f t="array" ref="E13">_xll.TrackingErrorArithmetic(A2:A37,B2:B37,1)</f>
+        <v>3.4801021696368507E-3</v>
+      </c>
+      <c r="F13" s="1" cm="1">
+        <f t="array" ref="F13">_xll.TrackingErrorArithmetic(A2:A37,B2:B37,12)</f>
+        <v>1.2055427546683418E-2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" t="b" cm="1">
+        <f t="array" ref="I13">AND(E7:F10=E13:F16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <v>0.04</v>
+      </c>
+      <c r="B14" s="32">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="1" cm="1">
+        <f t="array" ref="E14">_xll.TrackingErrorGeometric(A2:A37,B2:B37,1)</f>
+        <v>3.4318750190674599E-3</v>
+      </c>
+      <c r="F14" s="1" cm="1">
+        <f t="array" ref="F14">_xll.TrackingErrorGeometric(A2:A37,B2:B37,12)</f>
+        <v>1.18883637965025E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="B15" s="32">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="29" cm="1">
+        <f t="array" ref="E15">_xll.InformationRatioArithmetic(A2:A37,B2:B37,1)</f>
+        <v>-0.28277438795156884</v>
+      </c>
+      <c r="F15" s="29" cm="1">
+        <f t="array" ref="F15">_xll.InformationRatioArithmetic(A2:A37,B2:B37,12)</f>
+        <v>-1.1041590611991936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="B16" s="32">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="29" cm="1">
+        <f t="array" ref="E16">_xll.InformationRatioGeometric(A2:A37,B2:B37,1)</f>
+        <v>-0.28350589142369115</v>
+      </c>
+      <c r="F16" s="29" cm="1">
+        <f t="array" ref="F16">_xll.InformationRatioGeometric(A2:A37,B2:B37,12)</f>
+        <v>-0.97685478507947687</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B17" s="32">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C17" s="32"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="32">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="B18" s="32">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="32">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B19" s="32">
+        <v>-0.02</v>
+      </c>
+      <c r="C19" s="32"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <v>6.2E-2</v>
+      </c>
+      <c r="B20" s="32">
+        <v>0.06</v>
+      </c>
+      <c r="C20" s="32"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="32">
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="B21" s="32">
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="C21" s="32"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="32">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="B22" s="32">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="C22" s="32"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="32">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B23" s="32">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C23" s="32"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="32">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="B24" s="32">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="32"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="32">
+        <v>-2E-3</v>
+      </c>
+      <c r="B25" s="32">
+        <v>-1E-3</v>
+      </c>
+      <c r="C25" s="32"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="32">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B26" s="32">
+        <v>-2.6000000000000002E-2</v>
+      </c>
+      <c r="C26" s="32"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="32">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B27" s="32">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="C27" s="32"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="32">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B28" s="32">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C28" s="32"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="32">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B29" s="32">
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="C29" s="32"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="32">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="B30" s="32">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C30" s="32"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="32">
+        <v>-6.9999999999999993E-3</v>
+      </c>
+      <c r="B31" s="32">
+        <v>-2E-3</v>
+      </c>
+      <c r="C31" s="32"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="32">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B32" s="32">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C32" s="32"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="32">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B33" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C33" s="32"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="B34" s="32">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="C34" s="32"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="32">
+        <v>-2E-3</v>
+      </c>
+      <c r="B35" s="32">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C35" s="32"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="32">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B36" s="32">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C36" s="32"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="B37" s="32">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C37" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1041C9-4B35-43C1-9DE0-DEF26697FEC8}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <f>MAX(0,$H$1-A1)^$H$2</f>
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1">
+        <f>AVERAGE(A1:A10)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B10" si="0">MAX(0,$H$1-A2)^$H$2</f>
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="39">
+        <f>SUM(B1:B10)*(1/COUNT(B1:B10))</f>
+        <v>20</v>
+      </c>
+      <c r="C13" cm="1">
+        <f t="array" ref="C13">_xll.LowerPartialMoment(A1:A10, H1, H2,1)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a few functions, updated docs.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad9b1f9bd15b4598/C^N Source/PortfolioPerformance/PortfolioPerformance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1601" documentId="13_ncr:1_{279DD423-BAFB-4596-9FA7-C1D1A2B14100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE25DFB7-B722-4E05-8370-002781201400}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249F9969-9241-4222-8BE0-214A99BD5338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="4845" windowWidth="27480" windowHeight="15990" activeTab="6" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="9435" yWindow="5010" windowWidth="27480" windowHeight="15990" activeTab="4" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Table 3.2" sheetId="6" r:id="rId5"/>
     <sheet name="Tables 3.4 and 3.5" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet3" sheetId="8" r:id="rId7"/>
+    <sheet name="K-Ratio" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -101,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{5CCAA0DA-5FA8-4FC8-B47B-DA427260DD08}">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{5CCAA0DA-5FA8-4FC8-B47B-DA427260DD08}">
       <text>
         <r>
           <rPr>
@@ -130,7 +131,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -152,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="125">
   <si>
     <t>RFR</t>
   </si>
@@ -430,17 +431,122 @@
     <t>Degree</t>
   </si>
   <si>
-    <t>Semi-variance</t>
-  </si>
-  <si>
-    <t>Semi-deviation</t>
+    <t>K Ratio</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
+  </si>
+  <si>
+    <t>Port Value</t>
+  </si>
+  <si>
+    <t>Cum Ret</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Pred</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>Semi-variance Below Mean</t>
+  </si>
+  <si>
+    <t>Semi-deviation Below Mean</t>
+  </si>
+  <si>
+    <t>Semi-variance Above Mean</t>
+  </si>
+  <si>
+    <t>Sem--deviation Above Mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="14">
+  <numFmts count="15">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -455,8 +561,9 @@
     <numFmt numFmtId="174" formatCode="0.0%"/>
     <numFmt numFmtId="175" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="0.00000000%"/>
+    <numFmt numFmtId="177" formatCode="0.00000000000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,6 +603,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -505,12 +619,32 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -519,7 +653,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -572,13 +706,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -589,6 +761,917 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>'K-Ratio'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.23E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9100000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.3200000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.6000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7500000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.9199999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.2200000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.3599999999999989E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.3699999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.1017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3514-409B-8841-FDA775E4D652}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="885381352"/>
+        <c:axId val="885381680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="885381352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885381680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="885381680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="885381352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,6 +1758,47 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>100012</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63D74C09-E992-4897-879D-A9C83468F94E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1668,7 +2792,7 @@
       </c>
       <c r="L21" cm="1">
         <f t="array" ref="L21">_xll.Beta(L3:L17,K3:K17)</f>
-        <v>0.12710524781890767</v>
+        <v>0.1271052478189077</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1706,7 +2830,7 @@
       </c>
       <c r="G23" s="9" cm="1">
         <f t="array" ref="G23">_xll.BullBeta(D3:D17,C3:C17)</f>
-        <v>1.0869212641710995</v>
+        <v>1.0869212641710992</v>
       </c>
       <c r="H23" s="10">
         <f t="shared" ref="H23:H38" si="1">D23-G23</f>
@@ -1714,7 +2838,7 @@
       </c>
       <c r="L23" cm="1">
         <f t="array" ref="L23">_xll.BullBeta(L3:L17,K3:K17)</f>
-        <v>0.12710524781890767</v>
+        <v>0.1271052478189077</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1731,7 +2855,7 @@
       </c>
       <c r="G24" s="9" cm="1">
         <f t="array" ref="G24">_xll.BearBeta(D3:D17,C3:C17)</f>
-        <v>0.54207326774062647</v>
+        <v>0.54207326774062659</v>
       </c>
       <c r="H24" s="10">
         <f t="shared" si="1"/>
@@ -1756,7 +2880,7 @@
       </c>
       <c r="G25" s="9" cm="1">
         <f t="array" ref="G25">_xll.BetaTimingRatio(D3:D17,C3:C17)</f>
-        <v>2.005118733674899</v>
+        <v>2.0051187336748981</v>
       </c>
       <c r="H25" s="10">
         <f t="shared" si="1"/>
@@ -1783,11 +2907,11 @@
       <c r="E26" s="2"/>
       <c r="G26" s="9" cm="1">
         <f t="array" ref="G26">_xll.SharpeRatio(D3:D17,B3:B17)</f>
-        <v>5.1687248496316764E-2</v>
+        <v>5.0860520440393318E-2</v>
       </c>
       <c r="H26" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.2672805592344523E-4</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1806,11 +2930,11 @@
       <c r="E27" s="2"/>
       <c r="G27" s="9" cm="1">
         <f t="array" ref="G27">_xll.RevisedSharpeRatio(D3:D17,B3:B17)</f>
-        <v>5.1676557020390521E-2</v>
+        <v>5.0849999972662811E-2</v>
       </c>
       <c r="H27" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.2655704772772315E-4</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1828,11 +2952,11 @@
       </c>
       <c r="G28" s="9" cm="1">
         <f t="array" ref="G28">_xll.TreynorIndex(D3:D17,G21,B3:B17)</f>
-        <v>2.9990416146271964E-4</v>
+        <v>2.8510068879922587E-4</v>
       </c>
       <c r="H28" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4803472663493876E-5</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1849,11 +2973,11 @@
       </c>
       <c r="G29" s="9" cm="1">
         <f t="array" ref="G29">_xll.MSquared(D3:D17,C3:C17,B3:B17)</f>
-        <v>3.1381112145320415E-4</v>
+        <v>3.0318779856168554E-4</v>
       </c>
       <c r="H29" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.0623322891518668E-5</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3072,7 +4196,7 @@
       </c>
       <c r="K27" s="21" cm="1">
         <f t="array" ref="K27">_xll.Beta(K2:K11,$L$2:$L$11)</f>
-        <v>1.3736080990295685</v>
+        <v>1.3736080990295683</v>
       </c>
       <c r="L27" s="21" cm="1">
         <f t="array" ref="L27">_xll.Beta(L2:L11,$L$2:$L$11)</f>
@@ -3080,7 +4204,7 @@
       </c>
       <c r="M27" s="21" cm="1">
         <f t="array" ref="M27">_xll.Beta(M2:M11,$L$2:$L$11)</f>
-        <v>-1.0437227785546526E-2</v>
+        <v>-1.0437227785546527E-2</v>
       </c>
     </row>
     <row r="28" spans="8:13" x14ac:dyDescent="0.25">
@@ -3089,19 +4213,19 @@
       </c>
       <c r="I28" s="21" cm="1">
         <f t="array" ref="I28">_xll.SharpeRatio(I2:I11,$M$2:$M$11)</f>
-        <v>1.1661937725811693</v>
+        <v>1.1545617546995548</v>
       </c>
       <c r="J28" s="21" cm="1">
         <f t="array" ref="J28">_xll.SharpeRatio(J2:J11,$M$2:$M$11)</f>
-        <v>5.599865370514838E-2</v>
+        <v>-0.14124422465973449</v>
       </c>
       <c r="K28" s="21" cm="1">
         <f t="array" ref="K28">_xll.SharpeRatio(K2:K11,$M$2:$M$11)</f>
-        <v>0.45962709975051652</v>
+        <v>0.40908560600556776</v>
       </c>
       <c r="L28" s="21" cm="1">
         <f t="array" ref="L28">_xll.SharpeRatio(L2:L11,$M$2:$M$11)</f>
-        <v>0.56182641192316762</v>
+        <v>0.54723236351096227</v>
       </c>
       <c r="M28" s="21" cm="1">
         <f t="array" ref="M28">_xll.SharpeRatio(M2:M11,$M$2:$M$11)</f>
@@ -3114,19 +4238,19 @@
       </c>
       <c r="I29" s="21" cm="1">
         <f t="array" ref="I29">_xll.TreynorIndex(I2:I11,I27,$M$2:$M$11)</f>
-        <v>0.16550865893152097</v>
+        <v>0.1554491757883816</v>
       </c>
       <c r="J29" s="21" cm="1">
         <f t="array" ref="J29">_xll.TreynorIndex(J2:J11,J27,$M$2:$M$11)</f>
-        <v>1.9257822880708833E-2</v>
+        <v>-4.6080963991636754E-2</v>
       </c>
       <c r="K29" s="21" cm="1">
         <f t="array" ref="K29">_xll.TreynorIndex(K2:K11,K27,$M$2:$M$11)</f>
-        <v>6.5476970730925316E-2</v>
+        <v>5.5286411934401029E-2</v>
       </c>
       <c r="L29" s="21" cm="1">
         <f t="array" ref="L29">_xll.TreynorIndex(L2:L11,L27,$M$2:$M$11)</f>
-        <v>6.5437700595033191E-2</v>
+        <v>6.0467067503411798E-2</v>
       </c>
       <c r="M29" s="21" cm="1">
         <f t="array" ref="M29">_xll.TreynorIndex(M2:M11,M27,$M$2:$M$11)</f>
@@ -3139,15 +4263,15 @@
       </c>
       <c r="I30" s="21" cm="1">
         <f t="array" ref="I30">_xll.JensensAlpha(I2:I11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>0.15408274855897586</v>
+        <v>0.14624726845588906</v>
       </c>
       <c r="J30" s="21" cm="1">
         <f t="array" ref="J30">_xll.JensensAlpha(J2:J11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>-5.190139544964778E-2</v>
+        <v>-0.11974894241200459</v>
       </c>
       <c r="K30" s="21" cm="1">
         <f t="array" ref="K30">_xll.JensensAlpha(K2:K11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>5.394177671140532E-5</v>
+        <v>-7.1161904478758281E-3</v>
       </c>
       <c r="L30" s="21" cm="1">
         <f t="array" ref="L30">_xll.JensensAlpha(L2:L11,$L$2:$L$11,$M$2:$M$11)</f>
@@ -3155,7 +4279,7 @@
       </c>
       <c r="M30" s="21" cm="1">
         <f t="array" ref="M30">_xll.JensensAlpha(M2:M11,$L$2:$L$11,$M$2:$M$11)</f>
-        <v>6.8298818687275483E-4</v>
+        <v>6.3110855705712711E-4</v>
       </c>
     </row>
   </sheetData>
@@ -4348,25 +5472,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD720BF-B3A2-4768-8CA5-EE00905CFCE9}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -4388,8 +5515,11 @@
         <v>68</v>
       </c>
       <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -4417,8 +5547,24 @@
       <c r="M2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" cm="1">
+        <f t="array" ref="N2:N38">_xlfn.SEQUENCE(37)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="26">
+        <f>A2</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P2" s="14" cm="1">
+        <f t="array" ref="P2:P37">(1+O1:O36)*(1+O2:O37)-1</f>
+        <v>2.9999999999998916E-3</v>
+      </c>
+      <c r="R2" s="21" cm="1">
+        <f t="array" ref="R2:R38">TRANSPOSE(_xll.TotalReturnIndex(A2:A37,1000))</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2.6000000000000002E-2</v>
       </c>
@@ -4455,8 +5601,25 @@
         <f t="array" ref="M3">PRODUCT(1+C2:C37)^(12/36)-1</f>
         <v>2.4260669083983943E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3" s="26">
+        <f t="shared" ref="O3:O37" si="0">A3</f>
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="P3" s="14">
+        <v>2.9077999999999937E-2</v>
+      </c>
+      <c r="R3" s="21">
+        <v>1002.9999999999999</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" s="43"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>1.1000000000000001E-2</v>
       </c>
@@ -4493,8 +5656,27 @@
         <f>L4*SQRT(12)</f>
         <v>3.1622776601683785E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" s="26">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="P4" s="14">
+        <v>3.728599999999993E-2</v>
+      </c>
+      <c r="R4" s="21">
+        <v>1029.078</v>
+      </c>
+      <c r="T4" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" s="40">
+        <v>1.0924384153101352E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>-9.0000000000000011E-3</v>
       </c>
@@ -4504,8 +5686,27 @@
       <c r="C5" s="14">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5" s="26">
+        <f t="shared" si="0"/>
+        <v>-9.0000000000000011E-3</v>
+      </c>
+      <c r="P5" s="14">
+        <v>1.9009999999999305E-3</v>
+      </c>
+      <c r="R5" s="21">
+        <v>1040.3978579999998</v>
+      </c>
+      <c r="T5" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="U5" s="40">
+        <v>1.1934216912453192E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>1.3999999999999999E-2</v>
       </c>
@@ -4526,8 +5727,27 @@
         <f>(G3-M3)/G4</f>
         <v>0.94531290051723404</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6" s="26">
+        <f t="shared" si="0"/>
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="P6" s="14">
+        <v>4.874000000000045E-3</v>
+      </c>
+      <c r="R6" s="21">
+        <v>1031.0342772779998</v>
+      </c>
+      <c r="T6" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" s="40">
+        <v>-2.9288912472960039E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>2.4E-2</v>
       </c>
@@ -4552,8 +5772,27 @@
         <f>_xlfn.VAR.P(B2:B37)</f>
         <v>1.1303333333333335E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7" s="26">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
+      </c>
+      <c r="P7" s="14">
+        <v>3.8335999999999926E-2</v>
+      </c>
+      <c r="R7" s="21">
+        <v>1045.4687571598918</v>
+      </c>
+      <c r="T7" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="U7" s="40">
+        <v>4.7995453798732747E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -4574,8 +5813,28 @@
         <f t="array" ref="G8">G6+_xll.Skewness_P(A2:A37)/6*G6^2-(_xll.Kurtosis_P(A2:A37)-3)/24*G6^3</f>
         <v>0.91065390211902919</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="H8" s="35"/>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8" s="26">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P8" s="14">
+        <v>3.935999999999984E-2</v>
+      </c>
+      <c r="R8" s="21">
+        <v>1070.5600073317291</v>
+      </c>
+      <c r="T8" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="U8" s="41">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -4596,8 +5855,21 @@
         <f>G6*_xlfn.STDEV.P($B$2:$B$37)*SQRT(12)+M3</f>
         <v>0.13435614552670944</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9" s="26">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="P9" s="14">
+        <v>8.1990000000000007E-2</v>
+      </c>
+      <c r="R9" s="21">
+        <v>1086.6184074417049</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>-1.3999999999999999E-2</v>
       </c>
@@ -4615,8 +5887,24 @@
         <v>0.98144598446869191</v>
       </c>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>9</v>
+      </c>
+      <c r="O10" s="26">
+        <f t="shared" si="0"/>
+        <v>-1.3999999999999999E-2</v>
+      </c>
+      <c r="P10" s="14">
+        <v>5.1076000000000121E-2</v>
+      </c>
+      <c r="R10" s="21">
+        <v>1158.3352223328575</v>
+      </c>
+      <c r="T10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>3.9E-2</v>
       </c>
@@ -4637,8 +5925,37 @@
         <f>(G3-M3)/F10</f>
         <v>0.11068654428760948</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11" s="26">
+        <f t="shared" si="0"/>
+        <v>3.9E-2</v>
+      </c>
+      <c r="P11" s="14">
+        <v>2.4453999999999976E-2</v>
+      </c>
+      <c r="R11" s="21">
+        <v>1142.1185292201974</v>
+      </c>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="V11" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="W11" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="X11" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y11" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>-5.0000000000000001E-3</v>
       </c>
@@ -4659,9 +5976,40 @@
         <f>G3-M3-F10*(J3-M3)</f>
         <v>-1.104855917497638E-2</v>
       </c>
-      <c r="I12" s="28"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+      <c r="N12">
+        <v>11</v>
+      </c>
+      <c r="O12" s="26">
+        <f t="shared" si="0"/>
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="P12" s="14">
+        <v>3.3804999999999863E-2</v>
+      </c>
+      <c r="R12" s="21">
+        <v>1186.6611518597849</v>
+      </c>
+      <c r="T12" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="U12" s="40">
+        <v>1</v>
+      </c>
+      <c r="V12" s="40">
+        <v>9.3481329761779808E-6</v>
+      </c>
+      <c r="W12" s="40">
+        <v>9.3481329761779808E-6</v>
+      </c>
+      <c r="X12" s="40">
+        <v>4.0581180548453135E-3</v>
+      </c>
+      <c r="Y12" s="40">
+        <v>0.94957948962616467</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>8.1000000000000003E-2</v>
       </c>
@@ -4678,8 +6026,35 @@
         <f>F12/SQRT(_xlfn.VAR.P(A2:A37)-F10^2*_xlfn.VAR.P(B2:B37))</f>
         <v>-0.23629010561291675</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>12</v>
+      </c>
+      <c r="O13" s="26">
+        <f t="shared" si="0"/>
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="P13" s="14">
+        <v>7.5594999999999857E-2</v>
+      </c>
+      <c r="R13" s="21">
+        <v>1180.727846100486</v>
+      </c>
+      <c r="T13" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="U13" s="40">
+        <v>34</v>
+      </c>
+      <c r="V13" s="40">
+        <v>7.8321161901773836E-2</v>
+      </c>
+      <c r="W13" s="40">
+        <v>2.3035635853462895E-3</v>
+      </c>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="40"/>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>0.04</v>
       </c>
@@ -4690,14 +6065,39 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="F14" s="8" cm="1">
         <f t="array" ref="F14">SUM(IF(AVERAGE(A2:A37)-A2:A37&lt;0,0,(AVERAGE(A2:A37)-A2:A37)^2))/COUNT(A2:A37)</f>
         <v>5.83888888888889E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>13</v>
+      </c>
+      <c r="O14" s="26">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="P14" s="14">
+        <v>0.12423999999999991</v>
+      </c>
+      <c r="R14" s="21">
+        <v>1276.3668016346253</v>
+      </c>
+      <c r="T14" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="U14" s="41">
+        <v>35</v>
+      </c>
+      <c r="V14" s="41">
+        <v>7.8330510034750014E-2</v>
+      </c>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>-3.7000000000000005E-2</v>
       </c>
@@ -4708,14 +6108,27 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="F15" s="8">
         <f>SQRT(F14)</f>
         <v>2.4163792932585915E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>14</v>
+      </c>
+      <c r="O15" s="26">
+        <f t="shared" si="0"/>
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="P15" s="14">
+        <v>1.5199999999999658E-3</v>
+      </c>
+      <c r="R15" s="21">
+        <v>1327.4214737000104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>-6.0999999999999999E-2</v>
       </c>
@@ -4725,8 +6138,53 @@
       <c r="C16" s="14">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="8" cm="1">
+        <f t="array" ref="F16">SUM(IF(A2:A37-AVERAGE(A2:A37)&lt;0,0,(A2:A37-AVERAGE(A2:A37))^2))/COUNT(A2:A37)</f>
+        <v>5.1661111111111103E-4</v>
+      </c>
+      <c r="N16">
+        <v>15</v>
+      </c>
+      <c r="O16" s="26">
+        <f t="shared" si="0"/>
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="P16" s="14">
+        <v>-9.5743000000000023E-2</v>
+      </c>
+      <c r="R16" s="21">
+        <v>1278.30687917311</v>
+      </c>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="V16" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="W16" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="X16" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y16" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z16" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA16" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB16" s="42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>1.3999999999999999E-2</v>
       </c>
@@ -4737,25 +6195,54 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="21" cm="1">
-        <f t="array" ref="F17">_xll.SharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25479695255981605</v>
-      </c>
-      <c r="G17" s="21" cm="1">
-        <f t="array" ref="G17">_xll.SharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.94531290051723404</v>
-      </c>
-      <c r="I17" t="s">
-        <v>80</v>
-      </c>
-      <c r="J17" t="b" cm="1">
-        <f t="array" ref="J17">AND(F6:G15=F17:G26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="F17" s="8">
+        <f>SQRT(F16)</f>
+        <v>2.2729080736165089E-2</v>
+      </c>
+      <c r="N17">
+        <v>16</v>
+      </c>
+      <c r="O17" s="26">
+        <f t="shared" si="0"/>
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="P17" s="14">
+        <v>-4.7853999999999952E-2</v>
+      </c>
+      <c r="R17" s="21">
+        <v>1200.3301595435503</v>
+      </c>
+      <c r="T17" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="U17" s="40">
+        <v>2.0897433333333274E-2</v>
+      </c>
+      <c r="V17" s="40">
+        <v>1.6337712810835302E-2</v>
+      </c>
+      <c r="W17" s="40">
+        <v>1.2790917293804998</v>
+      </c>
+      <c r="X17" s="40">
+        <v>0.20952592019712854</v>
+      </c>
+      <c r="Y17" s="40">
+        <v>-1.2304793821296529E-2</v>
+      </c>
+      <c r="Z17" s="40">
+        <v>5.409966048796308E-2</v>
+      </c>
+      <c r="AA17" s="40">
+        <v>-1.2304793821296529E-2</v>
+      </c>
+      <c r="AB17" s="40">
+        <v>5.409966048796308E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>-4.9000000000000002E-2</v>
       </c>
@@ -4765,19 +6252,49 @@
       <c r="C18" s="14">
         <v>2E-3</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="21" cm="1">
-        <f t="array" ref="F18">_xll.RevisedSharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25497722129753936</v>
-      </c>
-      <c r="G18" s="21" cm="1">
-        <f t="array" ref="G18">_xll.RevisedSharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.9459817090002941</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F18" s="8"/>
+      <c r="N18">
+        <v>17</v>
+      </c>
+      <c r="O18" s="26">
+        <f t="shared" si="0"/>
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="P18" s="14">
+        <v>-3.5685999999999996E-2</v>
+      </c>
+      <c r="R18" s="21">
+        <v>1217.13478177716</v>
+      </c>
+      <c r="T18" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="U18" s="41">
+        <v>4.9053153153154153E-5</v>
+      </c>
+      <c r="V18" s="41">
+        <v>7.7002458389716024E-4</v>
+      </c>
+      <c r="W18" s="41">
+        <v>6.3703359839359874E-2</v>
+      </c>
+      <c r="X18" s="41">
+        <v>0.94957948962630323</v>
+      </c>
+      <c r="Y18" s="41">
+        <v>-1.515825079511511E-3</v>
+      </c>
+      <c r="Z18" s="41">
+        <v>1.6139313858178192E-3</v>
+      </c>
+      <c r="AA18" s="41">
+        <v>-1.515825079511511E-3</v>
+      </c>
+      <c r="AB18" s="41">
+        <v>1.6139313858178192E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>-2.1000000000000001E-2</v>
       </c>
@@ -4787,19 +6304,21 @@
       <c r="C19" s="14">
         <v>2E-3</v>
       </c>
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="21" cm="1">
-        <f t="array" ref="F19">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25223719852260701</v>
-      </c>
-      <c r="G19" s="21" cm="1">
-        <f t="array" ref="G19">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.91065390211902919</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>18</v>
+      </c>
+      <c r="O19" s="26">
+        <f t="shared" si="0"/>
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="P19" s="14">
+        <v>-6.8971000000000116E-2</v>
+      </c>
+      <c r="R19" s="21">
+        <v>1157.4951774700792</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>6.2E-2</v>
       </c>
@@ -4810,18 +6329,42 @@
         <v>2E-3</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="1" cm="1">
-        <f t="array" ref="F20">_xll.MSquared(A2:A37,B2:B37,C2:C37,1)</f>
-        <v>1.0565967513977965E-2</v>
-      </c>
-      <c r="G20" s="1" cm="1">
-        <f t="array" ref="G20">_xll.MSquared(A2:A37,B2:B37,C2:C37,12)</f>
-        <v>0.13435614552670944</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F20" s="21" cm="1">
+        <f t="array" ref="F20">_xll.SharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25479695255981605</v>
+      </c>
+      <c r="G20" s="21" cm="1">
+        <f t="array" ref="G20">_xll.SharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.94531290051723404</v>
+      </c>
+      <c r="I20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" t="b" cm="1">
+        <f t="array" ref="J20">AND(ABS(F6:G17-F20:G31)&lt;0.000000001)</f>
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>19</v>
+      </c>
+      <c r="O20" s="26">
+        <f t="shared" si="0"/>
+        <v>6.2E-2</v>
+      </c>
+      <c r="P20" s="14">
+        <v>3.9698000000000011E-2</v>
+      </c>
+      <c r="R20" s="21">
+        <v>1133.1877787432074</v>
+      </c>
+      <c r="U20">
+        <f>U18/V18</f>
+        <v>6.3703359839359874E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>5.7999999999999996E-2</v>
       </c>
@@ -4831,15 +6374,32 @@
       <c r="C21" s="14">
         <v>1E-3</v>
       </c>
-      <c r="E21" t="s">
-        <v>8</v>
+      <c r="E21" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="F21" s="21" cm="1">
-        <f t="array" ref="F21">_xll.Beta(A2:A37,B2:B37)</f>
-        <v>0.98144598446869202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="F21">_xll.RevisedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25497722129753936</v>
+      </c>
+      <c r="G21" s="21" cm="1">
+        <f t="array" ref="G21">_xll.RevisedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.9459817090002941</v>
+      </c>
+      <c r="N21">
+        <v>20</v>
+      </c>
+      <c r="O21" s="26">
+        <f t="shared" si="0"/>
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="P21" s="14">
+        <v>0.12359600000000004</v>
+      </c>
+      <c r="R21" s="21">
+        <v>1203.4454210252864</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>-6.4000000000000001E-2</v>
       </c>
@@ -4850,18 +6410,34 @@
         <v>1E-3</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="F22" s="21" cm="1">
-        <f t="array" ref="F22">_xll.TreynorIndex(A2:A37,F21,C2:C37,1)</f>
-        <v>8.6123733893902332E-3</v>
+        <f t="array" ref="F22">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25223719852260701</v>
       </c>
       <c r="G22" s="21" cm="1">
-        <f t="array" ref="G22">_xll.TreynorIndex(A2:A37,F21,C2:C37,12)</f>
-        <v>0.11068654428760946</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="G22">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.91065390211902919</v>
+      </c>
+      <c r="N22">
+        <v>21</v>
+      </c>
+      <c r="O22" s="26">
+        <f t="shared" si="0"/>
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="P22" s="14">
+        <v>-9.7120000000000539E-3</v>
+      </c>
+      <c r="R22" s="21">
+        <v>1273.245255444753</v>
+      </c>
+      <c r="T22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -4872,22 +6448,31 @@
         <v>1E-3</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1" cm="1">
-        <f t="array" ref="F23">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,1)</f>
-        <v>-8.089957684054485E-4</v>
+        <f t="array" ref="F23">_xll.MSquared(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>1.0565967513977965E-2</v>
       </c>
       <c r="G23" s="1" cm="1">
-        <f t="array" ref="G23">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,12)</f>
-        <v>-1.1048559174976394E-2</v>
-      </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="G23">_xll.MSquared(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>0.13435614552670944</v>
+      </c>
+      <c r="N23">
+        <v>22</v>
+      </c>
+      <c r="O23" s="26">
+        <f t="shared" si="0"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P23" s="14">
+        <v>-4.8088000000000131E-2</v>
+      </c>
+      <c r="R23" s="21">
+        <v>1191.7575590962888</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>-4.0000000000000001E-3</v>
       </c>
@@ -4898,15 +6483,31 @@
         <v>1E-3</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24" s="8" cm="1">
-        <f t="array" ref="F24">_xll.AppraisalRatio($A$2:$A$37,$B$2:$B$37,$C$2:$C$37,1)</f>
-        <v>-0.23629010561291894</v>
-      </c>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="F24" s="21" cm="1">
+        <f t="array" ref="F24">_xll.Beta(A2:A37,B2:B37)</f>
+        <v>0.98144598446869213</v>
+      </c>
+      <c r="N24">
+        <v>23</v>
+      </c>
+      <c r="O24" s="26">
+        <f t="shared" si="0"/>
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="P24" s="14">
+        <v>1.2931999999999944E-2</v>
+      </c>
+      <c r="R24" s="21">
+        <v>1212.0174376009256</v>
+      </c>
+      <c r="T24" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="U24" s="43"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>-2E-3</v>
       </c>
@@ -4917,14 +6518,37 @@
         <v>1E-3</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="8" cm="1">
-        <f t="array" ref="F25">_xll.SemiVariance(A2:A37)</f>
-        <v>5.83888888888889E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="F25" s="21" cm="1">
+        <f t="array" ref="F25">_xll.TreynorIndex(A2:A37,F24,C2:C37,1)</f>
+        <v>8.6123733893902314E-3</v>
+      </c>
+      <c r="G25" s="21" cm="1">
+        <f t="array" ref="G25">_xll.TreynorIndex(A2:A37,F24,C2:C37,12)</f>
+        <v>0.11068654428760945</v>
+      </c>
+      <c r="N25">
+        <v>24</v>
+      </c>
+      <c r="O25" s="26">
+        <f t="shared" si="0"/>
+        <v>-2E-3</v>
+      </c>
+      <c r="P25" s="14">
+        <v>-5.9919999999999973E-3</v>
+      </c>
+      <c r="R25" s="21">
+        <v>1207.1693678505219</v>
+      </c>
+      <c r="T25" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="U25" s="40">
+        <v>0.87798755875532652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>-2.1000000000000001E-2</v>
       </c>
@@ -4935,56 +6559,161 @@
         <v>1E-3</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="8" cm="1">
-        <f t="array" ref="F26">_xll.SemiDeviation(A2:A37)</f>
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" cm="1">
+        <f t="array" ref="F26">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>-8.0899576840545023E-4</v>
+      </c>
+      <c r="G26" s="1" cm="1">
+        <f t="array" ref="G26">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>-1.1048559174976408E-2</v>
+      </c>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="N26">
+        <v>25</v>
+      </c>
+      <c r="O26" s="26">
+        <f t="shared" si="0"/>
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="P26" s="14">
+        <v>-2.2958000000000034E-2</v>
+      </c>
+      <c r="R26" s="21">
+        <v>1204.7550291148209</v>
+      </c>
+      <c r="T26" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="U26" s="40">
+        <v>0.77086215332913799</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B27" s="32">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="8" cm="1">
+        <f t="array" ref="F27">_xll.AppraisalRatio($A$2:$A$37,$B$2:$B$37,$C$2:$C$37,1)</f>
+        <v>-0.23629010561292166</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="N27">
+        <v>26</v>
+      </c>
+      <c r="O27" s="26">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="P27" s="14">
+        <v>-1.0231000000000101E-2</v>
+      </c>
+      <c r="R27" s="21">
+        <v>1179.4551735034097</v>
+      </c>
+      <c r="T27" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="U27" s="40">
+        <v>0.7643153577099705</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B28" s="32">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" s="8" cm="1">
+        <f t="array" ref="F28">_xll.SemiVariance(A2:A37)</f>
+        <v>5.83888888888889E-4</v>
+      </c>
+      <c r="N28">
+        <v>27</v>
+      </c>
+      <c r="O28" s="26">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="P28" s="14">
+        <v>5.851699999999993E-2</v>
+      </c>
+      <c r="R28" s="21">
+        <v>1192.4291804119471</v>
+      </c>
+      <c r="T28" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="U28" s="40">
+        <v>60.139733692262261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B29" s="32">
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="8" cm="1">
+        <f t="array" ref="F29">_xll.SemiDeviation(A2:A37)</f>
         <v>2.4163792932585915E-2</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J29" s="1">
         <f>_xlfn.VAR.P(B2:B37)*12*F10^2</f>
         <v>1.3065336093908721E-2</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K29" s="14">
         <f>F10*_xlfn.STDEV.P(B2:B37)</f>
         <v>3.2996636310777601E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <v>1.1000000000000001E-2</v>
-      </c>
-      <c r="B27" s="32">
-        <v>6.9999999999999993E-3</v>
-      </c>
-      <c r="C27" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="F27" s="35"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <v>4.7E-2</v>
-      </c>
-      <c r="B28" s="32">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="C28" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="N29">
+        <v>28</v>
+      </c>
+      <c r="O29" s="26">
+        <f t="shared" si="0"/>
         <v>2.4E-2</v>
       </c>
-      <c r="B29" s="32">
-        <v>2.8999999999999998E-2</v>
-      </c>
-      <c r="C29" s="14">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P29" s="14">
+        <v>7.212799999999997E-2</v>
+      </c>
+      <c r="R29" s="21">
+        <v>1248.4733518913085</v>
+      </c>
+      <c r="T29" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="U29" s="41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -4994,8 +6723,28 @@
       <c r="C30" s="14">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="8" cm="1">
+        <f t="array" ref="F30">_xll.UpperPartialMoment(A2:A37,,2,1)</f>
+        <v>5.1661111111111103E-4</v>
+      </c>
+      <c r="N30">
+        <v>29</v>
+      </c>
+      <c r="O30" s="26">
+        <f t="shared" si="0"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="P30" s="14">
+        <v>5.7791999999999843E-2</v>
+      </c>
+      <c r="R30" s="21">
+        <v>1278.4367123366999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
         <v>-6.9999999999999993E-3</v>
       </c>
@@ -5006,145 +6755,430 @@
         <v>2E-3</v>
       </c>
       <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="8">
+        <f>SQRT(F30)</f>
+        <v>2.2729080736165089E-2</v>
+      </c>
+      <c r="N31">
+        <v>30</v>
+      </c>
+      <c r="O31" s="26">
+        <f t="shared" si="0"/>
+        <v>-6.9999999999999993E-3</v>
+      </c>
+      <c r="P31" s="14">
+        <v>2.5768999999999931E-2</v>
+      </c>
+      <c r="R31" s="21">
+        <v>1320.6251238438108</v>
+      </c>
+      <c r="T31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B32" s="32">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C32" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="8" cm="1">
+        <f t="array" ref="F32">_xll.KRatio(A2:A37)</f>
+        <v>0.16768620342592805</v>
+      </c>
+      <c r="N32">
+        <v>31</v>
+      </c>
+      <c r="O32" s="26">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="P32" s="14">
+        <v>3.9671000000000012E-2</v>
+      </c>
+      <c r="R32" s="21">
+        <v>1311.3807479769041</v>
+      </c>
+      <c r="T32" s="42"/>
+      <c r="U32" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="V32" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="W32" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="X32" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y32" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B33" s="32">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C33" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="N33">
+        <v>32</v>
+      </c>
+      <c r="O33" s="26">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P33" s="14">
+        <v>5.3281999999999829E-2</v>
+      </c>
+      <c r="R33" s="21">
+        <v>1373.0156431318185</v>
+      </c>
+      <c r="T33" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="U33" s="40">
+        <v>1</v>
+      </c>
+      <c r="V33" s="40">
+        <v>425864.01278267859</v>
+      </c>
+      <c r="W33" s="40">
+        <v>425864.01278267859</v>
+      </c>
+      <c r="X33" s="40">
+        <v>117.74648212206812</v>
+      </c>
+      <c r="Y33" s="40">
+        <v>9.5848430684232274E-13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="B34" s="32">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="C34" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="N34">
+        <v>33</v>
+      </c>
+      <c r="O34" s="26">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="P34" s="14">
+        <v>1.6059999999999963E-2</v>
+      </c>
+      <c r="R34" s="21">
+        <v>1381.2537369906095</v>
+      </c>
+      <c r="T34" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="U34" s="40">
+        <v>35</v>
+      </c>
+      <c r="V34" s="40">
+        <v>126587.56490016784</v>
+      </c>
+      <c r="W34" s="40">
+        <v>3616.7875685762242</v>
+      </c>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
+    </row>
+    <row r="35" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>-2E-3</v>
+      </c>
+      <c r="B35" s="32">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C35" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="N35">
+        <v>34</v>
+      </c>
+      <c r="O35" s="26">
+        <f t="shared" si="0"/>
+        <v>-2E-3</v>
+      </c>
+      <c r="P35" s="14">
+        <v>7.9800000000000981E-3</v>
+      </c>
+      <c r="R35" s="21">
+        <v>1395.0662743605155</v>
+      </c>
+      <c r="T35" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="U35" s="41">
+        <v>36</v>
+      </c>
+      <c r="V35" s="41">
+        <v>552451.57768284646</v>
+      </c>
+      <c r="W35" s="41"/>
+      <c r="X35" s="41"/>
+      <c r="Y35" s="41"/>
+    </row>
+    <row r="36" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B36" s="32">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C36" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="N36">
+        <v>35</v>
+      </c>
+      <c r="O36" s="26">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="P36" s="14">
+        <v>3.1932000000000071E-2</v>
+      </c>
+      <c r="R36" s="21">
+        <v>1392.2761418117946</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="B37" s="32">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C37" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="N37">
+        <v>36</v>
+      </c>
+      <c r="O37" s="26">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="P37" s="14">
+        <v>4.4340000000000046E-2</v>
+      </c>
+      <c r="R37" s="21">
+        <v>1439.6135306333956</v>
+      </c>
+      <c r="T37" s="42"/>
+      <c r="U37" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="V37" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="W37" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="X37" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y37" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z37" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA37" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB37" s="42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
         <v>83</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F38" s="1">
         <f>_xlfn.VAR.P(A2:A37)</f>
         <v>1.1005000000000001E-3</v>
       </c>
-      <c r="G31" s="1">
-        <f>SQRT(F31*12)</f>
+      <c r="G38" s="1">
+        <f>SQRT(F38*12)</f>
         <v>0.11491736161259535</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
-        <v>4.7E-2</v>
-      </c>
-      <c r="B32" s="32">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="C32" s="14">
-        <v>2E-3</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="N38">
+        <v>37</v>
+      </c>
+      <c r="R38" s="21">
+        <v>1454.0096659397295</v>
+      </c>
+      <c r="T38" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="U38" s="40">
+        <v>1020.5103479428813</v>
+      </c>
+      <c r="V38" s="40">
+        <v>20.181573213260343</v>
+      </c>
+      <c r="W38" s="40">
+        <v>50.566441830825802</v>
+      </c>
+      <c r="X38" s="40">
+        <v>2.5839067739645967E-34</v>
+      </c>
+      <c r="Y38" s="40">
+        <v>979.53957615807667</v>
+      </c>
+      <c r="Z38" s="40">
+        <v>1061.4811197276858</v>
+      </c>
+      <c r="AA38" s="40">
+        <v>979.53957615807667</v>
+      </c>
+      <c r="AB38" s="40">
+        <v>1061.4811197276858</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
         <v>84</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F39" s="1">
         <f>_xlfn.VAR.P(B2:B37)</f>
         <v>1.1303333333333335E-3</v>
       </c>
-      <c r="G32" s="1">
-        <f>F32*12</f>
+      <c r="G39" s="1">
+        <f>F39*12</f>
         <v>1.3564000000000001E-2</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J39" s="1">
         <f>F10^2*_xlfn.VAR.P(B2:B37)</f>
         <v>1.0887780078257267E-3</v>
       </c>
-      <c r="K32">
-        <f>SQRT(J32)</f>
+      <c r="K39">
+        <f>SQRT(J39)</f>
         <v>3.2996636310777601E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="B33" s="32">
-        <v>1.3999999999999999E-2</v>
-      </c>
-      <c r="C33" s="14">
-        <v>2E-3</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="T39" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="U39" s="41">
+        <v>10.048059157673292</v>
+      </c>
+      <c r="V39" s="41">
+        <v>0.92599408587651855</v>
+      </c>
+      <c r="W39" s="41">
+        <v>10.851105110635881</v>
+      </c>
+      <c r="X39" s="41">
+        <v>9.5848430684231911E-13</v>
+      </c>
+      <c r="Y39" s="41">
+        <v>8.1681912224224416</v>
+      </c>
+      <c r="Z39" s="41">
+        <v>11.927927092924142</v>
+      </c>
+      <c r="AA39" s="41">
+        <v>8.1681912224224416</v>
+      </c>
+      <c r="AB39" s="41">
+        <v>11.927927092924142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
         <v>85</v>
       </c>
-      <c r="F33" s="1">
-        <f>F10^2*F32</f>
+      <c r="F40" s="1">
+        <f>F10^2*F39</f>
         <v>1.0887780078257267E-3</v>
       </c>
-      <c r="G33" s="14">
-        <f>SQRT(F33)</f>
+      <c r="G40" s="14">
+        <f>SQRT(F40)</f>
         <v>3.2996636310777601E-2</v>
       </c>
-      <c r="H33" s="1" cm="1">
-        <f t="array" ref="H33">SQRT(_xll.MarketRisk(A2:A37,B2:B37,1))</f>
+      <c r="H40" s="1" cm="1">
+        <f t="array" ref="H40">SQRT(_xll.MarketRisk(A2:A37,B2:B37,1))</f>
         <v>3.2996636310777601E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="B34" s="32">
-        <v>1.3000000000000001E-2</v>
-      </c>
-      <c r="C34" s="14">
-        <v>2E-3</v>
-      </c>
-      <c r="E34" t="s">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
         <v>86</v>
       </c>
-      <c r="F34" s="1">
-        <f>F31-F10^2*F32</f>
+      <c r="F41" s="1">
+        <f>F38-F10^2*F39</f>
         <v>1.1721992174273423E-5</v>
       </c>
-      <c r="G34" s="1">
-        <f>SQRT(F34)</f>
+      <c r="G41" s="1">
+        <f>SQRT(F41)</f>
         <v>3.4237395015207311E-3</v>
       </c>
-      <c r="H34" s="1" cm="1">
-        <f t="array" ref="H34">_xll.UniqueRisk(A2:A37,B2:B37,1)</f>
-        <v>1.1721992174273206E-5</v>
-      </c>
-      <c r="I34">
-        <f>SQRT(H34)</f>
-        <v>3.4237395015206994E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
-        <v>-2E-3</v>
-      </c>
-      <c r="B35" s="32">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C35" s="14">
-        <v>2E-3</v>
-      </c>
-      <c r="H35" s="11">
-        <f>SUM(H33:H34)</f>
+      <c r="H41" s="1" cm="1">
+        <f t="array" ref="H41">_xll.UniqueRisk(A2:A37,B2:B37,1)</f>
+        <v>1.1721992174272989E-5</v>
+      </c>
+      <c r="I41">
+        <f>SQRT(H41)</f>
+        <v>3.4237395015206673E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="H42" s="11">
+        <f>SUM(H40:H41)</f>
         <v>3.3008358302951873E-2</v>
       </c>
-      <c r="I35">
-        <f>SQRT(H35)</f>
+      <c r="I42">
+        <f>SQRT(H42)</f>
         <v>0.18168202526103641</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="B36" s="32">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="C36" s="14">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
-        <v>0.01</v>
-      </c>
-      <c r="B37" s="32">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="C37" s="14">
-        <v>2E-3</v>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U43">
+        <f>U39/U28</f>
+        <v>0.16707854426309343</v>
+      </c>
+      <c r="V43" s="35">
+        <f>_xlfn.COVARIANCE.P(_xlfn.ANCHORARRAY(R2),_xlfn.ANCHORARRAY(N2))/_xlfn.VAR.P(_xlfn.ANCHORARRAY(N2))</f>
+        <v>10.048059157673293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U45" s="35">
+        <f>STEYX(_xlfn.ANCHORARRAY(R2),_xlfn.ANCHORARRAY(N2))/SQRT(DEVSQ(_xlfn.ANCHORARRAY(N2)))</f>
+        <v>0.9259940858765181</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F20:G32">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ABS(F20:G32-F6:G17) &gt; 0.0000000001</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -5665,8 +7699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1041C9-4B35-43C1-9DE0-DEF26697FEC8}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5794,4 +7828,1029 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F12073D-9724-4911-AFA1-DE839FEC917E}">
+  <dimension ref="A1:Z43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" cm="1">
+        <f t="array" ref="A2:A21">_xlfn.SEQUENCE(20)</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>$S$17+$S$18*A2</f>
+        <v>-1.67000000000001E-3</v>
+      </c>
+      <c r="I2" s="26">
+        <f>B2-H2</f>
+        <v>1.67000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="D3" s="14">
+        <f>(1+B3)/(1+B2)-1</f>
+        <v>-1.4999999999999458E-3</v>
+      </c>
+      <c r="E3">
+        <f>E2*(1+D3)</f>
+        <v>99.850000000000009</v>
+      </c>
+      <c r="F3" s="14">
+        <f>(1+F2)*(1+D3)-1</f>
+        <v>-1.4999999999999458E-3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H21" si="0">$S$17+$S$18*A3</f>
+        <v>4.1357894736842003E-3</v>
+      </c>
+      <c r="I3" s="26">
+        <f t="shared" ref="I3:I21" si="1">B3-H3</f>
+        <v>-5.6357894736841999E-3</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="S3" s="43"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="D4" s="14">
+        <f>(1+B4)/(1+B3)-1</f>
+        <v>8.7130696044066536E-3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E21" si="2">E3*(1+D4)</f>
+        <v>100.72000000000001</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" ref="F4:F21" si="3">(1+F3)*(1+D4)-1</f>
+        <v>7.2000000000000952E-3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>9.9415789473684124E-3</v>
+      </c>
+      <c r="I4" s="26">
+        <f t="shared" si="1"/>
+        <v>-2.7415789473684126E-3</v>
+      </c>
+      <c r="R4" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="S4" s="40">
+        <v>0.98736178085940562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1.23E-2</v>
+      </c>
+      <c r="D5" s="14">
+        <f t="shared" ref="D5:D21" si="4">(1+B5)/(1+B4)-1</f>
+        <v>5.0635424940428386E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>101.23</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="3"/>
+        <v>1.2299999999999978E-2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.5747368421052621E-2</v>
+      </c>
+      <c r="I5" s="26">
+        <f t="shared" si="1"/>
+        <v>-3.4473684210526209E-3</v>
+      </c>
+      <c r="R5" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="40">
+        <v>0.97488328630185694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D6" s="14">
+        <f t="shared" si="4"/>
+        <v>1.2545688037143066E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>102.5</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="3"/>
+        <v>2.4999999999999911E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>2.155315789473683E-2</v>
+      </c>
+      <c r="I6" s="26">
+        <f t="shared" si="1"/>
+        <v>3.4468421052631718E-3</v>
+      </c>
+      <c r="R6" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="S6" s="40">
+        <v>0.97348791331862672</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" si="4"/>
+        <v>-1.6585365853656331E-3</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>102.33000000000003</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="3"/>
+        <v>2.3300000000000098E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2.7358947368421045E-2</v>
+      </c>
+      <c r="I7" s="26">
+        <f t="shared" si="1"/>
+        <v>-4.0589473684210439E-3</v>
+      </c>
+      <c r="R7" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="S7" s="40">
+        <v>5.6642309006524841E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="D8" s="14">
+        <f t="shared" si="4"/>
+        <v>2.0521841102316696E-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>102.54000000000003</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="3"/>
+        <v>2.5400000000000089E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>3.3164736842105254E-2</v>
+      </c>
+      <c r="I8" s="26">
+        <f t="shared" si="1"/>
+        <v>-7.7647368421052548E-3</v>
+      </c>
+      <c r="R8" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="S8" s="41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="D9" s="14">
+        <f t="shared" si="4"/>
+        <v>1.0629998049541456E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>103.63000000000001</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="3"/>
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>3.8970526315789462E-2</v>
+      </c>
+      <c r="I9" s="26">
+        <f t="shared" si="1"/>
+        <v>-2.6705263157894635E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>4.9100000000000005E-2</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="4"/>
+        <v>1.2351635626749013E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>104.91000000000001</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="3"/>
+        <v>4.9099999999999921E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>4.4776315789473671E-2</v>
+      </c>
+      <c r="I10" s="26">
+        <f t="shared" si="1"/>
+        <v>4.3236842105263337E-3</v>
+      </c>
+      <c r="R10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D11" s="14">
+        <f t="shared" si="4"/>
+        <v>1.2772852921551836E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>106.25000000000001</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>5.058210526315788E-2</v>
+      </c>
+      <c r="I11" s="26">
+        <f t="shared" si="1"/>
+        <v>1.191789473684212E-2</v>
+      </c>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="T11" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="U11" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="V11" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="W11" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14">
+        <v>6.3200000000000006E-2</v>
+      </c>
+      <c r="D12" s="14">
+        <f t="shared" si="4"/>
+        <v>6.5882352941160072E-4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>106.32</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="3"/>
+        <v>6.3199999999999923E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>5.6387894736842088E-2</v>
+      </c>
+      <c r="I12" s="26">
+        <f t="shared" si="1"/>
+        <v>6.8121052631579179E-3</v>
+      </c>
+      <c r="R12" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="S12" s="40">
+        <v>1</v>
+      </c>
+      <c r="T12" s="40">
+        <v>2.2415282289473679E-2</v>
+      </c>
+      <c r="U12" s="40">
+        <v>2.2415282289473679E-2</v>
+      </c>
+      <c r="V12" s="40">
+        <v>698.6542652166612</v>
+      </c>
+      <c r="W12" s="40">
+        <v>7.4628755475986974E-16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D13" s="14">
+        <f t="shared" si="4"/>
+        <v>2.6335590669677167E-3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>106.6</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="3"/>
+        <v>6.6000000000000059E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>6.2193684210526311E-2</v>
+      </c>
+      <c r="I13" s="26">
+        <f t="shared" si="1"/>
+        <v>3.8063157894736924E-3</v>
+      </c>
+      <c r="R13" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="S13" s="40">
+        <v>18</v>
+      </c>
+      <c r="T13" s="40">
+        <v>5.7750321052631626E-4</v>
+      </c>
+      <c r="U13" s="40">
+        <v>3.2083511695906456E-5</v>
+      </c>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="D14" s="14">
+        <f t="shared" si="4"/>
+        <v>1.4071294559097058E-3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>106.74999999999997</v>
+      </c>
+      <c r="F14" s="14">
+        <f t="shared" si="3"/>
+        <v>6.7499999999999893E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>6.7999473684210526E-2</v>
+      </c>
+      <c r="I14" s="26">
+        <f t="shared" si="1"/>
+        <v>-4.9947368421052185E-4</v>
+      </c>
+      <c r="R14" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="S14" s="41">
+        <v>19</v>
+      </c>
+      <c r="T14" s="41">
+        <v>2.2992785499999994E-2</v>
+      </c>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14">
+        <v>7.9199999999999993E-2</v>
+      </c>
+      <c r="D15" s="14">
+        <f t="shared" si="4"/>
+        <v>1.0960187353630024E-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>107.91999999999997</v>
+      </c>
+      <c r="F15" s="14">
+        <f t="shared" si="3"/>
+        <v>7.9199999999999937E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>7.3805263157894735E-2</v>
+      </c>
+      <c r="I15" s="26">
+        <f t="shared" si="1"/>
+        <v>5.3947368421052577E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D16" s="14">
+        <f t="shared" si="4"/>
+        <v>3.5211267605634866E-3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>108.29999999999998</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="3"/>
+        <v>8.2999999999999963E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>7.9611052631578944E-2</v>
+      </c>
+      <c r="I16" s="26">
+        <f t="shared" si="1"/>
+        <v>3.3889473684210608E-3</v>
+      </c>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="T16" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="U16" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="V16" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="W16" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="X16" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y16" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z16" s="42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" si="4"/>
+        <v>6.4635272391506682E-3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="F17" s="14">
+        <f t="shared" si="3"/>
+        <v>9.000000000000008E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>8.5416842105263152E-2</v>
+      </c>
+      <c r="I17" s="26">
+        <f t="shared" si="1"/>
+        <v>4.5831578947368445E-3</v>
+      </c>
+      <c r="R17" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="S17" s="40">
+        <v>-7.4757894736842204E-3</v>
+      </c>
+      <c r="T17" s="40">
+        <v>2.631213427831514E-3</v>
+      </c>
+      <c r="U17" s="40">
+        <v>-2.8411946346159045</v>
+      </c>
+      <c r="V17" s="40">
+        <v>1.0835016469266913E-2</v>
+      </c>
+      <c r="W17" s="40">
+        <v>-1.3003763756793619E-2</v>
+      </c>
+      <c r="X17" s="40">
+        <v>-1.947815190574821E-3</v>
+      </c>
+      <c r="Y17" s="40">
+        <v>-1.3003763756793619E-2</v>
+      </c>
+      <c r="Z17" s="40">
+        <v>-1.947815190574821E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14">
+        <v>9.2200000000000004E-2</v>
+      </c>
+      <c r="D18" s="14">
+        <f t="shared" si="4"/>
+        <v>2.0183486238531945E-3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>109.22</v>
+      </c>
+      <c r="F18" s="14">
+        <f t="shared" si="3"/>
+        <v>9.220000000000006E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>9.1222631578947361E-2</v>
+      </c>
+      <c r="I18" s="26">
+        <f t="shared" si="1"/>
+        <v>9.7736842105264343E-4</v>
+      </c>
+      <c r="R18" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="S18" s="41">
+        <v>5.8057894736842103E-3</v>
+      </c>
+      <c r="T18" s="41">
+        <v>2.1964945310535921E-4</v>
+      </c>
+      <c r="U18" s="41">
+        <v>26.43206887885739</v>
+      </c>
+      <c r="V18" s="41">
+        <v>7.4628755475986974E-16</v>
+      </c>
+      <c r="W18" s="41">
+        <v>5.3443230965282713E-3</v>
+      </c>
+      <c r="X18" s="41">
+        <v>6.2672558508401494E-3</v>
+      </c>
+      <c r="Y18" s="41">
+        <v>5.3443230965282713E-3</v>
+      </c>
+      <c r="Z18" s="41">
+        <v>6.2672558508401494E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14">
+        <v>9.3599999999999989E-2</v>
+      </c>
+      <c r="D19" s="14">
+        <f t="shared" si="4"/>
+        <v>1.2818165171213369E-3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>109.35999999999999</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="3"/>
+        <v>9.3599999999999905E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>9.7028421052631569E-2</v>
+      </c>
+      <c r="I19" s="26">
+        <f t="shared" si="1"/>
+        <v>-3.4284210526315806E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="14">
+        <v>9.3699999999999992E-2</v>
+      </c>
+      <c r="D20" s="14">
+        <f t="shared" si="4"/>
+        <v>9.1441111923939999E-5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>109.36999999999999</v>
+      </c>
+      <c r="F20" s="14">
+        <f t="shared" si="3"/>
+        <v>9.3699999999999894E-2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.10283421052631578</v>
+      </c>
+      <c r="I20" s="26">
+        <f t="shared" si="1"/>
+        <v>-9.1342105263157863E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="14">
+        <v>0.1017</v>
+      </c>
+      <c r="D21" s="14">
+        <f t="shared" si="4"/>
+        <v>7.3146200969187447E-3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>110.16999999999999</v>
+      </c>
+      <c r="F21" s="14">
+        <f t="shared" si="3"/>
+        <v>0.1016999999999999</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.10863999999999999</v>
+      </c>
+      <c r="I21" s="26">
+        <f t="shared" si="1"/>
+        <v>-6.9399999999999878E-3</v>
+      </c>
+      <c r="T21">
+        <f>U18/SQRT(20)</f>
+        <v>5.9103902799081771</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>SLOPE(B2:B21,_xlfn.ANCHORARRAY(A2))*SQRT(DEVSQ(_xlfn.ANCHORARRAY(A2)))/STEYX(B2:B21,_xlfn.ANCHORARRAY(A2))/SQRT(20)</f>
+        <v>5.9103902799082544</v>
+      </c>
+      <c r="D23" s="14" cm="1">
+        <f t="array" ref="D23">_xll.KRatio(D2:D21)</f>
+        <v>1.0804360835735838</v>
+      </c>
+      <c r="E23">
+        <f>SLOPE(E2:E21,_xlfn.ANCHORARRAY(A2))*SQRT(DEVSQ(_xlfn.ANCHORARRAY(A2)))/STEYX(E2:E21,_xlfn.ANCHORARRAY(A2))/SQRT(20)</f>
+        <v>5.9103902799081878</v>
+      </c>
+      <c r="R23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="44">
+        <f>INTERCEPT(F2:F21,_xlfn.ANCHORARRAY(A2))</f>
+        <v>-7.4757894736841718E-3</v>
+      </c>
+      <c r="R25" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="S25" s="43"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="44">
+        <f>SLOPE(F2:F21,_xlfn.ANCHORARRAY(A2))</f>
+        <v>5.8057894736842051E-3</v>
+      </c>
+      <c r="R26" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="S26" s="40">
+        <v>0.98736178085940574</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="44" cm="1">
+        <f t="array" ref="D27">SUM(I2:I21^2)</f>
+        <v>5.7750321052631615E-4</v>
+      </c>
+      <c r="R27" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="S27" s="40">
+        <v>0.97488328630185705</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R28" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="S28" s="40">
+        <v>0.97348791331862694</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R29" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="S29" s="40">
+        <v>0.56642309006524494</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R30" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="S30" s="41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="18:26" x14ac:dyDescent="0.25">
+      <c r="R33" s="42"/>
+      <c r="S33" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="T33" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="U33" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="V33" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="W33" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="18:26" x14ac:dyDescent="0.25">
+      <c r="R34" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="S34" s="40">
+        <v>1</v>
+      </c>
+      <c r="T34" s="40">
+        <v>224.15282289473561</v>
+      </c>
+      <c r="U34" s="40">
+        <v>224.15282289473561</v>
+      </c>
+      <c r="V34" s="40">
+        <v>698.65426521666598</v>
+      </c>
+      <c r="W34" s="40">
+        <v>7.4628755475982725E-16</v>
+      </c>
+    </row>
+    <row r="35" spans="18:26" x14ac:dyDescent="0.25">
+      <c r="R35" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="S35" s="40">
+        <v>18</v>
+      </c>
+      <c r="T35" s="40">
+        <v>5.775032105263092</v>
+      </c>
+      <c r="U35" s="40">
+        <v>0.32083511695906064</v>
+      </c>
+      <c r="V35" s="40"/>
+      <c r="W35" s="40"/>
+    </row>
+    <row r="36" spans="18:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R36" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="S36" s="41">
+        <v>19</v>
+      </c>
+      <c r="T36" s="41">
+        <v>229.92785499999869</v>
+      </c>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+    </row>
+    <row r="37" spans="18:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="18:26" x14ac:dyDescent="0.25">
+      <c r="R38" s="42"/>
+      <c r="S38" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="T38" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="U38" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="V38" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="W38" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="X38" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y38" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z38" s="42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="18:26" x14ac:dyDescent="0.25">
+      <c r="R39" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="S39" s="40">
+        <v>99.25242105263159</v>
+      </c>
+      <c r="T39" s="40">
+        <v>0.26312134278314986</v>
+      </c>
+      <c r="U39" s="40">
+        <v>377.21159371868202</v>
+      </c>
+      <c r="V39" s="40">
+        <v>1.5371890743051605E-36</v>
+      </c>
+      <c r="W39" s="40">
+        <v>98.699623624320651</v>
+      </c>
+      <c r="X39" s="40">
+        <v>99.805218480942528</v>
+      </c>
+      <c r="Y39" s="40">
+        <v>98.699623624320651</v>
+      </c>
+      <c r="Z39" s="40">
+        <v>99.805218480942528</v>
+      </c>
+    </row>
+    <row r="40" spans="18:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R40" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="S40" s="41">
+        <v>0.58057894736841931</v>
+      </c>
+      <c r="T40" s="41">
+        <v>2.1964945310535788E-2</v>
+      </c>
+      <c r="U40" s="41">
+        <v>26.432068878857468</v>
+      </c>
+      <c r="V40" s="41">
+        <v>7.4628755475982725E-16</v>
+      </c>
+      <c r="W40" s="41">
+        <v>0.53443230965282562</v>
+      </c>
+      <c r="X40" s="41">
+        <v>0.62672558508401299</v>
+      </c>
+      <c r="Y40" s="41">
+        <v>0.53443230965282562</v>
+      </c>
+      <c r="Z40" s="41">
+        <v>0.62672558508401299</v>
+      </c>
+    </row>
+    <row r="43" spans="18:26" x14ac:dyDescent="0.25">
+      <c r="U43">
+        <f>U40/SQRT(20)</f>
+        <v>5.9103902799081949</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fix in LPM and UPM Fixed bug in the way that lower partial moments and upper partial moments were being calculated. Specifically, the code wasn't ignoring values above (or below) the target return. Instead, it was setting them to 0. This affected the calculations when degree was 0.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249F9969-9241-4222-8BE0-214A99BD5338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053D96A0-C9EB-4904-9EFE-E6281D70B3DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9435" yWindow="5010" windowWidth="27480" windowHeight="15990" activeTab="4" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -721,28 +721,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -5474,8 +5453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD720BF-B3A2-4768-8CA5-EE00905CFCE9}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7175,7 +7154,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F20:G32">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>ABS(F20:G32-F6:G17) &gt; 0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Roy's Safety First ratio and updated docs
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053D96A0-C9EB-4904-9EFE-E6281D70B3DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCB2DF0-B7BE-484E-8D76-D29BF3E60827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9435" yWindow="5010" windowWidth="27480" windowHeight="15990" activeTab="4" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{5CCAA0DA-5FA8-4FC8-B47B-DA427260DD08}">
+    <comment ref="G24" authorId="0" shapeId="0" xr:uid="{5CCAA0DA-5FA8-4FC8-B47B-DA427260DD08}">
       <text>
         <r>
           <rPr>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="127">
   <si>
     <t>RFR</t>
   </si>
@@ -540,6 +540,12 @@
   </si>
   <si>
     <t>Sem--deviation Above Mean</t>
+  </si>
+  <si>
+    <t>Minimum Target Return</t>
+  </si>
+  <si>
+    <t>Roy Ratio (Safety First)</t>
   </si>
 </sst>
 </file>
@@ -721,7 +727,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5453,8 +5473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD720BF-B3A2-4768-8CA5-EE00905CFCE9}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5665,6 +5685,20 @@
       <c r="C5" s="14">
         <v>2E-3</v>
       </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G5" s="1">
+        <f>(1+F5)^12-1</f>
+        <v>6.1677811864497611E-2</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
       <c r="N5">
         <v>4</v>
       </c>
@@ -5695,17 +5729,6 @@
       <c r="C6" s="14">
         <v>2E-3</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="21">
-        <f>(F3-L3)/F4</f>
-        <v>0.25479695255981605</v>
-      </c>
-      <c r="G6" s="21">
-        <f>(G3-M3)/G4</f>
-        <v>0.94531290051723404</v>
-      </c>
       <c r="N6">
         <v>5</v>
       </c>
@@ -5736,20 +5759,16 @@
       <c r="C7" s="14">
         <v>2E-3</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="21" cm="1">
-        <f t="array" ref="F7">(F3-L3)/_xlfn.STDEV.P(A2:A37-C2:C37)</f>
-        <v>0.25497722129753936</v>
-      </c>
-      <c r="G7" s="21" cm="1">
-        <f t="array" ref="G7">(G3-M3)/(_xlfn.STDEV.P(A2:A37-C2:C37)*SQRT(12))</f>
-        <v>0.9459817090002941</v>
-      </c>
-      <c r="J7">
-        <f>_xlfn.VAR.P(B2:B37)</f>
-        <v>1.1303333333333335E-3</v>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="21">
+        <f>(F3-L3)/F4</f>
+        <v>0.25479695255981605</v>
+      </c>
+      <c r="G7" s="21">
+        <f>(G3-M3)/G4</f>
+        <v>0.94531290051723404</v>
       </c>
       <c r="N7">
         <v>6</v>
@@ -5781,18 +5800,21 @@
       <c r="C8" s="14">
         <v>2E-3</v>
       </c>
-      <c r="E8" t="s">
-        <v>69</v>
+      <c r="E8" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="F8" s="21" cm="1">
-        <f t="array" ref="F8">F6+_xll.Skewness_P(A2:A37)/6*F6^2-(_xll.Kurtosis_P(A2:A37)-3)/24*F6^3</f>
-        <v>0.25223719852260701</v>
-      </c>
-      <c r="G8" s="27" cm="1">
-        <f t="array" ref="G8">G6+_xll.Skewness_P(A2:A37)/6*G6^2-(_xll.Kurtosis_P(A2:A37)-3)/24*G6^3</f>
-        <v>0.91065390211902919</v>
-      </c>
-      <c r="H8" s="35"/>
+        <f t="array" ref="F8">(F3-L3)/_xlfn.STDEV.P(A2:A37-C2:C37)</f>
+        <v>0.25497722129753936</v>
+      </c>
+      <c r="G8" s="21" cm="1">
+        <f t="array" ref="G8">(G3-M3)/(_xlfn.STDEV.P(A2:A37-C2:C37)*SQRT(12))</f>
+        <v>0.9459817090002941</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.VAR.P(B2:B37)</f>
+        <v>1.1303333333333335E-3</v>
+      </c>
       <c r="N8">
         <v>7</v>
       </c>
@@ -5813,7 +5835,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -5824,16 +5846,17 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="1">
-        <f>F6*_xlfn.STDEV.P($B$2:$B$37)+$L$3</f>
-        <v>1.0565967513977965E-2</v>
-      </c>
-      <c r="G9" s="1">
-        <f>G6*_xlfn.STDEV.P($B$2:$B$37)*SQRT(12)+M3</f>
-        <v>0.13435614552670944</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F9" s="21" cm="1">
+        <f t="array" ref="F9">F7+_xll.Skewness_P(A2:A37)/6*F7^2-(_xll.Kurtosis_P(A2:A37)-3)/24*F7^3</f>
+        <v>0.25223719852260701</v>
+      </c>
+      <c r="G9" s="27" cm="1">
+        <f t="array" ref="G9">G7+_xll.Skewness_P(A2:A37)/6*G7^2-(_xll.Kurtosis_P(A2:A37)-3)/24*G7^3</f>
+        <v>0.91065390211902919</v>
+      </c>
+      <c r="H9" s="35"/>
       <c r="N9">
         <v>8</v>
       </c>
@@ -5848,7 +5871,7 @@
         <v>1086.6184074417049</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>-1.3999999999999999E-2</v>
       </c>
@@ -5859,13 +5882,16 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="21">
-        <f>_xlfn.COVARIANCE.P(A2:A37,B2:B37)/_xlfn.VAR.P(B2:B37)</f>
-        <v>0.98144598446869191</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="F10" s="1">
+        <f>F7*_xlfn.STDEV.P($B$2:$B$37)+$L$3</f>
+        <v>1.0565967513977965E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <f>G7*_xlfn.STDEV.P($B$2:$B$37)*SQRT(12)+M3</f>
+        <v>0.13435614552670944</v>
+      </c>
       <c r="N10">
         <v>9</v>
       </c>
@@ -5894,16 +5920,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="F11" s="21">
-        <f>(F3-L3)/F10</f>
-        <v>8.6123733893902332E-3</v>
-      </c>
-      <c r="G11" s="21">
-        <f>(G3-M3)/F10</f>
-        <v>0.11068654428760948</v>
-      </c>
+        <f>(F3-F5)/F4</f>
+        <v>0.16435156971709106</v>
+      </c>
+      <c r="G11" s="1"/>
       <c r="N11">
         <v>10</v>
       </c>
@@ -5945,17 +5968,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1">
-        <f>F3-L3-F10*(I3-L3)</f>
-        <v>-8.089957684054485E-4</v>
-      </c>
-      <c r="G12" s="1">
-        <f>G3-M3-F10*(J3-M3)</f>
-        <v>-1.104855917497638E-2</v>
-      </c>
-      <c r="I12" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="F12" s="21">
+        <f>_xlfn.COVARIANCE.P(A2:A37,B2:B37)/_xlfn.VAR.P(B2:B37)</f>
+        <v>0.98144598446869191</v>
+      </c>
+      <c r="G12" s="1"/>
       <c r="N12">
         <v>11</v>
       </c>
@@ -5999,11 +6018,15 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="8">
-        <f>F12/SQRT(_xlfn.VAR.P(A2:A37)-F10^2*_xlfn.VAR.P(B2:B37))</f>
-        <v>-0.23629010561291675</v>
+        <v>7</v>
+      </c>
+      <c r="F13" s="21">
+        <f>(F3-L3)/F12</f>
+        <v>8.6123733893902332E-3</v>
+      </c>
+      <c r="G13" s="21">
+        <f>(G3-M3)/F12</f>
+        <v>0.11068654428760948</v>
       </c>
       <c r="N13">
         <v>12</v>
@@ -6044,12 +6067,17 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="8" cm="1">
-        <f t="array" ref="F14">SUM(IF(AVERAGE(A2:A37)-A2:A37&lt;0,0,(AVERAGE(A2:A37)-A2:A37)^2))/COUNT(A2:A37)</f>
-        <v>5.83888888888889E-4</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F14" s="1">
+        <f>F3-L3-F12*(I3-L3)</f>
+        <v>-8.089957684054485E-4</v>
+      </c>
+      <c r="G14" s="1">
+        <f>G3-M3-F12*(J3-M3)</f>
+        <v>-1.104855917497638E-2</v>
+      </c>
+      <c r="I14" s="1"/>
       <c r="N14">
         <v>13</v>
       </c>
@@ -6087,11 +6115,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="F15" s="8">
-        <f>SQRT(F14)</f>
-        <v>2.4163792932585915E-2</v>
+        <f>F14/SQRT(_xlfn.VAR.P(A2:A37)-F12^2*_xlfn.VAR.P(B2:B37))</f>
+        <v>-0.23629010561291675</v>
       </c>
       <c r="N15">
         <v>14</v>
@@ -6118,11 +6146,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F16" s="8" cm="1">
-        <f t="array" ref="F16">SUM(IF(A2:A37-AVERAGE(A2:A37)&lt;0,0,(A2:A37-AVERAGE(A2:A37))^2))/COUNT(A2:A37)</f>
-        <v>5.1661111111111103E-4</v>
+        <f t="array" ref="F16">SUM(IF(AVERAGE(A2:A37)-A2:A37&lt;0,0,(AVERAGE(A2:A37)-A2:A37)^2))/COUNT(A2:A37)</f>
+        <v>5.83888888888889E-4</v>
       </c>
       <c r="N16">
         <v>15</v>
@@ -6174,11 +6202,11 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F17" s="8">
         <f>SQRT(F16)</f>
-        <v>2.2729080736165089E-2</v>
+        <v>2.4163792932585915E-2</v>
       </c>
       <c r="N17">
         <v>16</v>
@@ -6231,7 +6259,13 @@
       <c r="C18" s="14">
         <v>2E-3</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="8" cm="1">
+        <f t="array" ref="F18">SUM(IF(A2:A37-AVERAGE(A2:A37)&lt;0,0,(A2:A37-AVERAGE(A2:A37))^2))/COUNT(A2:A37)</f>
+        <v>5.1661111111111103E-4</v>
+      </c>
       <c r="N18">
         <v>17</v>
       </c>
@@ -6283,6 +6317,13 @@
       <c r="C19" s="14">
         <v>2E-3</v>
       </c>
+      <c r="E19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="8">
+        <f>SQRT(F18)</f>
+        <v>2.2729080736165089E-2</v>
+      </c>
       <c r="N19">
         <v>18</v>
       </c>
@@ -6307,24 +6348,7 @@
       <c r="C20" s="14">
         <v>2E-3</v>
       </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="21" cm="1">
-        <f t="array" ref="F20">_xll.SharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25479695255981605</v>
-      </c>
-      <c r="G20" s="21" cm="1">
-        <f t="array" ref="G20">_xll.SharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.94531290051723404</v>
-      </c>
-      <c r="I20" t="s">
-        <v>80</v>
-      </c>
-      <c r="J20" t="b" cm="1">
-        <f t="array" ref="J20">AND(ABS(F6:G17-F20:G31)&lt;0.000000001)</f>
-        <v>1</v>
-      </c>
+      <c r="F20" s="8"/>
       <c r="N20">
         <v>19</v>
       </c>
@@ -6353,17 +6377,6 @@
       <c r="C21" s="14">
         <v>1E-3</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="21" cm="1">
-        <f t="array" ref="F21">_xll.RevisedSharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25497722129753936</v>
-      </c>
-      <c r="G21" s="21" cm="1">
-        <f t="array" ref="G21">_xll.RevisedSharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.9459817090002941</v>
-      </c>
       <c r="N21">
         <v>20</v>
       </c>
@@ -6389,15 +6402,22 @@
         <v>1E-3</v>
       </c>
       <c r="E22" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="F22" s="21" cm="1">
-        <f t="array" ref="F22">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25223719852260701</v>
+        <f t="array" ref="F22">_xll.SharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25479695255981605</v>
       </c>
       <c r="G22" s="21" cm="1">
-        <f t="array" ref="G22">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.91065390211902919</v>
+        <f t="array" ref="G22">_xll.SharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.94531290051723404</v>
+      </c>
+      <c r="I22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" t="b" cm="1">
+        <f t="array" ref="J22">AND(ABS(F7:G19-F22:G34)&lt;0.000000001)</f>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>21</v>
@@ -6416,7 +6436,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -6426,16 +6446,16 @@
       <c r="C23" s="14">
         <v>1E-3</v>
       </c>
-      <c r="E23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="1" cm="1">
-        <f t="array" ref="F23">_xll.MSquared(A2:A37,B2:B37,C2:C37,1)</f>
-        <v>1.0565967513977965E-2</v>
-      </c>
-      <c r="G23" s="1" cm="1">
-        <f t="array" ref="G23">_xll.MSquared(A2:A37,B2:B37,C2:C37,12)</f>
-        <v>0.13435614552670944</v>
+      <c r="E23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="21" cm="1">
+        <f t="array" ref="F23">_xll.RevisedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25497722129753936</v>
+      </c>
+      <c r="G23" s="21" cm="1">
+        <f t="array" ref="G23">_xll.RevisedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.9459817090002941</v>
       </c>
       <c r="N23">
         <v>22</v>
@@ -6462,11 +6482,15 @@
         <v>1E-3</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="F24" s="21" cm="1">
-        <f t="array" ref="F24">_xll.Beta(A2:A37,B2:B37)</f>
-        <v>0.98144598446869213</v>
+        <f t="array" ref="F24">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25223719852260701</v>
+      </c>
+      <c r="G24" s="21" cm="1">
+        <f t="array" ref="G24">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.91065390211902919</v>
       </c>
       <c r="N24">
         <v>23</v>
@@ -6486,7 +6510,7 @@
       </c>
       <c r="U24" s="43"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>-2E-3</v>
       </c>
@@ -6497,15 +6521,15 @@
         <v>1E-3</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="21" cm="1">
-        <f t="array" ref="F25">_xll.TreynorIndex(A2:A37,F24,C2:C37,1)</f>
-        <v>8.6123733893902314E-3</v>
-      </c>
-      <c r="G25" s="21" cm="1">
-        <f t="array" ref="G25">_xll.TreynorIndex(A2:A37,F24,C2:C37,12)</f>
-        <v>0.11068654428760945</v>
+        <v>79</v>
+      </c>
+      <c r="F25" s="1" cm="1">
+        <f t="array" ref="F25">_xll.MSquared(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>1.0565967513977965E-2</v>
+      </c>
+      <c r="G25" s="1" cm="1">
+        <f t="array" ref="G25">_xll.MSquared(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>0.13435614552670944</v>
       </c>
       <c r="N25">
         <v>24</v>
@@ -6538,20 +6562,13 @@
         <v>1E-3</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="1" cm="1">
-        <f t="array" ref="F26">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,1)</f>
-        <v>-8.0899576840545023E-4</v>
-      </c>
-      <c r="G26" s="1" cm="1">
-        <f t="array" ref="G26">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,12)</f>
-        <v>-1.1048559174976408E-2</v>
-      </c>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
+        <v>126</v>
+      </c>
+      <c r="F26" s="21" cm="1">
+        <f t="array" ref="F26">_xll.RoyRatio(A2:A37,F5,1)</f>
+        <v>0.16435156971709428</v>
+      </c>
+      <c r="G26" s="1"/>
       <c r="N26">
         <v>25</v>
       </c>
@@ -6583,13 +6600,12 @@
         <v>1E-3</v>
       </c>
       <c r="E27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="8" cm="1">
-        <f t="array" ref="F27">_xll.AppraisalRatio($A$2:$A$37,$B$2:$B$37,$C$2:$C$37,1)</f>
-        <v>-0.23629010561292166</v>
-      </c>
-      <c r="G27" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="F27" s="21" cm="1">
+        <f t="array" ref="F27">_xll.Beta(A2:A37,B2:B37)</f>
+        <v>0.98144598446869213</v>
+      </c>
       <c r="N27">
         <v>26</v>
       </c>
@@ -6621,11 +6637,15 @@
         <v>1E-3</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="8" cm="1">
-        <f t="array" ref="F28">_xll.SemiVariance(A2:A37)</f>
-        <v>5.83888888888889E-4</v>
+        <v>7</v>
+      </c>
+      <c r="F28" s="21" cm="1">
+        <f t="array" ref="F28">_xll.TreynorIndex(A2:A37,F27,C2:C37,1)</f>
+        <v>8.6123733893902314E-3</v>
+      </c>
+      <c r="G28" s="21" cm="1">
+        <f t="array" ref="G28">_xll.TreynorIndex(A2:A37,F27,C2:C37,12)</f>
+        <v>0.11068654428760945</v>
       </c>
       <c r="N28">
         <v>27</v>
@@ -6658,20 +6678,20 @@
         <v>1E-3</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="8" cm="1">
-        <f t="array" ref="F29">_xll.SemiDeviation(A2:A37)</f>
-        <v>2.4163792932585915E-2</v>
-      </c>
-      <c r="J29" s="1">
-        <f>_xlfn.VAR.P(B2:B37)*12*F10^2</f>
-        <v>1.3065336093908721E-2</v>
-      </c>
-      <c r="K29" s="14">
-        <f>F10*_xlfn.STDEV.P(B2:B37)</f>
-        <v>3.2996636310777601E-2</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F29" s="1" cm="1">
+        <f t="array" ref="F29">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>-8.0899576840545023E-4</v>
+      </c>
+      <c r="G29" s="1" cm="1">
+        <f t="array" ref="G29">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>-1.1048559174976408E-2</v>
+      </c>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
       <c r="N29">
         <v>28</v>
       </c>
@@ -6703,12 +6723,13 @@
         <v>1E-3</v>
       </c>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="F30" s="8" cm="1">
-        <f t="array" ref="F30">_xll.UpperPartialMoment(A2:A37,,2,1)</f>
-        <v>5.1661111111111103E-4</v>
-      </c>
+        <f t="array" ref="F30">_xll.AppraisalRatio($A$2:$A$37,$B$2:$B$37,$C$2:$C$37,1)</f>
+        <v>-0.23629010561292166</v>
+      </c>
+      <c r="G30" s="8"/>
       <c r="N30">
         <v>29</v>
       </c>
@@ -6734,11 +6755,11 @@
         <v>2E-3</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" s="8">
-        <f>SQRT(F30)</f>
-        <v>2.2729080736165089E-2</v>
+        <v>121</v>
+      </c>
+      <c r="F31" s="8" cm="1">
+        <f t="array" ref="F31">_xll.SemiVariance(A2:A37)</f>
+        <v>5.83888888888889E-4</v>
       </c>
       <c r="N31">
         <v>30</v>
@@ -6768,11 +6789,19 @@
         <v>2E-3</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="F32" s="8" cm="1">
-        <f t="array" ref="F32">_xll.KRatio(A2:A37)</f>
-        <v>0.16768620342592805</v>
+        <f t="array" ref="F32">_xll.SemiDeviation(A2:A37)</f>
+        <v>2.4163792932585915E-2</v>
+      </c>
+      <c r="J32" s="1">
+        <f>_xlfn.VAR.P(B2:B37)*12*F12^2</f>
+        <v>1.3065336093908721E-2</v>
+      </c>
+      <c r="K32" s="14">
+        <f>F12*_xlfn.STDEV.P(B2:B37)</f>
+        <v>3.2996636310777601E-2</v>
       </c>
       <c r="N32">
         <v>31</v>
@@ -6814,7 +6843,13 @@
       <c r="C33" s="14">
         <v>2E-3</v>
       </c>
-      <c r="F33" s="8"/>
+      <c r="E33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="8" cm="1">
+        <f t="array" ref="F33">_xll.UpperPartialMoment(A2:A37,,2,1)</f>
+        <v>5.1661111111111103E-4</v>
+      </c>
       <c r="N33">
         <v>32</v>
       </c>
@@ -6857,6 +6892,13 @@
       <c r="C34" s="14">
         <v>2E-3</v>
       </c>
+      <c r="E34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="8">
+        <f>SQRT(F33)</f>
+        <v>2.2729080736165089E-2</v>
+      </c>
       <c r="N34">
         <v>33</v>
       </c>
@@ -6895,6 +6937,13 @@
       <c r="C35" s="14">
         <v>2E-3</v>
       </c>
+      <c r="E35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="8" cm="1">
+        <f t="array" ref="F35">_xll.KRatio(A2:A37)</f>
+        <v>0.16768620342592805</v>
+      </c>
       <c r="N35">
         <v>34</v>
       </c>
@@ -6931,6 +6980,7 @@
       <c r="C36" s="14">
         <v>2E-3</v>
       </c>
+      <c r="F36" s="8"/>
       <c r="N36">
         <v>35</v>
       </c>
@@ -6995,148 +7045,119 @@
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
+      <c r="N38">
+        <v>37</v>
+      </c>
+      <c r="R38" s="21">
+        <v>1454.0096659397295</v>
+      </c>
+      <c r="T38" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="U38" s="40">
+        <v>1020.5103479428813</v>
+      </c>
+      <c r="V38" s="40">
+        <v>20.181573213260343</v>
+      </c>
+      <c r="W38" s="40">
+        <v>50.566441830825802</v>
+      </c>
+      <c r="X38" s="40">
+        <v>2.5839067739645967E-34</v>
+      </c>
+      <c r="Y38" s="40">
+        <v>979.53957615807667</v>
+      </c>
+      <c r="Z38" s="40">
+        <v>1061.4811197276858</v>
+      </c>
+      <c r="AA38" s="40">
+        <v>979.53957615807667</v>
+      </c>
+      <c r="AB38" s="40">
+        <v>1061.4811197276858</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T39" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="U39" s="41">
+        <v>10.048059157673292</v>
+      </c>
+      <c r="V39" s="41">
+        <v>0.92599408587651855</v>
+      </c>
+      <c r="W39" s="41">
+        <v>10.851105110635881</v>
+      </c>
+      <c r="X39" s="41">
+        <v>9.5848430684231911E-13</v>
+      </c>
+      <c r="Y39" s="41">
+        <v>8.1681912224224416</v>
+      </c>
+      <c r="Z39" s="41">
+        <v>11.927927092924142</v>
+      </c>
+      <c r="AA39" s="41">
+        <v>8.1681912224224416</v>
+      </c>
+      <c r="AB39" s="41">
+        <v>11.927927092924142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
         <v>83</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F41" s="1">
         <f>_xlfn.VAR.P(A2:A37)</f>
         <v>1.1005000000000001E-3</v>
       </c>
-      <c r="G38" s="1">
-        <f>SQRT(F38*12)</f>
+      <c r="G41" s="1">
+        <f>SQRT(F41*12)</f>
         <v>0.11491736161259535</v>
       </c>
-      <c r="N38">
-        <v>37</v>
-      </c>
-      <c r="R38" s="21">
-        <v>1454.0096659397295</v>
-      </c>
-      <c r="T38" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="U38" s="40">
-        <v>1020.5103479428813</v>
-      </c>
-      <c r="V38" s="40">
-        <v>20.181573213260343</v>
-      </c>
-      <c r="W38" s="40">
-        <v>50.566441830825802</v>
-      </c>
-      <c r="X38" s="40">
-        <v>2.5839067739645967E-34</v>
-      </c>
-      <c r="Y38" s="40">
-        <v>979.53957615807667</v>
-      </c>
-      <c r="Z38" s="40">
-        <v>1061.4811197276858</v>
-      </c>
-      <c r="AA38" s="40">
-        <v>979.53957615807667</v>
-      </c>
-      <c r="AB38" s="40">
-        <v>1061.4811197276858</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E39" t="s">
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
         <v>84</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F42" s="1">
         <f>_xlfn.VAR.P(B2:B37)</f>
         <v>1.1303333333333335E-3</v>
       </c>
-      <c r="G39" s="1">
-        <f>F39*12</f>
+      <c r="G42" s="1">
+        <f>F42*12</f>
         <v>1.3564000000000001E-2</v>
       </c>
-      <c r="J39" s="1">
-        <f>F10^2*_xlfn.VAR.P(B2:B37)</f>
+      <c r="J42" s="1">
+        <f>F12^2*_xlfn.VAR.P(B2:B37)</f>
         <v>1.0887780078257267E-3</v>
       </c>
-      <c r="K39">
-        <f>SQRT(J39)</f>
+      <c r="K42">
+        <f>SQRT(J42)</f>
         <v>3.2996636310777601E-2</v>
       </c>
-      <c r="T39" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="U39" s="41">
-        <v>10.048059157673292</v>
-      </c>
-      <c r="V39" s="41">
-        <v>0.92599408587651855</v>
-      </c>
-      <c r="W39" s="41">
-        <v>10.851105110635881</v>
-      </c>
-      <c r="X39" s="41">
-        <v>9.5848430684231911E-13</v>
-      </c>
-      <c r="Y39" s="41">
-        <v>8.1681912224224416</v>
-      </c>
-      <c r="Z39" s="41">
-        <v>11.927927092924142</v>
-      </c>
-      <c r="AA39" s="41">
-        <v>8.1681912224224416</v>
-      </c>
-      <c r="AB39" s="41">
-        <v>11.927927092924142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="1">
-        <f>F10^2*F39</f>
+      <c r="F43" s="1">
+        <f>F12^2*F42</f>
         <v>1.0887780078257267E-3</v>
       </c>
-      <c r="G40" s="14">
-        <f>SQRT(F40)</f>
+      <c r="G43" s="14">
+        <f>SQRT(F43)</f>
         <v>3.2996636310777601E-2</v>
       </c>
-      <c r="H40" s="1" cm="1">
-        <f t="array" ref="H40">SQRT(_xll.MarketRisk(A2:A37,B2:B37,1))</f>
+      <c r="H43" s="1" cm="1">
+        <f t="array" ref="H43">SQRT(_xll.MarketRisk(A2:A37,B2:B37,1))</f>
         <v>3.2996636310777601E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" s="1">
-        <f>F38-F10^2*F39</f>
-        <v>1.1721992174273423E-5</v>
-      </c>
-      <c r="G41" s="1">
-        <f>SQRT(F41)</f>
-        <v>3.4237395015207311E-3</v>
-      </c>
-      <c r="H41" s="1" cm="1">
-        <f t="array" ref="H41">_xll.UniqueRisk(A2:A37,B2:B37,1)</f>
-        <v>1.1721992174272989E-5</v>
-      </c>
-      <c r="I41">
-        <f>SQRT(H41)</f>
-        <v>3.4237395015206673E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H42" s="11">
-        <f>SUM(H40:H41)</f>
-        <v>3.3008358302951873E-2</v>
-      </c>
-      <c r="I42">
-        <f>SQRT(H42)</f>
-        <v>0.18168202526103641</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="U43">
         <f>U39/U28</f>
         <v>0.16707854426309343</v>
@@ -7146,16 +7167,55 @@
         <v>10.048059157673293</v>
       </c>
     </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" s="1">
+        <f>F41-F12^2*F42</f>
+        <v>1.1721992174273423E-5</v>
+      </c>
+      <c r="G44" s="1">
+        <f>SQRT(F44)</f>
+        <v>3.4237395015207311E-3</v>
+      </c>
+      <c r="H44" s="1" cm="1">
+        <f t="array" ref="H44">_xll.UniqueRisk(A2:A37,B2:B37,1)</f>
+        <v>1.1721992174272989E-5</v>
+      </c>
+      <c r="I44">
+        <f>SQRT(H44)</f>
+        <v>3.4237395015206673E-3</v>
+      </c>
+    </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="H45" s="11">
+        <f>SUM(H43:H44)</f>
+        <v>3.3008358302951873E-2</v>
+      </c>
+      <c r="I45">
+        <f>SQRT(H45)</f>
+        <v>0.18168202526103641</v>
+      </c>
       <c r="U45" s="35">
         <f>STEYX(_xlfn.ANCHORARRAY(R2),_xlfn.ANCHORARRAY(N2))/SQRT(DEVSQ(_xlfn.ANCHORARRAY(N2)))</f>
         <v>0.9259940858765181</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F20:G32">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ABS(F20:G32-F6:G17) &gt; 0.0000000001</formula>
+  <conditionalFormatting sqref="F30:G35">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>ABS(F30:G42-F15:G27) &gt; 0.0000000001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:G29">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>ABS(F27:G39-F12:G23) &gt; 0.0000000001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:G25 G26">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>ABS(F22:G35-F7:G19) &gt; 0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new functions and updated documentation and add-ins I added the following functions: AverageMaxDrawDown, MaxDrawDownDuration, and SterlingRatio.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452DACC8-60C2-40FF-8957-F8283E1B3E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55F89A7-43B2-4DD8-A219-174CE41D0E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="27510" windowHeight="17460" activeTab="6" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="9990" yWindow="3300" windowWidth="27510" windowHeight="17460" activeTab="6" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="150">
   <si>
     <t>RFR</t>
   </si>
@@ -631,6 +631,12 @@
   </si>
   <si>
     <t>Ulcer Performance Index</t>
+  </si>
+  <si>
+    <t>Sterling Ratio (3 drawdowns)</t>
+  </si>
+  <si>
+    <t>Average Max Drawdown per Year</t>
   </si>
 </sst>
 </file>
@@ -9585,12 +9591,12 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -9875,9 +9881,7 @@
         <f t="array" ref="E8">_xll.AverageDrawDown($A$2:$A$37)</f>
         <v>-3.2508907555555577E-2</v>
       </c>
-      <c r="F8" s="14">
-        <v>-3.2508907555555577E-2</v>
-      </c>
+      <c r="F8" s="14"/>
       <c r="H8">
         <v>6</v>
       </c>
@@ -9922,9 +9926,7 @@
         <f t="array" ref="E9">_xll.AverageDrawDown($A$2:$A$37,3)</f>
         <v>-7.623800000000007E-2</v>
       </c>
-      <c r="F9" s="14">
-        <v>-7.623800000000007E-2</v>
-      </c>
+      <c r="F9" s="14"/>
       <c r="H9">
         <v>7</v>
       </c>
@@ -10006,6 +10008,13 @@
       <c r="B11" s="14">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="D11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="14" cm="1">
+        <f t="array" ref="E11">_xll.AverageMaxDrawDown(A2:A37,12)</f>
+        <v>-6.0441352226886035E-2</v>
+      </c>
       <c r="H11">
         <v>9</v>
       </c>
@@ -10603,6 +10612,13 @@
       <c r="B26" s="14">
         <v>1E-3</v>
       </c>
+      <c r="D26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="21" cm="1">
+        <f t="array" ref="E26">(PRODUCT(1+A2:A37)^(1/3)-PRODUCT(1+B2:B37)^(1/3))/ABS(E9)</f>
+        <v>1.4249175532646481</v>
+      </c>
       <c r="H26">
         <v>24</v>
       </c>
@@ -10639,6 +10655,13 @@
       </c>
       <c r="B27" s="14">
         <v>1E-3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="21" cm="1">
+        <f t="array" ref="E27">_xll.SterlingRatio(A2:A37,B2:B37,3,12)</f>
+        <v>1.4249175532646481</v>
       </c>
       <c r="H27">
         <v>25</v>

</xml_diff>

<commit_message>
Added some new functions and code cleanup Added HoldingPeriodReturn, HPRWithReinvestment, SubPeriodReturns, LogSubPeriodReturns, and MaxDrawdownByYear.
</commit_message>
<xml_diff>
--- a/PortfolioPerformance/Test Data.xlsx
+++ b/PortfolioPerformance/Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22508"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\OneDrive\C# Source\PortfolioPerformance\PortfolioPerformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55F89A7-43B2-4DD8-A219-174CE41D0E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9766FE-7A33-4C9D-A101-9E4833EA5B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9990" yWindow="3300" windowWidth="27510" windowHeight="17460" activeTab="6" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
+    <workbookView xWindow="3255" yWindow="2040" windowWidth="27150" windowHeight="17460" firstSheet="3" activeTab="6" xr2:uid="{344BB257-92D6-46F2-9766-17934D9BF305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="Tables 3.4 and 3.5" sheetId="7" r:id="rId6"/>
     <sheet name="Table 5.1 Drawdown Statistics" sheetId="10" r:id="rId7"/>
     <sheet name="K-Ratio" sheetId="9" r:id="rId8"/>
+    <sheet name="Value at Risk" sheetId="11" r:id="rId9"/>
+    <sheet name="Calculating Returns" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -102,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G24" authorId="0" shapeId="0" xr:uid="{5CCAA0DA-5FA8-4FC8-B47B-DA427260DD08}">
+    <comment ref="G28" authorId="0" shapeId="0" xr:uid="{5CCAA0DA-5FA8-4FC8-B47B-DA427260DD08}">
       <text>
         <r>
           <rPr>
@@ -153,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="169">
   <si>
     <t>RFR</t>
   </si>
@@ -637,6 +639,63 @@
   </si>
   <si>
     <t>Average Max Drawdown per Year</t>
+  </si>
+  <si>
+    <t>Omega Ratio</t>
+  </si>
+  <si>
+    <t>Kappa Index</t>
+  </si>
+  <si>
+    <t>Para VaR</t>
+  </si>
+  <si>
+    <t>Mod Para VaR</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Portfolio Returns</t>
+  </si>
+  <si>
+    <t>Benmark Returns</t>
+  </si>
+  <si>
+    <t>Risk-Free Rate</t>
+  </si>
+  <si>
+    <t>Testing Excel's Norm.S.Inv against my NormalCdfInverse</t>
+  </si>
+  <si>
+    <t>Conf Level</t>
+  </si>
+  <si>
+    <t>Norm.S.Inv</t>
+  </si>
+  <si>
+    <t>NormalCdfInverse</t>
+  </si>
+  <si>
+    <t>Hist Sim VaR</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Cash Flow</t>
+  </si>
+  <si>
+    <t>HPR Reinvest</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Log Price Relatives</t>
   </si>
 </sst>
 </file>
@@ -841,7 +900,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5169,6 +5242,176 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13322D9B-6A6B-4627-B4EF-3D607F2E0DD2}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="14">
+        <f>(B3+C3)/B2-1</f>
+        <v>-3.0000000000000027E-2</v>
+      </c>
+      <c r="H3" s="14" cm="1">
+        <f t="array" ref="H3:H6">_xll.SubPeriodReturns(B2:B6,C3:C6)</f>
+        <v>-3.0000000000000027E-2</v>
+      </c>
+      <c r="I3" s="14" cm="1">
+        <f t="array" ref="I3:I6">_xll.LogSubPeriodReturns(B2:B6,C3:C6)</f>
+        <v>-3.0459207484708574E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" ref="E4:E6" si="0">(B4+C4)/B3-1</f>
+        <v>4.2105263157894646E-2</v>
+      </c>
+      <c r="H4" s="14">
+        <v>4.2105263157894646E-2</v>
+      </c>
+      <c r="I4" s="14">
+        <v>4.1242958534049003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" si="0"/>
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="H5" s="14">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="I5" s="14">
+        <v>6.8992871486951421E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>108</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
+        <v>7.7669902912621325E-2</v>
+      </c>
+      <c r="H6" s="14">
+        <v>7.7669902912621325E-2</v>
+      </c>
+      <c r="I6" s="14">
+        <v>7.480121308269834E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14">
+        <f>(B6+SUM(C3:C6))/B2-1</f>
+        <v>0.15999999999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="14" cm="1">
+        <f t="array" ref="B9">_xll.HoldingPeriodReturn(B2:B6,C3:C6)</f>
+        <v>0.15999999999999992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="14" cm="1">
+        <f t="array" ref="B11">PRODUCT((B3:B6+C3:C6)/B2:B5)-1</f>
+        <v>0.16716512154171803</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="14" cm="1">
+        <f t="array" ref="B12">_xll.HPRWithReinvestment(B2:B6,C3:C6)</f>
+        <v>0.16716512154171803</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5E2AEA-8CFA-45DF-BCFE-1A720439ADBA}">
   <dimension ref="A1:M30"/>
@@ -7270,10 +7513,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD720BF-B3A2-4768-8CA5-EE00905CFCE9}">
-  <dimension ref="A1:AB45"/>
+  <dimension ref="A1:BB52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C37"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7291,7 +7534,7 @@
     <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -7320,7 +7563,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -7361,11 +7604,119 @@
         <v>2.9999999999998916E-3</v>
       </c>
       <c r="R2" s="21" cm="1">
-        <f t="array" ref="R2:R38">TRANSPOSE(_xll.TotalReturnIndex(A2:A37,1000))</f>
+        <f t="array" ref="R2:BB2">TRANSPOSE(_xll.TotalReturnIndex(A2:A37,1000))</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S2">
+        <v>1002.9999999999999</v>
+      </c>
+      <c r="T2">
+        <v>1029.078</v>
+      </c>
+      <c r="U2">
+        <v>1040.3978579999998</v>
+      </c>
+      <c r="V2">
+        <v>1031.0342772779998</v>
+      </c>
+      <c r="W2">
+        <v>1045.4687571598918</v>
+      </c>
+      <c r="X2">
+        <v>1070.5600073317291</v>
+      </c>
+      <c r="Y2">
+        <v>1086.6184074417049</v>
+      </c>
+      <c r="Z2">
+        <v>1158.3352223328575</v>
+      </c>
+      <c r="AA2">
+        <v>1142.1185292201974</v>
+      </c>
+      <c r="AB2">
+        <v>1186.6611518597849</v>
+      </c>
+      <c r="AC2">
+        <v>1180.727846100486</v>
+      </c>
+      <c r="AD2">
+        <v>1276.3668016346253</v>
+      </c>
+      <c r="AE2">
+        <v>1327.4214737000104</v>
+      </c>
+      <c r="AF2">
+        <v>1278.30687917311</v>
+      </c>
+      <c r="AG2">
+        <v>1200.3301595435503</v>
+      </c>
+      <c r="AH2">
+        <v>1217.13478177716</v>
+      </c>
+      <c r="AI2">
+        <v>1157.4951774700792</v>
+      </c>
+      <c r="AJ2">
+        <v>1133.1877787432074</v>
+      </c>
+      <c r="AK2">
+        <v>1203.4454210252864</v>
+      </c>
+      <c r="AL2">
+        <v>1273.245255444753</v>
+      </c>
+      <c r="AM2">
+        <v>1191.7575590962888</v>
+      </c>
+      <c r="AN2">
+        <v>1212.0174376009256</v>
+      </c>
+      <c r="AO2">
+        <v>1207.1693678505219</v>
+      </c>
+      <c r="AP2">
+        <v>1204.7550291148209</v>
+      </c>
+      <c r="AQ2">
+        <v>1179.4551735034097</v>
+      </c>
+      <c r="AR2">
+        <v>1192.4291804119471</v>
+      </c>
+      <c r="AS2">
+        <v>1248.4733518913085</v>
+      </c>
+      <c r="AT2">
+        <v>1278.4367123366999</v>
+      </c>
+      <c r="AU2">
+        <v>1320.6251238438108</v>
+      </c>
+      <c r="AV2">
+        <v>1311.3807479769041</v>
+      </c>
+      <c r="AW2">
+        <v>1373.0156431318185</v>
+      </c>
+      <c r="AX2">
+        <v>1381.2537369906095</v>
+      </c>
+      <c r="AY2">
+        <v>1395.0662743605155</v>
+      </c>
+      <c r="AZ2">
+        <v>1392.2761418117946</v>
+      </c>
+      <c r="BA2">
+        <v>1439.6135306333956</v>
+      </c>
+      <c r="BB2">
+        <v>1454.0096659397295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2.6000000000000002E-2</v>
       </c>
@@ -7413,15 +7764,13 @@
         <f t="shared" ref="P3:P37" si="1">(1+P2)*(1+O3)-1</f>
         <v>2.9077999999999937E-2</v>
       </c>
-      <c r="R3" s="21">
-        <v>1002.9999999999999</v>
-      </c>
+      <c r="R3" s="21"/>
       <c r="T3" s="41" t="s">
         <v>89</v>
       </c>
       <c r="U3" s="41"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>1.1000000000000001E-2</v>
       </c>
@@ -7469,9 +7818,7 @@
         <f t="shared" si="1"/>
         <v>4.0397857999999731E-2</v>
       </c>
-      <c r="R4" s="21">
-        <v>1029.078</v>
-      </c>
+      <c r="R4" s="21"/>
       <c r="T4" s="38" t="s">
         <v>90</v>
       </c>
@@ -7479,7 +7826,7 @@
         <v>0.8672578125579653</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>-9.0000000000000011E-3</v>
       </c>
@@ -7514,9 +7861,7 @@
         <f t="shared" si="1"/>
         <v>3.1034277277999678E-2</v>
       </c>
-      <c r="R5" s="21">
-        <v>1040.3978579999998</v>
-      </c>
+      <c r="R5" s="21"/>
       <c r="T5" s="38" t="s">
         <v>91</v>
       </c>
@@ -7524,7 +7869,7 @@
         <v>0.75213611344282683</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>1.3999999999999999E-2</v>
       </c>
@@ -7545,9 +7890,7 @@
         <f t="shared" si="1"/>
         <v>4.5468757159891737E-2</v>
       </c>
-      <c r="R6" s="21">
-        <v>1031.0342772779998</v>
-      </c>
+      <c r="R6" s="21"/>
       <c r="T6" s="38" t="s">
         <v>92</v>
       </c>
@@ -7555,7 +7898,7 @@
         <v>0.74484599913232175</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>2.4E-2</v>
       </c>
@@ -7587,9 +7930,7 @@
         <f t="shared" si="1"/>
         <v>7.056000733172918E-2</v>
       </c>
-      <c r="R7" s="21">
-        <v>1045.4687571598918</v>
-      </c>
+      <c r="R7" s="21"/>
       <c r="T7" s="38" t="s">
         <v>93</v>
       </c>
@@ -7597,7 +7938,7 @@
         <v>6.0766076195599643E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -7618,10 +7959,6 @@
         <f t="array" ref="G8">(G3-M3)/(_xlfn.STDEV.P(A2:A37-C2:C37)*SQRT(12))</f>
         <v>0.9459817090002941</v>
       </c>
-      <c r="J8">
-        <f>_xlfn.VAR.P(B2:B37)</f>
-        <v>1.1303333333333335E-3</v>
-      </c>
       <c r="N8">
         <v>7</v>
       </c>
@@ -7633,9 +7970,7 @@
         <f t="shared" si="1"/>
         <v>8.6618407441704903E-2</v>
       </c>
-      <c r="R8" s="21">
-        <v>1070.5600073317291</v>
-      </c>
+      <c r="R8" s="21"/>
       <c r="T8" s="39" t="s">
         <v>94</v>
       </c>
@@ -7643,7 +7978,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -7676,11 +8011,9 @@
         <f t="shared" si="1"/>
         <v>0.15833522233285757</v>
       </c>
-      <c r="R9" s="21">
-        <v>1086.6184074417049</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="21"/>
+    </row>
+    <row r="10" spans="1:54" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>-1.3999999999999999E-2</v>
       </c>
@@ -7712,14 +8045,12 @@
         <f t="shared" si="1"/>
         <v>0.14211852922019763</v>
       </c>
-      <c r="R10" s="21">
-        <v>1158.3352223328575</v>
-      </c>
+      <c r="R10" s="21"/>
       <c r="T10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>3.9E-2</v>
       </c>
@@ -7748,9 +8079,7 @@
         <f t="shared" si="1"/>
         <v>0.18666115185978516</v>
       </c>
-      <c r="R11" s="21">
-        <v>1142.1185292201974</v>
-      </c>
+      <c r="R11" s="21"/>
       <c r="T11" s="40"/>
       <c r="U11" s="40" t="s">
         <v>100</v>
@@ -7768,7 +8097,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>-5.0000000000000001E-3</v>
       </c>
@@ -7786,6 +8115,7 @@
         <v>0.98144598446869191</v>
       </c>
       <c r="G12" s="1"/>
+      <c r="J12" s="14"/>
       <c r="N12">
         <v>11</v>
       </c>
@@ -7797,9 +8127,7 @@
         <f t="shared" si="1"/>
         <v>0.1807278461004862</v>
       </c>
-      <c r="R12" s="21">
-        <v>1186.6611518597849</v>
-      </c>
+      <c r="R12" s="21"/>
       <c r="T12" s="38" t="s">
         <v>96</v>
       </c>
@@ -7819,7 +8147,7 @@
         <v>7.8089252451616348E-12</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>8.1000000000000003E-2</v>
       </c>
@@ -7840,6 +8168,7 @@
         <f>(G3-M3)/F12</f>
         <v>0.11068654428760948</v>
       </c>
+      <c r="J13" s="14"/>
       <c r="N13">
         <v>12</v>
       </c>
@@ -7851,9 +8180,7 @@
         <f t="shared" si="1"/>
         <v>0.27636680163462546</v>
       </c>
-      <c r="R13" s="21">
-        <v>1180.727846100486</v>
-      </c>
+      <c r="R13" s="21"/>
       <c r="T13" s="38" t="s">
         <v>97</v>
       </c>
@@ -7869,7 +8196,7 @@
       <c r="X13" s="38"/>
       <c r="Y13" s="38"/>
     </row>
-    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>0.04</v>
       </c>
@@ -7891,6 +8218,7 @@
         <v>-1.104855917497638E-2</v>
       </c>
       <c r="I14" s="1"/>
+      <c r="J14" s="28"/>
       <c r="N14">
         <v>13</v>
       </c>
@@ -7902,9 +8230,7 @@
         <f t="shared" si="1"/>
         <v>0.32742147370001051</v>
       </c>
-      <c r="R14" s="21">
-        <v>1276.3668016346253</v>
-      </c>
+      <c r="R14" s="21"/>
       <c r="T14" s="39" t="s">
         <v>98</v>
       </c>
@@ -7918,7 +8244,7 @@
       <c r="X14" s="39"/>
       <c r="Y14" s="39"/>
     </row>
-    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>-3.7000000000000005E-2</v>
       </c>
@@ -7946,11 +8272,9 @@
         <f t="shared" si="1"/>
         <v>0.27830687917311003</v>
       </c>
-      <c r="R15" s="21">
-        <v>1327.4214737000104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R15" s="21"/>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>-6.0999999999999999E-2</v>
       </c>
@@ -7978,9 +8302,7 @@
         <f t="shared" si="1"/>
         <v>0.20033015954355049</v>
       </c>
-      <c r="R16" s="21">
-        <v>1278.30687917311</v>
-      </c>
+      <c r="R16" s="21"/>
       <c r="T16" s="40"/>
       <c r="U16" s="40" t="s">
         <v>105</v>
@@ -8024,6 +8346,7 @@
         <f>SQRT(F16)</f>
         <v>2.4163792932585915E-2</v>
       </c>
+      <c r="H17" s="11"/>
       <c r="N17">
         <v>16</v>
       </c>
@@ -8035,9 +8358,7 @@
         <f t="shared" si="1"/>
         <v>0.21713478177716028</v>
       </c>
-      <c r="R17" s="21">
-        <v>1200.3301595435503</v>
-      </c>
+      <c r="R17" s="21"/>
       <c r="T17" s="38" t="s">
         <v>99</v>
       </c>
@@ -8094,9 +8415,7 @@
         <f t="shared" si="1"/>
         <v>0.15749517747007946</v>
       </c>
-      <c r="R18" s="21">
-        <v>1217.13478177716</v>
-      </c>
+      <c r="R18" s="21"/>
       <c r="T18" s="39" t="s">
         <v>112</v>
       </c>
@@ -8153,9 +8472,7 @@
         <f t="shared" si="1"/>
         <v>0.13318777874320786</v>
       </c>
-      <c r="R19" s="21">
-        <v>1157.4951774700792</v>
-      </c>
+      <c r="R19" s="21"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
@@ -8185,9 +8502,7 @@
         <f t="shared" si="1"/>
         <v>0.20344542102528673</v>
       </c>
-      <c r="R20" s="21">
-        <v>1133.1877787432074</v>
-      </c>
+      <c r="R20" s="21"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
@@ -8199,6 +8514,13 @@
       <c r="C21" s="14">
         <v>1E-3</v>
       </c>
+      <c r="E21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="21" cm="1">
+        <f t="array" ref="F21">SUM(IF(A2:A37-F5&lt;0,0,(A2:A37-F5)))/SUM(IF(F5-A2:A37&lt;0,0,(F5-A2:A37)))</f>
+        <v>1.5950413223140494</v>
+      </c>
       <c r="N21">
         <v>20</v>
       </c>
@@ -8210,9 +8532,7 @@
         <f t="shared" si="1"/>
         <v>0.27324525544475353</v>
       </c>
-      <c r="R21" s="21">
-        <v>1203.4454210252864</v>
-      </c>
+      <c r="R21" s="21"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
@@ -8225,22 +8545,11 @@
         <v>1E-3</v>
       </c>
       <c r="E22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="21" cm="1">
-        <f t="array" ref="F22">_xll.SharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25479695255981605</v>
-      </c>
-      <c r="G22" s="21" cm="1">
-        <f t="array" ref="G22">_xll.SharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.94531290051723404</v>
-      </c>
-      <c r="I22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J22" t="b" cm="1">
-        <f t="array" ref="J22">AND(ABS(F7:G19-F22:G34)&lt;0.000000001)</f>
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="F22" s="8" cm="1">
+        <f t="array" ref="F22">(AVERAGE(A2:A37)-F5)/(SUM(IF(F5-A2:A37&lt;0,0,(F5-A2:A37)))/COUNT(A2:A37))</f>
+        <v>0.59504132231404949</v>
       </c>
       <c r="N22">
         <v>21</v>
@@ -8253,9 +8562,7 @@
         <f t="shared" si="1"/>
         <v>0.19175755909628922</v>
       </c>
-      <c r="R22" s="21">
-        <v>1273.245255444753</v>
-      </c>
+      <c r="R22" s="21"/>
       <c r="T22" t="s">
         <v>88</v>
       </c>
@@ -8270,17 +8577,7 @@
       <c r="C23" s="14">
         <v>1E-3</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="21" cm="1">
-        <f t="array" ref="F23">_xll.RevisedSharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25497722129753936</v>
-      </c>
-      <c r="G23" s="21" cm="1">
-        <f t="array" ref="G23">_xll.RevisedSharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.9459817090002941</v>
-      </c>
+      <c r="F23" s="8"/>
       <c r="N23">
         <v>22</v>
       </c>
@@ -8292,9 +8589,7 @@
         <f t="shared" si="1"/>
         <v>0.21201743760092606</v>
       </c>
-      <c r="R23" s="21">
-        <v>1191.7575590962888</v>
-      </c>
+      <c r="R23" s="21"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
@@ -8306,17 +8601,7 @@
       <c r="C24" s="14">
         <v>1E-3</v>
       </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="21" cm="1">
-        <f t="array" ref="F24">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,1)</f>
-        <v>0.25223719852260701</v>
-      </c>
-      <c r="G24" s="21" cm="1">
-        <f t="array" ref="G24">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,12)</f>
-        <v>0.91065390211902919</v>
-      </c>
+      <c r="F24" s="8"/>
       <c r="N24">
         <v>23</v>
       </c>
@@ -8328,15 +8613,13 @@
         <f t="shared" si="1"/>
         <v>0.20716936785052242</v>
       </c>
-      <c r="R24" s="21">
-        <v>1212.0174376009256</v>
-      </c>
+      <c r="R24" s="21"/>
       <c r="T24" s="41" t="s">
         <v>89</v>
       </c>
       <c r="U24" s="41"/>
     </row>
-    <row r="25" spans="1:28" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>-2E-3</v>
       </c>
@@ -8346,17 +8629,6 @@
       <c r="C25" s="14">
         <v>1E-3</v>
       </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="1" cm="1">
-        <f t="array" ref="F25">_xll.MSquared(A2:A37,B2:B37,C2:C37,1)</f>
-        <v>1.0565967513977965E-2</v>
-      </c>
-      <c r="G25" s="1" cm="1">
-        <f t="array" ref="G25">_xll.MSquared(A2:A37,B2:B37,C2:C37,12)</f>
-        <v>0.13435614552670944</v>
-      </c>
       <c r="N25">
         <v>24</v>
       </c>
@@ -8368,9 +8640,7 @@
         <f t="shared" si="1"/>
         <v>0.20475502911482146</v>
       </c>
-      <c r="R25" s="21">
-        <v>1207.1693678505219</v>
-      </c>
+      <c r="R25" s="21"/>
       <c r="T25" s="38" t="s">
         <v>90</v>
       </c>
@@ -8389,13 +8659,23 @@
         <v>1E-3</v>
       </c>
       <c r="E26" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="F26" s="21" cm="1">
-        <f t="array" ref="F26">_xll.RoyRatio(A2:A37,F5,1)</f>
-        <v>0.16435156971709428</v>
-      </c>
-      <c r="G26" s="1"/>
+        <f t="array" ref="F26">_xll.SharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25479695255981605</v>
+      </c>
+      <c r="G26" s="21" cm="1">
+        <f t="array" ref="G26">_xll.SharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.94531290051723404</v>
+      </c>
+      <c r="I26" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" t="e" cm="1">
+        <f t="array" ref="J26">AND(ABS(F7:G22-F26:G41)&lt;0.000000001)</f>
+        <v>#N/A</v>
+      </c>
       <c r="N26">
         <v>25</v>
       </c>
@@ -8407,9 +8687,7 @@
         <f t="shared" si="1"/>
         <v>0.17945517350341023</v>
       </c>
-      <c r="R26" s="21">
-        <v>1204.7550291148209</v>
-      </c>
+      <c r="R26" s="21"/>
       <c r="T26" s="38" t="s">
         <v>91</v>
       </c>
@@ -8427,12 +8705,16 @@
       <c r="C27" s="14">
         <v>1E-3</v>
       </c>
-      <c r="E27" t="s">
-        <v>8</v>
+      <c r="E27" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="F27" s="21" cm="1">
-        <f t="array" ref="F27">_xll.Beta(A2:A37,B2:B37)</f>
-        <v>0.98144598446869213</v>
+        <f t="array" ref="F27">_xll.RevisedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25497722129753936</v>
+      </c>
+      <c r="G27" s="21" cm="1">
+        <f t="array" ref="G27">_xll.RevisedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.9459817090002941</v>
       </c>
       <c r="N27">
         <v>26</v>
@@ -8445,9 +8727,7 @@
         <f t="shared" si="1"/>
         <v>0.19242918041194756</v>
       </c>
-      <c r="R27" s="21">
-        <v>1179.4551735034097</v>
-      </c>
+      <c r="R27" s="21"/>
       <c r="T27" s="38" t="s">
         <v>92</v>
       </c>
@@ -8466,15 +8746,15 @@
         <v>1E-3</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="F28" s="21" cm="1">
-        <f t="array" ref="F28">_xll.TreynorIndex(A2:A37,F27,C2:C37,1)</f>
-        <v>8.6123733893902314E-3</v>
+        <f t="array" ref="F28">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,1)</f>
+        <v>0.25223719852260701</v>
       </c>
       <c r="G28" s="21" cm="1">
-        <f t="array" ref="G28">_xll.TreynorIndex(A2:A37,F27,C2:C37,12)</f>
-        <v>0.11068654428760945</v>
+        <f t="array" ref="G28">_xll.AdjustedSharpeRatio(A2:A37,C2:C37,12)</f>
+        <v>0.91065390211902919</v>
       </c>
       <c r="N28">
         <v>27</v>
@@ -8487,9 +8767,7 @@
         <f t="shared" si="1"/>
         <v>0.24847335189130892</v>
       </c>
-      <c r="R28" s="21">
-        <v>1192.4291804119471</v>
-      </c>
+      <c r="R28" s="21"/>
       <c r="T28" s="38" t="s">
         <v>93</v>
       </c>
@@ -8497,7 +8775,7 @@
         <v>4.7422874864075884E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
         <v>2.4E-2</v>
       </c>
@@ -8508,20 +8786,16 @@
         <v>1E-3</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="F29" s="1" cm="1">
-        <f t="array" ref="F29">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,1)</f>
-        <v>-8.0899576840545023E-4</v>
+        <f t="array" ref="F29">_xll.MSquared(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>1.0565967513977965E-2</v>
       </c>
       <c r="G29" s="1" cm="1">
-        <f t="array" ref="G29">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,12)</f>
-        <v>-1.1048559174976408E-2</v>
-      </c>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
+        <f t="array" ref="G29">_xll.MSquared(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>0.13435614552670944</v>
+      </c>
       <c r="N29">
         <v>28</v>
       </c>
@@ -8533,9 +8807,7 @@
         <f t="shared" si="1"/>
         <v>0.27843671233670042</v>
       </c>
-      <c r="R29" s="21">
-        <v>1248.4733518913085</v>
-      </c>
+      <c r="R29" s="21"/>
       <c r="T29" s="39" t="s">
         <v>94</v>
       </c>
@@ -8554,13 +8826,13 @@
         <v>1E-3</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="8" cm="1">
-        <f t="array" ref="F30">_xll.AppraisalRatio($A$2:$A$37,$B$2:$B$37,$C$2:$C$37,1)</f>
-        <v>-0.23629010561292166</v>
-      </c>
-      <c r="G30" s="8"/>
+        <v>124</v>
+      </c>
+      <c r="F30" s="21" cm="1">
+        <f t="array" ref="F30">_xll.RoyRatio(A2:A37,F5,1)</f>
+        <v>0.16435156971709428</v>
+      </c>
+      <c r="G30" s="1"/>
       <c r="N30">
         <v>29</v>
       </c>
@@ -8572,9 +8844,7 @@
         <f t="shared" si="1"/>
         <v>0.32062512384381137</v>
       </c>
-      <c r="R30" s="21">
-        <v>1278.4367123366999</v>
-      </c>
+      <c r="R30" s="21"/>
     </row>
     <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
@@ -8587,11 +8857,11 @@
         <v>2E-3</v>
       </c>
       <c r="E31" t="s">
-        <v>120</v>
-      </c>
-      <c r="F31" s="8" cm="1">
-        <f t="array" ref="F31">_xll.SemiVariance(A2:A37)</f>
-        <v>5.83888888888889E-4</v>
+        <v>8</v>
+      </c>
+      <c r="F31" s="21" cm="1">
+        <f t="array" ref="F31">_xll.Beta(A2:A37,B2:B37)</f>
+        <v>0.98144598446869213</v>
       </c>
       <c r="N31">
         <v>30</v>
@@ -8604,9 +8874,7 @@
         <f t="shared" si="1"/>
         <v>0.31138074797690463</v>
       </c>
-      <c r="R31" s="21">
-        <v>1320.6251238438108</v>
-      </c>
+      <c r="R31" s="21"/>
       <c r="T31" t="s">
         <v>95</v>
       </c>
@@ -8622,19 +8890,15 @@
         <v>2E-3</v>
       </c>
       <c r="E32" t="s">
-        <v>121</v>
-      </c>
-      <c r="F32" s="8" cm="1">
-        <f t="array" ref="F32">_xll.SemiDeviation(A2:A37)</f>
-        <v>2.4163792932585915E-2</v>
-      </c>
-      <c r="J32" s="1">
-        <f>_xlfn.VAR.P(B2:B37)*12*F12^2</f>
-        <v>1.3065336093908721E-2</v>
-      </c>
-      <c r="K32" s="14">
-        <f>F12*_xlfn.STDEV.P(B2:B37)</f>
-        <v>3.2996636310777601E-2</v>
+        <v>7</v>
+      </c>
+      <c r="F32" s="21" cm="1">
+        <f t="array" ref="F32">_xll.TreynorIndex(A2:A37,F31,C2:C37,1)</f>
+        <v>8.6123733893902314E-3</v>
+      </c>
+      <c r="G32" s="21" cm="1">
+        <f t="array" ref="G32">_xll.TreynorIndex(A2:A37,F31,C2:C37,12)</f>
+        <v>0.11068654428760945</v>
       </c>
       <c r="N32">
         <v>31</v>
@@ -8647,9 +8911,7 @@
         <f t="shared" si="1"/>
         <v>0.37301564313181901</v>
       </c>
-      <c r="R32" s="21">
-        <v>1311.3807479769041</v>
-      </c>
+      <c r="R32" s="21"/>
       <c r="T32" s="40"/>
       <c r="U32" s="40" t="s">
         <v>100</v>
@@ -8678,12 +8940,20 @@
         <v>2E-3</v>
       </c>
       <c r="E33" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="8" cm="1">
-        <f t="array" ref="F33">_xll.UpperPartialMoment(A2:A37,,2,1)</f>
-        <v>5.1661111111111103E-4</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F33" s="1" cm="1">
+        <f t="array" ref="F33">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,1)</f>
+        <v>-8.0899576840545023E-4</v>
+      </c>
+      <c r="G33" s="1" cm="1">
+        <f t="array" ref="G33">_xll.JensensAlpha(A2:A37,B2:B37,C2:C37,12)</f>
+        <v>-1.1048559174976408E-2</v>
+      </c>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
       <c r="N33">
         <v>32</v>
       </c>
@@ -8695,9 +8965,7 @@
         <f t="shared" si="1"/>
         <v>0.38125373699060994</v>
       </c>
-      <c r="R33" s="21">
-        <v>1373.0156431318185</v>
-      </c>
+      <c r="R33" s="21"/>
       <c r="T33" s="38" t="s">
         <v>96</v>
       </c>
@@ -8728,12 +8996,13 @@
         <v>2E-3</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="8">
-        <f>SQRT(F33)</f>
-        <v>2.2729080736165089E-2</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F34" s="8" cm="1">
+        <f t="array" ref="F34">_xll.AppraisalRatio($A$2:$A$37,$B$2:$B$37,$C$2:$C$37,1)</f>
+        <v>-0.23629010561292166</v>
+      </c>
+      <c r="G34" s="8"/>
       <c r="N34">
         <v>33</v>
       </c>
@@ -8745,9 +9014,7 @@
         <f t="shared" si="1"/>
         <v>0.395066274360516</v>
       </c>
-      <c r="R34" s="21">
-        <v>1381.2537369906095</v>
-      </c>
+      <c r="R34" s="21"/>
       <c r="T34" s="38" t="s">
         <v>97</v>
       </c>
@@ -8774,13 +9041,12 @@
         <v>2E-3</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="F35" s="8" cm="1">
-        <f t="array" ref="F35">_xll.KRatio(A2:A37)</f>
-        <v>1.7839106913325309</v>
-      </c>
-      <c r="G35" s="35"/>
+        <f t="array" ref="F35">_xll.SemiVariance(A2:A37)</f>
+        <v>5.83888888888889E-4</v>
+      </c>
       <c r="N35">
         <v>34</v>
       </c>
@@ -8792,9 +9058,7 @@
         <f t="shared" si="1"/>
         <v>0.39227614181179504</v>
       </c>
-      <c r="R35" s="21">
-        <v>1395.0662743605155</v>
-      </c>
+      <c r="R35" s="21"/>
       <c r="T35" s="39" t="s">
         <v>98</v>
       </c>
@@ -8818,7 +9082,21 @@
       <c r="C36" s="14">
         <v>2E-3</v>
       </c>
-      <c r="F36" s="8"/>
+      <c r="E36" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="8" cm="1">
+        <f t="array" ref="F36">_xll.SemiDeviation(A2:A37)</f>
+        <v>2.4163792932585915E-2</v>
+      </c>
+      <c r="J36" s="1">
+        <f>_xlfn.VAR.P(B2:B37)*12*F12^2</f>
+        <v>1.3065336093908721E-2</v>
+      </c>
+      <c r="K36" s="14">
+        <f>F12*_xlfn.STDEV.P(B2:B37)</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
       <c r="N36">
         <v>35</v>
       </c>
@@ -8830,9 +9108,7 @@
         <f t="shared" si="1"/>
         <v>0.43961353063339614</v>
       </c>
-      <c r="R36" s="21">
-        <v>1392.2761418117946</v>
-      </c>
+      <c r="R36" s="21"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
@@ -8845,15 +9121,11 @@
         <v>2E-3</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
-      </c>
-      <c r="F37">
-        <f>W18</f>
-        <v>10.157364831893609</v>
-      </c>
-      <c r="G37">
-        <f>F37/SQRT(36)</f>
-        <v>1.6928941386489349</v>
+        <v>122</v>
+      </c>
+      <c r="F37" s="8" cm="1">
+        <f t="array" ref="F37">_xll.UpperPartialMoment(A2:A37,,2,1)</f>
+        <v>5.1661111111111103E-4</v>
       </c>
       <c r="N37">
         <v>36</v>
@@ -8866,9 +9138,7 @@
         <f t="shared" si="1"/>
         <v>0.45400966593973013</v>
       </c>
-      <c r="R37" s="21">
-        <v>1439.6135306333956</v>
-      </c>
+      <c r="R37" s="21"/>
       <c r="T37" s="40"/>
       <c r="U37" s="40" t="s">
         <v>105</v>
@@ -8896,13 +9166,18 @@
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38" s="8">
+        <f>SQRT(F37)</f>
+        <v>2.2729080736165089E-2</v>
+      </c>
       <c r="N38">
         <v>37</v>
       </c>
       <c r="P38" s="14"/>
-      <c r="R38" s="21">
-        <v>1454.0096659397295</v>
-      </c>
+      <c r="R38" s="21"/>
       <c r="T38" s="38" t="s">
         <v>99</v>
       </c>
@@ -8932,6 +9207,14 @@
       </c>
     </row>
     <row r="39" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" s="8" cm="1">
+        <f t="array" ref="F39">_xll.KRatio(A2:A37)</f>
+        <v>1.7839106913325309</v>
+      </c>
+      <c r="G39" s="35"/>
       <c r="T39" s="39" t="s">
         <v>112</v>
       </c>
@@ -8960,56 +9243,32 @@
         <v>1.6205914926820167E-3</v>
       </c>
     </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>150</v>
+      </c>
+      <c r="F40" s="8" cm="1">
+        <f t="array" ref="F40">_xll.OmegaRatio(A2:A37,F5,1)</f>
+        <v>1.5950413223140492</v>
+      </c>
+      <c r="G40" s="35"/>
+    </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" s="1">
-        <f>_xlfn.VAR.P(A2:A37)</f>
-        <v>1.1005000000000001E-3</v>
-      </c>
-      <c r="G41" s="1">
-        <f>SQRT(F41*12)</f>
-        <v>0.11491736161259535</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="F41" s="8" cm="1">
+        <f t="array" ref="F41">_xll.KappaIndex(A2:A37,F5,1,1)</f>
+        <v>0.59504132231404949</v>
+      </c>
+      <c r="G41" s="35"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>84</v>
-      </c>
-      <c r="F42" s="1">
-        <f>_xlfn.VAR.P(B2:B37)</f>
-        <v>1.1303333333333335E-3</v>
-      </c>
-      <c r="G42" s="1">
-        <f>F42*12</f>
-        <v>1.3564000000000001E-2</v>
-      </c>
-      <c r="J42" s="1">
-        <f>F12^2*_xlfn.VAR.P(B2:B37)</f>
-        <v>1.0887780078257267E-3</v>
-      </c>
-      <c r="K42">
-        <f>SQRT(J42)</f>
-        <v>3.2996636310777601E-2</v>
-      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="35"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="1">
-        <f>F12^2*F42</f>
-        <v>1.0887780078257267E-3</v>
-      </c>
-      <c r="G43" s="14">
-        <f>SQRT(F43)</f>
-        <v>3.2996636310777601E-2</v>
-      </c>
-      <c r="H43" s="1" cm="1">
-        <f t="array" ref="H43">SQRT(_xll.MarketRisk(A2:A37,B2:B37,1))</f>
-        <v>3.2996636310777601E-2</v>
-      </c>
+      <c r="F43" s="8"/>
       <c r="U43">
         <f>U39/U28</f>
         <v>2.9148673436653182E-3</v>
@@ -9021,53 +9280,129 @@
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>86</v>
-      </c>
-      <c r="F44" s="1">
-        <f>F41-F12^2*F42</f>
-        <v>1.1721992174273423E-5</v>
-      </c>
-      <c r="G44" s="1">
-        <f>SQRT(F44)</f>
-        <v>3.4237395015207311E-3</v>
-      </c>
-      <c r="H44" s="1" cm="1">
-        <f t="array" ref="H44">_xll.UniqueRisk(A2:A37,B2:B37,1)</f>
-        <v>1.1721992174272989E-5</v>
-      </c>
-      <c r="I44">
-        <f>SQRT(H44)</f>
-        <v>3.4237395015206673E-3</v>
+        <v>131</v>
+      </c>
+      <c r="F44">
+        <f>W18</f>
+        <v>10.157364831893609</v>
+      </c>
+      <c r="G44">
+        <f>F44/SQRT(36)</f>
+        <v>1.6928941386489349</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H45" s="11">
-        <f>SUM(H43:H44)</f>
-        <v>3.3008358302951873E-2</v>
-      </c>
-      <c r="I45">
-        <f>SQRT(H45)</f>
-        <v>0.18168202526103641</v>
-      </c>
       <c r="U45" s="35">
         <f>STEYX(_xlfn.ANCHORARRAY(R2),_xlfn.ANCHORARRAY(N2))/SQRT(DEVSQ(_xlfn.ANCHORARRAY(N2)))</f>
         <v>0.9259940858765181</v>
       </c>
     </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="1">
+        <f>_xlfn.VAR.P(A2:A37)</f>
+        <v>1.1005000000000001E-3</v>
+      </c>
+      <c r="G48" s="1">
+        <f>SQRT(F48*12)</f>
+        <v>0.11491736161259535</v>
+      </c>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>84</v>
+      </c>
+      <c r="F49" s="1">
+        <f>_xlfn.VAR.P(B2:B37)</f>
+        <v>1.1303333333333335E-3</v>
+      </c>
+      <c r="G49" s="1">
+        <f>F49*12</f>
+        <v>1.3564000000000001E-2</v>
+      </c>
+      <c r="J49" s="1">
+        <f>F12^2*_xlfn.VAR.P(B2:B37)</f>
+        <v>1.0887780078257267E-3</v>
+      </c>
+      <c r="K49">
+        <f>SQRT(J49)</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="1">
+        <f>F12^2*F49</f>
+        <v>1.0887780078257267E-3</v>
+      </c>
+      <c r="G50" s="14">
+        <f>SQRT(F50)</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
+      <c r="H50" s="1" cm="1">
+        <f t="array" ref="H50">SQRT(_xll.MarketRisk(A2:A37,B2:B37,1))</f>
+        <v>3.2996636310777601E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="1">
+        <f>F48-F12^2*F49</f>
+        <v>1.1721992174273423E-5</v>
+      </c>
+      <c r="G51" s="1">
+        <f>SQRT(F51)</f>
+        <v>3.4237395015207311E-3</v>
+      </c>
+      <c r="H51" s="1" cm="1">
+        <f t="array" ref="H51">_xll.UniqueRisk(A2:A37,B2:B37,1)</f>
+        <v>1.1721992174272989E-5</v>
+      </c>
+      <c r="I51">
+        <f>SQRT(H51)</f>
+        <v>3.4237395015206673E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H52" s="11">
+        <f>SUM(H50:H51)</f>
+        <v>3.3008358302951873E-2</v>
+      </c>
+      <c r="I52">
+        <f>SQRT(H52)</f>
+        <v>0.18168202526103641</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F30:G35">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>ABS(F30:G42-F15:G27) &gt; 0.0000000001</formula>
+  <conditionalFormatting sqref="F26:G26">
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>ABS(F26:G39-F7:G19) &gt; 0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F27:G29">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>ABS(F27:G39-F12:G23) &gt; 0.0000000001</formula>
+  <conditionalFormatting sqref="F34:G39 F42:G42">
+    <cfRule type="expression" dxfId="3" priority="10">
+      <formula>ABS(F34:G49-F15:G31) &gt; 0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:G25 G26">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>ABS(F22:G35-F7:G19) &gt; 0.0000000001</formula>
+  <conditionalFormatting sqref="F31:G33">
+    <cfRule type="expression" dxfId="2" priority="11">
+      <formula>ABS(F31:G46-F12:G27) &gt; 0.0000000001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:G27">
+    <cfRule type="expression" dxfId="1" priority="13">
+      <formula>ABS(F27:G43-F8:G20) &gt; 0.0000000001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28:G29 G30">
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>ABS(F28:G44-F9:G25) &gt; 0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9080,7 +9415,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9591,7 +9926,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11981,4 +12316,2158 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B6E961-1479-40EC-811A-DC8D5E7B239C}">
+  <dimension ref="A1:S101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1">
+        <v>0.95</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B2" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="14">
+        <f>AVERAGE($A$2:$A$37) + I5*_xlfn.STDEV.P($A$2:$A$37)</f>
+        <v>-4.3566020298643725E-2</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="L2" cm="1">
+        <f t="array" ref="L2:L101">_xlfn.SEQUENCE(100,,0.01,0.01)</f>
+        <v>0.01</v>
+      </c>
+      <c r="M2">
+        <f>_xlfn.NORM.S.INV(L2)</f>
+        <v>-2.3263478740408408</v>
+      </c>
+      <c r="N2" cm="1">
+        <f t="array" ref="N2">_xll.NormalCdfInverse(L2, 0, 1)</f>
+        <v>-2.3263478740408408</v>
+      </c>
+      <c r="O2" t="b">
+        <f>ABS(M2-N2)&lt;$Q$2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="14">
+        <f>AVERAGE($A$2:$A$37) + I6*_xlfn.STDEV.P($A$2:$A$37)</f>
+        <v>-4.3566020298643725E-2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="21" cm="1">
+        <f t="array" ref="I3">_xll.Skewness_P(A2:A37)</f>
+        <v>-0.23799512754333596</v>
+      </c>
+      <c r="L3">
+        <v>0.02</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M66" si="0">_xlfn.NORM.S.INV(L3)</f>
+        <v>-2.0537489106318225</v>
+      </c>
+      <c r="N3" cm="1">
+        <f t="array" ref="N3">_xll.NormalCdfInverse(L3, 0, 1)</f>
+        <v>-2.0537489106318225</v>
+      </c>
+      <c r="O3" t="b">
+        <f t="shared" ref="O3:O66" si="1">ABS(M3-N3)&lt;$Q$2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="14" cm="1">
+        <f t="array" ref="F4">_xll.ParametricVaR(A2:A37,0.95)</f>
+        <v>-4.3566020298643725E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" s="21" cm="1">
+        <f t="array" ref="I4">_xll.Kurtosis_P_Excess(A2:A37)</f>
+        <v>-2.2361140899221699E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.03</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>-1.8807936081512509</v>
+      </c>
+      <c r="N4" cm="1">
+        <f t="array" ref="N4">_xll.NormalCdfInverse(L4, 0, 1)</f>
+        <v>-1.8807936081512509</v>
+      </c>
+      <c r="O4" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>-9.0000000000000011E-3</v>
+      </c>
+      <c r="B5" s="14">
+        <v>-1.1000000000000001E-2</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="14">
+        <f>AVERAGE(A2:A37)+(I5+(I5^2-1)/6*I3+(I5^3-3*I5)/24*I4- (2*I5^3-5*I5)/36*I3^2)*_xlfn.STDEV.P(A2:A37)</f>
+        <v>-4.5789964909625162E-2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.NORM.S.INV(1-I1)</f>
+        <v>-1.6448536269514715</v>
+      </c>
+      <c r="L5">
+        <v>0.04</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>-1.7506860712521695</v>
+      </c>
+      <c r="N5" cm="1">
+        <f t="array" ref="N5">_xll.NormalCdfInverse(L5, 0, 1)</f>
+        <v>-1.7506860712521695</v>
+      </c>
+      <c r="O5" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S5" s="46"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="26" cm="1">
+        <f t="array" ref="F6">_xll.ModifiedParametricVaR(A2:A37,0.95)</f>
+        <v>-4.6219230340278056E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" cm="1">
+        <f t="array" ref="I6">_xll.NormalCdfInverse(1-I1,0,1)</f>
+        <v>-1.6448536269514715</v>
+      </c>
+      <c r="L6">
+        <v>0.05</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>-1.6448536269514726</v>
+      </c>
+      <c r="N6" cm="1">
+        <f t="array" ref="N6">_xll.NormalCdfInverse(L6, 0, 1)</f>
+        <v>-1.6448536269514726</v>
+      </c>
+      <c r="O6" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L7">
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>-1.554773594596853</v>
+      </c>
+      <c r="N7" cm="1">
+        <f t="array" ref="N7">_xll.NormalCdfInverse(L7, 0, 1)</f>
+        <v>-1.554773594596853</v>
+      </c>
+      <c r="O7" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="14">
+        <f>_xlfn.PERCENTILE.EXC(A2:A37,1-I1)</f>
+        <v>-6.1449999999999991E-2</v>
+      </c>
+      <c r="L8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>-1.4757910281791702</v>
+      </c>
+      <c r="N8" cm="1">
+        <f t="array" ref="N8">_xll.NormalCdfInverse(L8, 0, 1)</f>
+        <v>-1.4757910281791702</v>
+      </c>
+      <c r="O8" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B9" s="14">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C9" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" s="14" cm="1">
+        <f t="array" ref="F9">_xll.HistoricalSimulationVaR(A2:A37,I1)</f>
+        <v>-6.1449999999999991E-2</v>
+      </c>
+      <c r="L9">
+        <v>0.08</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>-1.4050715603096353</v>
+      </c>
+      <c r="N9" cm="1">
+        <f t="array" ref="N9">_xll.NormalCdfInverse(L9, 0, 1)</f>
+        <v>-1.4050715603096322</v>
+      </c>
+      <c r="O9" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>-1.3999999999999999E-2</v>
+      </c>
+      <c r="B10" s="14">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="C10" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="L10">
+        <v>0.09</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>-1.3407550336902161</v>
+      </c>
+      <c r="N10" cm="1">
+        <f t="array" ref="N10">_xll.NormalCdfInverse(L10, 0, 1)</f>
+        <v>-1.3407550336902165</v>
+      </c>
+      <c r="O10" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B11" s="14">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C11" s="14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="L11">
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>-1.2815515655446006</v>
+      </c>
+      <c r="N11" cm="1">
+        <f t="array" ref="N11">_xll.NormalCdfInverse(L11, 0, 1)</f>
+        <v>-1.2815515655446008</v>
+      </c>
+      <c r="O11" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="B12" s="14">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C12" s="14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L12">
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>-1.2265281200366105</v>
+      </c>
+      <c r="N12" cm="1">
+        <f t="array" ref="N12">_xll.NormalCdfInverse(L12, 0, 1)</f>
+        <v>-1.2265281200366105</v>
+      </c>
+      <c r="O12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="B13" s="14">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C13" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L13">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>-1.1749867920660904</v>
+      </c>
+      <c r="N13" cm="1">
+        <f t="array" ref="N13">_xll.NormalCdfInverse(L13, 0, 1)</f>
+        <v>-1.1749867920660899</v>
+      </c>
+      <c r="O13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="B14" s="14">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C14" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L14">
+        <v>0.12999999999999998</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>-1.1263911290388013</v>
+      </c>
+      <c r="N14" cm="1">
+        <f t="array" ref="N14">_xll.NormalCdfInverse(L14, 0, 1)</f>
+        <v>-1.1263911290388005</v>
+      </c>
+      <c r="O14" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="B15" s="14">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L15">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>-1.0803193408149565</v>
+      </c>
+      <c r="N15" cm="1">
+        <f t="array" ref="N15">_xll.NormalCdfInverse(L15, 0, 1)</f>
+        <v>-1.0803193408149561</v>
+      </c>
+      <c r="O15" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="B16" s="14">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="C16" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L16">
+        <v>0.15</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>-1.0364333894937898</v>
+      </c>
+      <c r="N16" cm="1">
+        <f t="array" ref="N16">_xll.NormalCdfInverse(L16, 0, 1)</f>
+        <v>-1.0364333894937894</v>
+      </c>
+      <c r="O16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="B17" s="14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C17" s="14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L17">
+        <v>0.16</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>-0.9944578832097497</v>
+      </c>
+      <c r="N17" cm="1">
+        <f t="array" ref="N17">_xll.NormalCdfInverse(L17, 0, 1)</f>
+        <v>-0.99445788320975281</v>
+      </c>
+      <c r="O17" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="B18" s="14">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L18">
+        <v>0.17</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>-0.95416525314619549</v>
+      </c>
+      <c r="N18" cm="1">
+        <f t="array" ref="N18">_xll.NormalCdfInverse(L18, 0, 1)</f>
+        <v>-0.95416525314619416</v>
+      </c>
+      <c r="O18" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B19" s="14">
+        <v>-0.02</v>
+      </c>
+      <c r="C19" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L19">
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>-0.91536508784281256</v>
+      </c>
+      <c r="N19" cm="1">
+        <f t="array" ref="N19">_xll.NormalCdfInverse(L19, 0, 1)</f>
+        <v>-0.9153650878428139</v>
+      </c>
+      <c r="O19" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>6.2E-2</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="C20" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L20">
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>-0.87789629505122779</v>
+      </c>
+      <c r="N20" cm="1">
+        <f t="array" ref="N20">_xll.NormalCdfInverse(L20, 0, 1)</f>
+        <v>-0.87789629505122824</v>
+      </c>
+      <c r="O20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="B21" s="14">
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L21">
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>-0.84162123357291341</v>
+      </c>
+      <c r="N21" cm="1">
+        <f t="array" ref="N21">_xll.NormalCdfInverse(L21, 0, 1)</f>
+        <v>-0.84162123357291407</v>
+      </c>
+      <c r="O21" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="B22" s="14">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L22">
+        <v>0.21000000000000005</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>-0.80642124701823992</v>
+      </c>
+      <c r="N22" cm="1">
+        <f t="array" ref="N22">_xll.NormalCdfInverse(L22, 0, 1)</f>
+        <v>-0.80642124701824003</v>
+      </c>
+      <c r="O22" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="B23" s="14">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C23" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L23">
+        <v>0.22000000000000006</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>-0.77219321418868436</v>
+      </c>
+      <c r="N23" cm="1">
+        <f t="array" ref="N23">_xll.NormalCdfInverse(L23, 0, 1)</f>
+        <v>-0.77219321418868447</v>
+      </c>
+      <c r="O23" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="B24" s="14">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L24">
+        <v>0.23000000000000007</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>-0.73884684918521337</v>
+      </c>
+      <c r="N24" cm="1">
+        <f t="array" ref="N24">_xll.NormalCdfInverse(L24, 0, 1)</f>
+        <v>-0.73884684918521337</v>
+      </c>
+      <c r="O24" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>-2E-3</v>
+      </c>
+      <c r="B25" s="14">
+        <v>-1E-3</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L25">
+        <v>0.24000000000000007</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>-0.70630256284008697</v>
+      </c>
+      <c r="N25" cm="1">
+        <f t="array" ref="N25">_xll.NormalCdfInverse(L25, 0, 1)</f>
+        <v>-0.70630256284008708</v>
+      </c>
+      <c r="O25" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="B26" s="14">
+        <v>-2.6000000000000002E-2</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L26">
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>-0.67448975019608148</v>
+      </c>
+      <c r="N26" cm="1">
+        <f t="array" ref="N26">_xll.NormalCdfInverse(L26, 0, 1)</f>
+        <v>-0.67448975019608159</v>
+      </c>
+      <c r="O26" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="B27" s="14">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L27">
+        <v>0.26000000000000006</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>-0.64334540539291729</v>
+      </c>
+      <c r="N27" cm="1">
+        <f t="array" ref="N27">_xll.NormalCdfInverse(L27, 0, 1)</f>
+        <v>-0.64334540539291662</v>
+      </c>
+      <c r="O27" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B28" s="14">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L28">
+        <v>0.27000000000000007</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>-0.61281299101662701</v>
+      </c>
+      <c r="N28" cm="1">
+        <f t="array" ref="N28">_xll.NormalCdfInverse(L28, 0, 1)</f>
+        <v>-0.6128129910166269</v>
+      </c>
+      <c r="O28" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="B29" s="14">
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L29">
+        <v>0.28000000000000008</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>-0.5828415072712162</v>
+      </c>
+      <c r="N29" cm="1">
+        <f t="array" ref="N29">_xll.NormalCdfInverse(L29, 0, 1)</f>
+        <v>-0.58284150727121598</v>
+      </c>
+      <c r="O29" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="B30" s="14">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C30" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="L30">
+        <v>0.29000000000000009</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>-0.55338471955567248</v>
+      </c>
+      <c r="N30" cm="1">
+        <f t="array" ref="N30">_xll.NormalCdfInverse(L30, 0, 1)</f>
+        <v>-0.55338471955567248</v>
+      </c>
+      <c r="O30" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>-6.9999999999999993E-3</v>
+      </c>
+      <c r="B31" s="14">
+        <v>-2E-3</v>
+      </c>
+      <c r="C31" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L31">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>-0.52440051270804067</v>
+      </c>
+      <c r="N31" cm="1">
+        <f t="array" ref="N31">_xll.NormalCdfInverse(L31, 0, 1)</f>
+        <v>-0.52440051270804056</v>
+      </c>
+      <c r="O31" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="B32" s="14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C32" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L32">
+        <v>0.31000000000000011</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>-0.49585034734745309</v>
+      </c>
+      <c r="N32" cm="1">
+        <f t="array" ref="N32">_xll.NormalCdfInverse(L32, 0, 1)</f>
+        <v>-0.49585034734745309</v>
+      </c>
+      <c r="O32" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B33" s="14">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="C33" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L33">
+        <v>0.32000000000000012</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>-0.46769879911450801</v>
+      </c>
+      <c r="N33" cm="1">
+        <f t="array" ref="N33">_xll.NormalCdfInverse(L33, 0, 1)</f>
+        <v>-0.4676987991145079</v>
+      </c>
+      <c r="O33" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="B34" s="14">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="C34" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L34">
+        <v>0.33000000000000013</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>-0.43991316567323352</v>
+      </c>
+      <c r="N34" cm="1">
+        <f t="array" ref="N34">_xll.NormalCdfInverse(L34, 0, 1)</f>
+        <v>-0.43991316567323341</v>
+      </c>
+      <c r="O34" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>-2E-3</v>
+      </c>
+      <c r="B35" s="14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C35" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L35">
+        <v>0.34000000000000014</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>-0.41246312944140451</v>
+      </c>
+      <c r="N35" cm="1">
+        <f t="array" ref="N35">_xll.NormalCdfInverse(L35, 0, 1)</f>
+        <v>-0.41246312944140429</v>
+      </c>
+      <c r="O35" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="B36" s="14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C36" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L36">
+        <v>0.35000000000000014</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>-0.38532046640756729</v>
+      </c>
+      <c r="N36" cm="1">
+        <f t="array" ref="N36">_xll.NormalCdfInverse(L36, 0, 1)</f>
+        <v>-0.38532046640756717</v>
+      </c>
+      <c r="O36" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="B37" s="14">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C37" s="14">
+        <v>2E-3</v>
+      </c>
+      <c r="L37">
+        <v>0.36000000000000015</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>-0.35845879325119329</v>
+      </c>
+      <c r="N37" cm="1">
+        <f t="array" ref="N37">_xll.NormalCdfInverse(L37, 0, 1)</f>
+        <v>-0.35845879325119323</v>
+      </c>
+      <c r="O37" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>0.37000000000000016</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>-0.33185334643681624</v>
+      </c>
+      <c r="N38" cm="1">
+        <f t="array" ref="N38">_xll.NormalCdfInverse(L38, 0, 1)</f>
+        <v>-0.33185334643681613</v>
+      </c>
+      <c r="O38" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>0.38000000000000017</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>-0.30548078809939694</v>
+      </c>
+      <c r="N39" cm="1">
+        <f t="array" ref="N39">_xll.NormalCdfInverse(L39, 0, 1)</f>
+        <v>-0.30548078809939688</v>
+      </c>
+      <c r="O39" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>0.39000000000000018</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="0"/>
+        <v>-0.27931903444745371</v>
+      </c>
+      <c r="N40" cm="1">
+        <f t="array" ref="N40">_xll.NormalCdfInverse(L40, 0, 1)</f>
+        <v>-0.27931903444745371</v>
+      </c>
+      <c r="O40" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>0.40000000000000019</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="0"/>
+        <v>-0.25334710313579939</v>
+      </c>
+      <c r="N41" cm="1">
+        <f t="array" ref="N41">_xll.NormalCdfInverse(L41, 0, 1)</f>
+        <v>-0.25334710313579939</v>
+      </c>
+      <c r="O41" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>0.4100000000000002</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="0"/>
+        <v>-0.22754497664114895</v>
+      </c>
+      <c r="N42" cm="1">
+        <f t="array" ref="N42">_xll.NormalCdfInverse(L42, 0, 1)</f>
+        <v>-0.22754497664114892</v>
+      </c>
+      <c r="O42" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>0.42000000000000021</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="0"/>
+        <v>-0.20189347914185035</v>
+      </c>
+      <c r="N43" cm="1">
+        <f t="array" ref="N43">_xll.NormalCdfInverse(L43, 0, 1)</f>
+        <v>-0.2018934791418503</v>
+      </c>
+      <c r="O43" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>0.43000000000000022</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="0"/>
+        <v>-0.17637416478086079</v>
+      </c>
+      <c r="N44" cm="1">
+        <f t="array" ref="N44">_xll.NormalCdfInverse(L44, 0, 1)</f>
+        <v>-0.17637416478086074</v>
+      </c>
+      <c r="O44" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>0.44000000000000022</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="0"/>
+        <v>-0.15096921549677669</v>
+      </c>
+      <c r="N45" cm="1">
+        <f t="array" ref="N45">_xll.NormalCdfInverse(L45, 0, 1)</f>
+        <v>-0.15096921549677672</v>
+      </c>
+      <c r="O45" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>0.45000000000000023</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="0"/>
+        <v>-0.12566134685507346</v>
+      </c>
+      <c r="N46" cm="1">
+        <f t="array" ref="N46">_xll.NormalCdfInverse(L46, 0, 1)</f>
+        <v>-0.12566134685507346</v>
+      </c>
+      <c r="O46" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>0.46000000000000024</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="0"/>
+        <v>-0.10043372051146918</v>
+      </c>
+      <c r="N47" cm="1">
+        <f t="array" ref="N47">_xll.NormalCdfInverse(L47, 0, 1)</f>
+        <v>-0.10043372051146919</v>
+      </c>
+      <c r="O47" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>0.47000000000000025</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="0"/>
+        <v>-7.5269862099829207E-2</v>
+      </c>
+      <c r="N48" cm="1">
+        <f t="array" ref="N48">_xll.NormalCdfInverse(L48, 0, 1)</f>
+        <v>-7.5269862099829193E-2</v>
+      </c>
+      <c r="O48" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>0.48000000000000026</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="0"/>
+        <v>-5.0153583464732969E-2</v>
+      </c>
+      <c r="N49" cm="1">
+        <f t="array" ref="N49">_xll.NormalCdfInverse(L49, 0, 1)</f>
+        <v>-5.0153583464732969E-2</v>
+      </c>
+      <c r="O49" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>0.49000000000000027</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="0"/>
+        <v>-2.5068908258710363E-2</v>
+      </c>
+      <c r="N50" cm="1">
+        <f t="array" ref="N50">_xll.NormalCdfInverse(L50, 0, 1)</f>
+        <v>-2.5068908258710363E-2</v>
+      </c>
+      <c r="O50" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>0.50000000000000022</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="0"/>
+        <v>5.5658328493435343E-16</v>
+      </c>
+      <c r="N51" cm="1">
+        <f t="array" ref="N51">_xll.NormalCdfInverse(L51, 0, 1)</f>
+        <v>5.5658328493435352E-16</v>
+      </c>
+      <c r="O51" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>0.51000000000000023</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="0"/>
+        <v>2.5068908258711619E-2</v>
+      </c>
+      <c r="N52" cm="1">
+        <f t="array" ref="N52">_xll.NormalCdfInverse(L52, 0, 1)</f>
+        <v>2.5068908258711626E-2</v>
+      </c>
+      <c r="O52" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>0.52000000000000024</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="0"/>
+        <v>5.0153583464734218E-2</v>
+      </c>
+      <c r="N53" cm="1">
+        <f t="array" ref="N53">_xll.NormalCdfInverse(L53, 0, 1)</f>
+        <v>5.0153583464734218E-2</v>
+      </c>
+      <c r="O53" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>0.53000000000000025</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="0"/>
+        <v>7.5269862099830456E-2</v>
+      </c>
+      <c r="N54" cm="1">
+        <f t="array" ref="N54">_xll.NormalCdfInverse(L54, 0, 1)</f>
+        <v>7.5269862099830456E-2</v>
+      </c>
+      <c r="O54" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>0.54000000000000026</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="0"/>
+        <v>0.10043372051147045</v>
+      </c>
+      <c r="N55" cm="1">
+        <f t="array" ref="N55">_xll.NormalCdfInverse(L55, 0, 1)</f>
+        <v>0.10043372051147047</v>
+      </c>
+      <c r="O55" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="0"/>
+        <v>0.12566134685507474</v>
+      </c>
+      <c r="N56" cm="1">
+        <f t="array" ref="N56">_xll.NormalCdfInverse(L56, 0, 1)</f>
+        <v>0.12566134685507468</v>
+      </c>
+      <c r="O56" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>0.56000000000000028</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="0"/>
+        <v>0.15096921549677797</v>
+      </c>
+      <c r="N57" cm="1">
+        <f t="array" ref="N57">_xll.NormalCdfInverse(L57, 0, 1)</f>
+        <v>0.15096921549677794</v>
+      </c>
+      <c r="O57" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>0.57000000000000028</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="0"/>
+        <v>0.17637416478086207</v>
+      </c>
+      <c r="N58" cm="1">
+        <f t="array" ref="N58">_xll.NormalCdfInverse(L58, 0, 1)</f>
+        <v>0.17637416478086201</v>
+      </c>
+      <c r="O58" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>0.58000000000000029</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="0"/>
+        <v>0.20189347914185163</v>
+      </c>
+      <c r="N59" cm="1">
+        <f t="array" ref="N59">_xll.NormalCdfInverse(L59, 0, 1)</f>
+        <v>0.20189347914185155</v>
+      </c>
+      <c r="O59" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>0.5900000000000003</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="0"/>
+        <v>0.22754497664115017</v>
+      </c>
+      <c r="N60" cm="1">
+        <f t="array" ref="N60">_xll.NormalCdfInverse(L60, 0, 1)</f>
+        <v>0.22754497664115017</v>
+      </c>
+      <c r="O60" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>0.60000000000000031</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="0"/>
+        <v>0.25334710313580061</v>
+      </c>
+      <c r="N61" cm="1">
+        <f t="array" ref="N61">_xll.NormalCdfInverse(L61, 0, 1)</f>
+        <v>0.25334710313580061</v>
+      </c>
+      <c r="O61" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>0.61000000000000032</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="0"/>
+        <v>0.27931903444745504</v>
+      </c>
+      <c r="N62" cm="1">
+        <f t="array" ref="N62">_xll.NormalCdfInverse(L62, 0, 1)</f>
+        <v>0.27931903444745504</v>
+      </c>
+      <c r="O62" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>0.62000000000000033</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="0"/>
+        <v>0.30548078809939821</v>
+      </c>
+      <c r="N63" cm="1">
+        <f t="array" ref="N63">_xll.NormalCdfInverse(L63, 0, 1)</f>
+        <v>0.30548078809939821</v>
+      </c>
+      <c r="O63" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>0.63000000000000034</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="0"/>
+        <v>0.33185334643681752</v>
+      </c>
+      <c r="N64" cm="1">
+        <f t="array" ref="N64">_xll.NormalCdfInverse(L64, 0, 1)</f>
+        <v>0.33185334643681741</v>
+      </c>
+      <c r="O64" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>0.64000000000000035</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="0"/>
+        <v>0.35845879325119467</v>
+      </c>
+      <c r="N65" cm="1">
+        <f t="array" ref="N65">_xll.NormalCdfInverse(L65, 0, 1)</f>
+        <v>0.35845879325119473</v>
+      </c>
+      <c r="O65" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>0.65000000000000036</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="0"/>
+        <v>0.38532046640756862</v>
+      </c>
+      <c r="N66" cm="1">
+        <f t="array" ref="N66">_xll.NormalCdfInverse(L66, 0, 1)</f>
+        <v>0.38532046640756856</v>
+      </c>
+      <c r="O66" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <v>0.66000000000000036</v>
+      </c>
+      <c r="M67">
+        <f t="shared" ref="M67:M101" si="2">_xlfn.NORM.S.INV(L67)</f>
+        <v>0.41246312944140584</v>
+      </c>
+      <c r="N67" cm="1">
+        <f t="array" ref="N67">_xll.NormalCdfInverse(L67, 0, 1)</f>
+        <v>0.41246312944140578</v>
+      </c>
+      <c r="O67" t="b">
+        <f t="shared" ref="O67:O101" si="3">ABS(M67-N67)&lt;$Q$2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <v>0.67000000000000037</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="2"/>
+        <v>0.43991316567323491</v>
+      </c>
+      <c r="N68" cm="1">
+        <f t="array" ref="N68">_xll.NormalCdfInverse(L68, 0, 1)</f>
+        <v>0.4399131656732348</v>
+      </c>
+      <c r="O68" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <v>0.68000000000000038</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="2"/>
+        <v>0.46769879911450934</v>
+      </c>
+      <c r="N69" cm="1">
+        <f t="array" ref="N69">_xll.NormalCdfInverse(L69, 0, 1)</f>
+        <v>0.46769879911450923</v>
+      </c>
+      <c r="O69" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L70">
+        <v>0.69000000000000039</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="2"/>
+        <v>0.49585034734745448</v>
+      </c>
+      <c r="N70" cm="1">
+        <f t="array" ref="N70">_xll.NormalCdfInverse(L70, 0, 1)</f>
+        <v>0.49585034734745442</v>
+      </c>
+      <c r="O70" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L71">
+        <v>0.7000000000000004</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="2"/>
+        <v>0.524400512708042</v>
+      </c>
+      <c r="N71" cm="1">
+        <f t="array" ref="N71">_xll.NormalCdfInverse(L71, 0, 1)</f>
+        <v>0.52440051270804189</v>
+      </c>
+      <c r="O71" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>0.71000000000000041</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="2"/>
+        <v>0.55338471955567414</v>
+      </c>
+      <c r="N72" cm="1">
+        <f t="array" ref="N72">_xll.NormalCdfInverse(L72, 0, 1)</f>
+        <v>0.55338471955567392</v>
+      </c>
+      <c r="O72" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <v>0.72000000000000042</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="2"/>
+        <v>0.58284150727121742</v>
+      </c>
+      <c r="N73" cm="1">
+        <f t="array" ref="N73">_xll.NormalCdfInverse(L73, 0, 1)</f>
+        <v>0.58284150727121753</v>
+      </c>
+      <c r="O73" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L74">
+        <v>0.73000000000000043</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="2"/>
+        <v>0.61281299101662867</v>
+      </c>
+      <c r="N74" cm="1">
+        <f t="array" ref="N74">_xll.NormalCdfInverse(L74, 0, 1)</f>
+        <v>0.61281299101662856</v>
+      </c>
+      <c r="O74" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>0.74000000000000044</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="2"/>
+        <v>0.6433454053929184</v>
+      </c>
+      <c r="N75" cm="1">
+        <f t="array" ref="N75">_xll.NormalCdfInverse(L75, 0, 1)</f>
+        <v>0.6433454053929184</v>
+      </c>
+      <c r="O75" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>0.75000000000000044</v>
+      </c>
+      <c r="M76">
+        <f t="shared" si="2"/>
+        <v>0.67448975019608293</v>
+      </c>
+      <c r="N76" cm="1">
+        <f t="array" ref="N76">_xll.NormalCdfInverse(L76, 0, 1)</f>
+        <v>0.67448975019608326</v>
+      </c>
+      <c r="O76" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>0.76000000000000045</v>
+      </c>
+      <c r="M77">
+        <f t="shared" si="2"/>
+        <v>0.70630256284008885</v>
+      </c>
+      <c r="N77" cm="1">
+        <f t="array" ref="N77">_xll.NormalCdfInverse(L77, 0, 1)</f>
+        <v>0.70630256284008874</v>
+      </c>
+      <c r="O77" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>0.77000000000000046</v>
+      </c>
+      <c r="M78">
+        <f t="shared" si="2"/>
+        <v>0.73884684918521504</v>
+      </c>
+      <c r="N78" cm="1">
+        <f t="array" ref="N78">_xll.NormalCdfInverse(L78, 0, 1)</f>
+        <v>0.73884684918521515</v>
+      </c>
+      <c r="O78" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <v>0.78000000000000047</v>
+      </c>
+      <c r="M79">
+        <f t="shared" si="2"/>
+        <v>0.77219321418868658</v>
+      </c>
+      <c r="N79" cm="1">
+        <f t="array" ref="N79">_xll.NormalCdfInverse(L79, 0, 1)</f>
+        <v>0.77219321418868636</v>
+      </c>
+      <c r="O79" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <v>0.79000000000000048</v>
+      </c>
+      <c r="M80">
+        <f t="shared" si="2"/>
+        <v>0.80642124701824136</v>
+      </c>
+      <c r="N80" cm="1">
+        <f t="array" ref="N80">_xll.NormalCdfInverse(L80, 0, 1)</f>
+        <v>0.80642124701824203</v>
+      </c>
+      <c r="O80" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>0.80000000000000049</v>
+      </c>
+      <c r="M81">
+        <f t="shared" si="2"/>
+        <v>0.84162123357291596</v>
+      </c>
+      <c r="N81" cm="1">
+        <f t="array" ref="N81">_xll.NormalCdfInverse(L81, 0, 1)</f>
+        <v>0.84162123357291574</v>
+      </c>
+      <c r="O81" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <v>0.8100000000000005</v>
+      </c>
+      <c r="M82">
+        <f t="shared" si="2"/>
+        <v>0.87789629505123112</v>
+      </c>
+      <c r="N82" cm="1">
+        <f t="array" ref="N82">_xll.NormalCdfInverse(L82, 0, 1)</f>
+        <v>0.87789629505123046</v>
+      </c>
+      <c r="O82" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L83">
+        <v>0.82000000000000051</v>
+      </c>
+      <c r="M83">
+        <f t="shared" si="2"/>
+        <v>0.91536508784281501</v>
+      </c>
+      <c r="N83" cm="1">
+        <f t="array" ref="N83">_xll.NormalCdfInverse(L83, 0, 1)</f>
+        <v>0.91536508784281601</v>
+      </c>
+      <c r="O83" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <v>0.83000000000000052</v>
+      </c>
+      <c r="M84">
+        <f t="shared" si="2"/>
+        <v>0.95416525314619716</v>
+      </c>
+      <c r="N84" cm="1">
+        <f t="array" ref="N84">_xll.NormalCdfInverse(L84, 0, 1)</f>
+        <v>0.95416525314619638</v>
+      </c>
+      <c r="O84" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <v>0.84000000000000052</v>
+      </c>
+      <c r="M85">
+        <f t="shared" si="2"/>
+        <v>0.99445788320975514</v>
+      </c>
+      <c r="N85" cm="1">
+        <f t="array" ref="N85">_xll.NormalCdfInverse(L85, 0, 1)</f>
+        <v>0.99445788320975526</v>
+      </c>
+      <c r="O85" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <v>0.85000000000000053</v>
+      </c>
+      <c r="M86">
+        <f t="shared" si="2"/>
+        <v>1.0364333894937905</v>
+      </c>
+      <c r="N86" cm="1">
+        <f t="array" ref="N86">_xll.NormalCdfInverse(L86, 0, 1)</f>
+        <v>1.036433389493792</v>
+      </c>
+      <c r="O86" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <v>0.86000000000000054</v>
+      </c>
+      <c r="M87">
+        <f t="shared" si="2"/>
+        <v>1.0803193408149587</v>
+      </c>
+      <c r="N87" cm="1">
+        <f t="array" ref="N87">_xll.NormalCdfInverse(L87, 0, 1)</f>
+        <v>1.0803193408149587</v>
+      </c>
+      <c r="O87" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <v>0.87000000000000055</v>
+      </c>
+      <c r="M88">
+        <f t="shared" si="2"/>
+        <v>1.1263911290388036</v>
+      </c>
+      <c r="N88" cm="1">
+        <f t="array" ref="N88">_xll.NormalCdfInverse(L88, 0, 1)</f>
+        <v>1.1263911290388033</v>
+      </c>
+      <c r="O88" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <v>0.88000000000000056</v>
+      </c>
+      <c r="M89">
+        <f t="shared" si="2"/>
+        <v>1.174986792066093</v>
+      </c>
+      <c r="N89" cm="1">
+        <f t="array" ref="N89">_xll.NormalCdfInverse(L89, 0, 1)</f>
+        <v>1.1749867920660926</v>
+      </c>
+      <c r="O89" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <v>0.89000000000000057</v>
+      </c>
+      <c r="M90">
+        <f t="shared" si="2"/>
+        <v>1.2265281200366132</v>
+      </c>
+      <c r="N90" cm="1">
+        <f t="array" ref="N90">_xll.NormalCdfInverse(L90, 0, 1)</f>
+        <v>1.2265281200366129</v>
+      </c>
+      <c r="O90" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <v>0.90000000000000058</v>
+      </c>
+      <c r="M91">
+        <f t="shared" si="2"/>
+        <v>1.2815515655446033</v>
+      </c>
+      <c r="N91" cm="1">
+        <f t="array" ref="N91">_xll.NormalCdfInverse(L91, 0, 1)</f>
+        <v>1.2815515655446037</v>
+      </c>
+      <c r="O91" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L92">
+        <v>0.91000000000000059</v>
+      </c>
+      <c r="M92">
+        <f t="shared" si="2"/>
+        <v>1.3407550336902203</v>
+      </c>
+      <c r="N92" cm="1">
+        <f t="array" ref="N92">_xll.NormalCdfInverse(L92, 0, 1)</f>
+        <v>1.3407550336902199</v>
+      </c>
+      <c r="O92" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L93">
+        <v>0.9200000000000006</v>
+      </c>
+      <c r="M93">
+        <f t="shared" si="2"/>
+        <v>1.4050715603096373</v>
+      </c>
+      <c r="N93" cm="1">
+        <f t="array" ref="N93">_xll.NormalCdfInverse(L93, 0, 1)</f>
+        <v>1.4050715603096364</v>
+      </c>
+      <c r="O93" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L94">
+        <v>0.9300000000000006</v>
+      </c>
+      <c r="M94">
+        <f t="shared" si="2"/>
+        <v>1.4757910281791757</v>
+      </c>
+      <c r="N94" cm="1">
+        <f t="array" ref="N94">_xll.NormalCdfInverse(L94, 0, 1)</f>
+        <v>1.4757910281791753</v>
+      </c>
+      <c r="O94" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L95">
+        <v>0.94000000000000061</v>
+      </c>
+      <c r="M95">
+        <f t="shared" si="2"/>
+        <v>1.5547735945968584</v>
+      </c>
+      <c r="N95" cm="1">
+        <f t="array" ref="N95">_xll.NormalCdfInverse(L95, 0, 1)</f>
+        <v>1.5547735945968584</v>
+      </c>
+      <c r="O95" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L96">
+        <v>0.95000000000000062</v>
+      </c>
+      <c r="M96">
+        <f t="shared" si="2"/>
+        <v>1.6448536269514784</v>
+      </c>
+      <c r="N96" cm="1">
+        <f t="array" ref="N96">_xll.NormalCdfInverse(L96, 0, 1)</f>
+        <v>1.6448536269514784</v>
+      </c>
+      <c r="O96" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L97">
+        <v>0.96000000000000063</v>
+      </c>
+      <c r="M97">
+        <f t="shared" si="2"/>
+        <v>1.7506860712521775</v>
+      </c>
+      <c r="N97" cm="1">
+        <f t="array" ref="N97">_xll.NormalCdfInverse(L97, 0, 1)</f>
+        <v>1.7506860712521775</v>
+      </c>
+      <c r="O97" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L98">
+        <v>0.97000000000000064</v>
+      </c>
+      <c r="M98">
+        <f t="shared" si="2"/>
+        <v>1.88079360815126</v>
+      </c>
+      <c r="N98" cm="1">
+        <f t="array" ref="N98">_xll.NormalCdfInverse(L98, 0, 1)</f>
+        <v>1.88079360815126</v>
+      </c>
+      <c r="O98" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L99">
+        <v>0.98000000000000065</v>
+      </c>
+      <c r="M99">
+        <f t="shared" si="2"/>
+        <v>2.0537489106318363</v>
+      </c>
+      <c r="N99" cm="1">
+        <f t="array" ref="N99">_xll.NormalCdfInverse(L99, 0, 1)</f>
+        <v>2.0537489106318363</v>
+      </c>
+      <c r="O99" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L100">
+        <v>0.99000000000000066</v>
+      </c>
+      <c r="M100">
+        <f t="shared" si="2"/>
+        <v>2.3263478740408656</v>
+      </c>
+      <c r="N100" cm="1">
+        <f t="array" ref="N100">_xll.NormalCdfInverse(L100, 0, 1)</f>
+        <v>2.3263478740408656</v>
+      </c>
+      <c r="O100" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L101">
+        <v>1.0000000000000007</v>
+      </c>
+      <c r="M101" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N101" t="e" cm="1">
+        <f t="array" ref="N101">_xll.NormalCdfInverse(L101, 0, 1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="O101" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>